<commit_message>
Add information about accids in table
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/proba/GABCtoMEI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A65F5F6-6D28-9A4E-BFF1-21AE3C96E7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E429209E-3F94-8C4F-89A2-09E7F4168059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="500" windowWidth="35680" windowHeight="17440" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="219">
   <si>
     <t>01_benedicte-omnes_pem82441_aquit</t>
   </si>
@@ -690,13 +690,16 @@
   </si>
   <si>
     <t>34_qui-manducat--panem_pem11919_aquit</t>
+  </si>
+  <si>
+    <t>accid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -715,6 +718,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -737,10 +751,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAB5ED-65C4-C540-BBD9-8DBFB51E3378}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1508,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1517,7 +1534,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1543,7 +1560,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1569,7 +1586,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1612,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1621,7 +1638,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1647,7 +1664,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1673,7 +1690,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1699,7 +1716,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1725,7 +1742,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1751,7 +1768,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1776,8 +1793,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1803,7 +1823,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1829,7 +1849,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1855,7 +1875,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1881,7 +1901,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1907,7 +1927,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1933,7 +1953,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1959,7 +1979,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1985,7 +2005,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/34_qui-manducat--panem_pem11919_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem11919_aquit.mei </v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2011,7 +2031,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2037,33 +2057,36 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D38" t="s">
-        <v>205</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>square</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="1"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G38" t="str">
+      <c r="D38" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>square</v>
+      </c>
+      <c r="F38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-notation square</v>
+      </c>
+      <c r="G38" s="3" t="str">
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2089,7 +2112,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2115,7 +2138,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2141,7 +2164,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2190,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2193,7 +2216,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2219,7 +2242,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2245,7 +2268,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2271,7 +2294,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -2297,7 +2320,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -2663,6 +2686,9 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
+      <c r="H61" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -3029,6 +3055,9 @@
       <c r="G75" t="str">
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
+      </c>
+      <c r="H75" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update table (for clef changes)
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/GABCtoMEI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E429209E-3F94-8C4F-89A2-09E7F4168059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC8444-9468-C24F-89FF-6357A431EEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="500" windowWidth="35680" windowHeight="17440" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="8040" yWindow="1660" windowWidth="21360" windowHeight="16060" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="220">
   <si>
     <t>01_benedicte-omnes_pem82441_aquit</t>
   </si>
@@ -683,9 +683,6 @@
     <t>Command</t>
   </si>
   <si>
-    <t>clef change</t>
-  </si>
-  <si>
     <t>34_deo-nostro_pem71013_square</t>
   </si>
   <si>
@@ -693,6 +690,12 @@
   </si>
   <si>
     <t>accid</t>
+  </si>
+  <si>
+    <t>clef changes (2)</t>
+  </si>
+  <si>
+    <t>clef changes (1)</t>
   </si>
 </sst>
 </file>
@@ -731,12 +734,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -751,13 +766,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,8 +1092,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAB5ED-65C4-C540-BBD9-8DBFB51E3378}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,6 +1108,7 @@
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="214" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1293,8 +1315,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
       </c>
-      <c r="H8" t="s">
-        <v>215</v>
+      <c r="H8" s="8" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1426,8 +1448,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
       </c>
-      <c r="H13" t="s">
-        <v>215</v>
+      <c r="H13" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1793,8 +1815,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
-      <c r="H27" t="s">
-        <v>218</v>
+      <c r="H27" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1984,7 +2006,7 @@
         <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>136</v>
@@ -2082,8 +2104,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>218</v>
+      <c r="H38" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -2345,6 +2367,9 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
       </c>
+      <c r="H48" s="8" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -2527,8 +2552,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
       </c>
-      <c r="H55" t="s">
-        <v>215</v>
+      <c r="H55" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2686,8 +2711,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
-      <c r="H61" t="s">
-        <v>218</v>
+      <c r="H61" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2819,8 +2844,8 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
       </c>
-      <c r="H66" t="s">
-        <v>215</v>
+      <c r="H66" s="8" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -3056,8 +3081,8 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
-      <c r="H75" t="s">
-        <v>218</v>
+      <c r="H75" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -3715,7 +3740,7 @@
         <v>67</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>202</v>

</xml_diff>

<commit_message>
Add links to the manuscript images for each file in the table
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC8444-9468-C24F-89FF-6357A431EEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C64B6-A361-9840-84AE-EFD3B3746858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="1660" windowWidth="21360" windowHeight="16060" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="-2880" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="291">
   <si>
     <t>01_benedicte-omnes_pem82441_aquit</t>
   </si>
@@ -696,13 +696,254 @@
   </si>
   <si>
     <t>clef changes (1)</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/82441</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85041</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/56766</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84909</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84540</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84623</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84873</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84614</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84548</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84882</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84878</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/86239</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84630</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84881</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84534</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84863</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/83892</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85059</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84600</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/83880</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84880</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84580</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85056</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/83911</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84665</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84905</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84532</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84919</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84595</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84872</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84666</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84874</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/76616</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/119191</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84924</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84057</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85065</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/83876</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85073</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/83869</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84946</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84570</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85037</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85014</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71059</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85026</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71210</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85972</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/86078</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85023</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/80113</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71112</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/80209</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71032</t>
+  </si>
+  <si>
+    <r>
+      <t>https://pemdatabase.eu/image/80148</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://pemdatabase.eu/image/80149</t>
+    </r>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71205</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/86046</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85997</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/80028</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71128</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85921</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/86009</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84967</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/84633</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/85642</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71108</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/92154</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71010</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/80159</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71012</t>
+  </si>
+  <si>
+    <t>https://pemdatabase.eu/image/71013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -733,6 +974,31 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -754,7 +1020,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -762,11 +1028,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -776,8 +1058,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1090,28 +1388,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAB5ED-65C4-C540-BBD9-8DBFB51E3378}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="214" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>208</v>
       </c>
@@ -1134,7 +1433,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1159,8 +1458,11 @@
         <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A2,"/",B2,".gabc MEI_outfiles/", A2, "/", C2, "_", D2, B2, ".mei ",F2)</f>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1185,8 +1487,11 @@
         <f t="shared" ref="G3:G66" si="2">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A3,"/",B3,".gabc MEI_outfiles/", A3, "/", C3, "_", D3, B3, ".mei ",F3)</f>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1211,8 +1516,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/03_de-fructu-operum_pem56766_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.mei </v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1237,8 +1545,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/04_de-fructu-operum_pem84909_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1263,8 +1574,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/05_dicit-dominus_pem84540_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.mei </v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1289,8 +1603,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/06_dicit-dominus_pem84623_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.mei </v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1315,11 +1632,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1344,8 +1664,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/08_ecce-virgo_pem84614_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.mei </v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1370,8 +1693,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/09_ecce-virgo_pem84548_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.mei </v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1396,8 +1722,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/10_ecce-virgo_pem84882_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1422,8 +1751,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/11_jerusalem-surge_pem84878_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1448,11 +1780,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1477,8 +1812,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/13_factus-est-repente_pem84630_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.mei </v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1503,8 +1841,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/14_factus-est-repente_pem84881_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1529,8 +1870,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1555,8 +1899,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1581,8 +1928,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1607,8 +1957,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1633,8 +1986,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1659,8 +2015,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1685,8 +2044,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1711,8 +2073,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H23" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1737,8 +2102,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H24" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1763,8 +2131,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H25" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1789,8 +2160,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1815,11 +2189,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1844,8 +2221,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H28" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1870,8 +2250,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1896,8 +2279,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1922,8 +2308,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H31" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1948,8 +2337,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1974,8 +2366,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2000,8 +2395,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2026,8 +2424,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/34_qui-manducat--panem_pem11919_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem11919_aquit.mei </v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2052,8 +2453,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2078,8 +2482,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
       </c>
-    </row>
-    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
@@ -2104,11 +2511,18 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2133,8 +2547,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2159,8 +2576,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H40" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2185,8 +2605,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H41" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2211,8 +2634,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H42" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2237,8 +2663,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2263,8 +2692,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H44" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2289,8 +2721,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H45" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2315,8 +2750,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -2341,8 +2779,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H47" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -2367,11 +2808,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="I48" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2396,8 +2840,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/05_o-crux_pem85972_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H49" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2422,8 +2869,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/06_o-crux_pem86078_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H50" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -2448,8 +2898,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/07_o-crux_pem85023_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H51" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2474,8 +2927,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/08_ihesum_pem80113_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.mei </v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H52" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -2500,8 +2956,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/09_ihesum_pem71112_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H53" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -2526,8 +2985,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/10_tunc-invocabis_pem80209_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.mei </v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H54" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -2552,11 +3014,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I55" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -2581,8 +3046,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/12_si-offers_pem80148-80149_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.mei </v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H56" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -2607,8 +3075,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/13_si-offers_pem71205_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H57" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -2633,8 +3104,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/14_isti-sunt_pem86046_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.mei </v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H58" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -2659,8 +3133,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/15_isti-sunt_pem85997_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H59" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -2685,8 +3162,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/16_mercennarius_pem80028_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.mei </v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H60" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -2711,11 +3191,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
-      <c r="H61" s="6" t="s">
+      <c r="H61" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="I61" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2740,8 +3223,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/18_o-lux_pem85921_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H62" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -2766,8 +3252,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/19_o-lux_pem86009_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H63" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -2792,8 +3281,11 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/20_o-lux_pem84967_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H64" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -2818,8 +3310,11 @@
         <f t="shared" si="2"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/21_vespere_pem84633_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.mei </v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H65" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2844,11 +3339,14 @@
         <f t="shared" si="2"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
       </c>
-      <c r="H66" s="8" t="s">
+      <c r="H66" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="I66" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2873,8 +3371,11 @@
         <f t="shared" ref="G67:G103" si="5">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H67" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2899,8 +3400,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H68" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2925,8 +3429,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H69" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -2951,8 +3458,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H70" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -2977,8 +3487,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H71" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -3003,8 +3516,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H72" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -3029,8 +3545,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H73" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -3055,8 +3574,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H74" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -3081,11 +3603,14 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H75" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="I75" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3110,8 +3635,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H76" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -3136,8 +3664,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H77" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -3162,8 +3693,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H78" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -3188,8 +3722,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H79" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -3214,8 +3751,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>67</v>
       </c>
@@ -3240,8 +3780,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -3266,8 +3809,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>67</v>
       </c>
@@ -3292,8 +3838,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>67</v>
       </c>
@@ -3318,8 +3867,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>67</v>
       </c>
@@ -3344,8 +3896,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -3370,8 +3925,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -3396,8 +3954,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>67</v>
       </c>
@@ -3422,8 +3983,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>67</v>
       </c>
@@ -3448,8 +4012,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>67</v>
       </c>
@@ -3474,8 +4041,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>67</v>
       </c>
@@ -3500,8 +4070,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>67</v>
       </c>
@@ -3526,8 +4099,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>67</v>
       </c>
@@ -3552,8 +4128,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>67</v>
       </c>
@@ -3578,8 +4157,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>67</v>
       </c>
@@ -3604,8 +4186,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>67</v>
       </c>
@@ -3630,8 +4215,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>67</v>
       </c>
@@ -3656,8 +4244,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>67</v>
       </c>
@@ -3682,8 +4273,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>67</v>
       </c>
@@ -3708,8 +4302,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>67</v>
       </c>
@@ -3734,8 +4331,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>67</v>
       </c>
@@ -3760,8 +4360,11 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>67</v>
       </c>
@@ -3786,8 +4389,11 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>67</v>
       </c>
@@ -3812,9 +4418,118 @@
         <f t="shared" si="5"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
+      <c r="H103" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H104" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{DB9705ED-1102-844D-8A04-BCDD8E8E1C9A}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{D77C11A9-E4F8-DB40-9661-517579200867}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{D4547D4F-3D45-BE48-A428-10938BAD2593}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{6200DF7A-A4F0-4F4F-A936-7E0ABA52812B}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{EEC7B717-F249-8F46-8EED-66E12D4C406C}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{40792145-400B-2F4D-9194-4B086DB7249D}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{14CB7A99-AD48-5245-A2BF-365DA359E239}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{9E67B4D6-ED25-BD47-ADB0-8D0778E0C7D0}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{A90FC4EC-8F44-B44A-BD6D-2E4B45209579}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{B057863F-F9F1-0A4F-B82C-2A4C3DADEBF5}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{01E8EB59-1B0C-9D4D-81AB-B319290DD44F}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{CE849FA7-20D0-4041-A822-3D3421A89DE3}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{9E29757E-8B5E-1D4A-8F7B-F9133DCBA973}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{20364D05-C7BB-0B46-83D7-2313604424D0}"/>
+    <hyperlink ref="H16" r:id="rId15" xr:uid="{0A99BCF0-83E3-D343-97E9-6A65FAB38C53}"/>
+    <hyperlink ref="H17" r:id="rId16" xr:uid="{0D34DFBA-2472-134E-9D59-CB1D7B8530AC}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{9D2E55B2-3E44-724D-8292-07CD28429884}"/>
+    <hyperlink ref="H19" r:id="rId18" xr:uid="{8E0B24A1-71B0-334E-815E-6F6795C9F3C5}"/>
+    <hyperlink ref="H20" r:id="rId19" xr:uid="{1E963136-3690-914E-AF44-8D5DAA29CD19}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{E86A8DA0-9472-9345-94AD-F5C68A29461F}"/>
+    <hyperlink ref="H22" r:id="rId21" xr:uid="{2F9E19DD-D389-734E-A2CC-164B62E4324B}"/>
+    <hyperlink ref="H23" r:id="rId22" xr:uid="{893BBCBF-CCB7-2D4A-B677-ACEBC416B761}"/>
+    <hyperlink ref="H24" r:id="rId23" xr:uid="{F50D8A05-7397-974F-B01F-764AE6C3C4DD}"/>
+    <hyperlink ref="H25" r:id="rId24" xr:uid="{98E0FFB8-21AD-454B-94D8-175690870EBD}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{CD540896-1648-0D46-92FC-E53D779DC609}"/>
+    <hyperlink ref="H27" r:id="rId26" xr:uid="{453D630D-575E-7248-A7BF-7D87A31ACC73}"/>
+    <hyperlink ref="H28" r:id="rId27" xr:uid="{0C00C7B9-21A3-8E46-8F3F-618DFCF85306}"/>
+    <hyperlink ref="H29" r:id="rId28" xr:uid="{19AF7838-3D45-154D-B232-907AB73C60AD}"/>
+    <hyperlink ref="H30" r:id="rId29" xr:uid="{87E401CF-CE72-DC4D-A817-72A457DB9204}"/>
+    <hyperlink ref="H31" r:id="rId30" xr:uid="{B4C3CE51-A97A-F74E-B1B7-9360CE4FA4F6}"/>
+    <hyperlink ref="H32" r:id="rId31" xr:uid="{9DE06E22-6A80-BA48-AD33-F62E0C25738B}"/>
+    <hyperlink ref="H33" r:id="rId32" xr:uid="{5145BB33-2874-6F47-BAC9-29CC6F536EF6}"/>
+    <hyperlink ref="H34" r:id="rId33" xr:uid="{7FACDA80-3BDD-1344-AE40-DE26B8CE8A00}"/>
+    <hyperlink ref="H35" r:id="rId34" xr:uid="{F282D038-D37F-0948-BB58-C27F8A21E406}"/>
+    <hyperlink ref="H36" r:id="rId35" xr:uid="{78F4E6DF-CE1D-2542-8829-F111269D9E82}"/>
+    <hyperlink ref="H37" r:id="rId36" xr:uid="{AB90628A-74C8-AE43-B367-8F344328C8DD}"/>
+    <hyperlink ref="H38" r:id="rId37" xr:uid="{6A028A2F-E1C9-8B4A-AB75-48974174A2CF}"/>
+    <hyperlink ref="H39" r:id="rId38" xr:uid="{CC0EBB72-AD4A-9243-A4E6-7A3B8DEEB393}"/>
+    <hyperlink ref="H40" r:id="rId39" xr:uid="{72476B32-E8A3-F94A-B4C4-1F7ACE5924A6}"/>
+    <hyperlink ref="H41" r:id="rId40" xr:uid="{D69A317D-2F55-5641-8495-7638D7FB61B6}"/>
+    <hyperlink ref="H42" r:id="rId41" xr:uid="{0D98BB49-EFC9-544B-89D0-18AF57E4183B}"/>
+    <hyperlink ref="H43" r:id="rId42" xr:uid="{E67105D9-6603-8B42-BB0F-39487ED176CB}"/>
+    <hyperlink ref="H44" r:id="rId43" xr:uid="{FFB09EEE-F66A-C040-B80E-C97CB1F9B115}"/>
+    <hyperlink ref="H45" r:id="rId44" xr:uid="{76E94D16-4F23-CE47-9DDD-A2AA7D960AEC}"/>
+    <hyperlink ref="H46" r:id="rId45" xr:uid="{4EBE8D1A-0A09-494C-AB31-B3890DA7390F}"/>
+    <hyperlink ref="H47" r:id="rId46" xr:uid="{FEF1047E-AA75-9042-A278-F879E7776B9F}"/>
+    <hyperlink ref="H48" r:id="rId47" xr:uid="{202525C7-3BCB-AF4E-B76A-1B503E3FEE30}"/>
+    <hyperlink ref="H49" r:id="rId48" xr:uid="{CD47F6FD-98C9-AC42-A9CD-4C343A1E3B10}"/>
+    <hyperlink ref="H50" r:id="rId49" xr:uid="{60BDB147-524C-3B41-AE90-E0977A366F17}"/>
+    <hyperlink ref="H51" r:id="rId50" xr:uid="{2B57DFCF-7D6B-A74C-8B1C-493CB7DBAA05}"/>
+    <hyperlink ref="H52" r:id="rId51" xr:uid="{E7700FC4-5E72-9C40-9144-CA1442DEDECC}"/>
+    <hyperlink ref="H53" r:id="rId52" xr:uid="{3DE21483-DDDB-A248-BA7A-EBEB96A88C1A}"/>
+    <hyperlink ref="H54" r:id="rId53" xr:uid="{5765242A-9978-B645-B6D5-5D18ABB69DBE}"/>
+    <hyperlink ref="H55" r:id="rId54" xr:uid="{F3921BD7-BD46-B242-B473-1C20EEDAA788}"/>
+    <hyperlink ref="H57" r:id="rId55" xr:uid="{43162756-13C3-5F43-A5F3-54AF19FE2570}"/>
+    <hyperlink ref="H58" r:id="rId56" xr:uid="{A77C9F00-E3C7-B647-A9A0-63BB8D5E5D3E}"/>
+    <hyperlink ref="H59" r:id="rId57" xr:uid="{798C58B6-B779-7946-A62E-FC3E57958AB1}"/>
+    <hyperlink ref="H60" r:id="rId58" xr:uid="{054BF8E6-8464-1D47-92C8-497785FFB9F6}"/>
+    <hyperlink ref="H61" r:id="rId59" xr:uid="{93A9484E-03E8-A54C-A066-0001CBFB1CAC}"/>
+    <hyperlink ref="H62" r:id="rId60" xr:uid="{A196408E-A03A-8249-888F-5E4AE72C584C}"/>
+    <hyperlink ref="H63" r:id="rId61" xr:uid="{306E8BAF-7683-2847-BCE5-A301781FDAF9}"/>
+    <hyperlink ref="H64" r:id="rId62" xr:uid="{F8E60D28-36A5-B949-943E-7F44CF901C6D}"/>
+    <hyperlink ref="H65" r:id="rId63" xr:uid="{398FAEEA-EAAB-F849-8343-7C7DE39C9438}"/>
+    <hyperlink ref="H66" r:id="rId64" xr:uid="{3ABABF49-D241-114F-A9B4-3CE6C0F5A4EF}"/>
+    <hyperlink ref="H67" r:id="rId65" xr:uid="{DD0E540A-4325-644C-B0EA-F464CD546FF0}"/>
+    <hyperlink ref="H68" r:id="rId66" xr:uid="{865A3FBB-D918-E34E-B265-1D0BC999522D}"/>
+    <hyperlink ref="H69" r:id="rId67" xr:uid="{95DD4DB0-71CE-D647-918A-002E6ECBEB94}"/>
+    <hyperlink ref="H70" r:id="rId68" xr:uid="{639777CE-4D86-A649-B073-03DBF2112747}"/>
+    <hyperlink ref="H71" r:id="rId69" xr:uid="{B589FDFC-EF2C-1C44-9878-FB99A3FE3084}"/>
+    <hyperlink ref="H72" r:id="rId70" xr:uid="{1ADC2FA9-A40D-2342-AF59-4D3059BF57B0}"/>
+    <hyperlink ref="H73" r:id="rId71" xr:uid="{9F6B7A2B-23E0-EA42-B956-D30AB33B2F7C}"/>
+    <hyperlink ref="H74" r:id="rId72" xr:uid="{715BAB7D-D261-D644-9AD8-6310DFA1F7E1}"/>
+    <hyperlink ref="H75" r:id="rId73" xr:uid="{B24576B4-D3A6-A14B-BBB7-4BBB7D423548}"/>
+    <hyperlink ref="H76" r:id="rId74" xr:uid="{1B2967DE-C72E-6744-A27A-E26017E7EDBD}"/>
+    <hyperlink ref="H77" r:id="rId75" xr:uid="{582BE366-16AF-C04A-8CC6-695DAA349893}"/>
+    <hyperlink ref="H78" r:id="rId76" xr:uid="{35BED227-43E1-B447-87BF-A30AD5F6719E}"/>
+    <hyperlink ref="H79" r:id="rId77" xr:uid="{58B8327E-CCC9-E840-9125-B8A3825ED800}"/>
+    <hyperlink ref="H80" r:id="rId78" xr:uid="{948B72B0-8A37-5941-B75D-E466F596BC2A}"/>
+    <hyperlink ref="H81" r:id="rId79" xr:uid="{28B301A0-9294-A64C-9D93-EEFBA997269B}"/>
+    <hyperlink ref="H82" r:id="rId80" xr:uid="{107E48B9-22C5-7D4D-8A1C-AE3718914DFA}"/>
+    <hyperlink ref="H83" r:id="rId81" xr:uid="{03A0A341-A897-5C45-8756-12035F6D355B}"/>
+    <hyperlink ref="H84" r:id="rId82" xr:uid="{0AC4D0D4-53F6-804C-9A5B-E7CA918A45E8}"/>
+    <hyperlink ref="H85" r:id="rId83" xr:uid="{2254E0F7-AC4F-3249-85F7-F5A5D9AD3AA0}"/>
+    <hyperlink ref="H86" r:id="rId84" xr:uid="{CEB6A97D-10B2-6243-9BB0-595457B0B092}"/>
+    <hyperlink ref="H87" r:id="rId85" xr:uid="{6A1410BE-42F5-D24D-8929-9D689F40F6DB}"/>
+    <hyperlink ref="H88" r:id="rId86" xr:uid="{3108121D-21AB-9D42-A4D1-98C2596A5668}"/>
+    <hyperlink ref="H95" r:id="rId87" xr:uid="{196C34E7-7A49-564E-B57E-036C482CD23C}"/>
+    <hyperlink ref="H89" r:id="rId88" xr:uid="{C7C0A0DD-6A53-4945-B828-9A641B29E3D5}"/>
+    <hyperlink ref="H90" r:id="rId89" xr:uid="{BC4CB298-7BE4-1647-85E1-D9F105DF22BD}"/>
+    <hyperlink ref="H91" r:id="rId90" xr:uid="{34B36FF9-1DE7-B54F-BAAC-BDB1B0192002}"/>
+    <hyperlink ref="H92" r:id="rId91" xr:uid="{060C2377-8023-D34C-95E4-71E6436596CB}"/>
+    <hyperlink ref="H93" r:id="rId92" xr:uid="{3B80174A-588E-7843-8D89-3808132970B4}"/>
+    <hyperlink ref="H94" r:id="rId93" xr:uid="{9645E53D-3621-FD46-8437-4C518CDFE965}"/>
+    <hyperlink ref="H96" r:id="rId94" xr:uid="{B0106854-0132-014D-8C2D-52AB517172AA}"/>
+    <hyperlink ref="H97" r:id="rId95" xr:uid="{BDAB3987-5155-9F46-83DC-5C50FFCA6295}"/>
+    <hyperlink ref="H98" r:id="rId96" xr:uid="{8A0B7C2F-56A3-2346-9AE8-955F7F2B3AE1}"/>
+    <hyperlink ref="H99" r:id="rId97" xr:uid="{7561E380-074D-C04D-9D97-FC75B63C535F}"/>
+    <hyperlink ref="H100" r:id="rId98" xr:uid="{F3DCB0B4-A87B-0C45-AD78-A2390310A1AA}"/>
+    <hyperlink ref="H101" r:id="rId99" xr:uid="{0E53CA68-795D-4C48-A675-EC9DF665131B}"/>
+    <hyperlink ref="H102" r:id="rId100" xr:uid="{D79F6DC3-F2C1-124F-8D43-4D22B47646F6}"/>
+    <hyperlink ref="H103" r:id="rId101" xr:uid="{B6A25681-9F9E-6444-951D-B087995A5857}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change filename (based on image link) and regenerate files with new filename
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C64B6-A361-9840-84AE-EFD3B3746858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531921FA-A736-0D4E-A24A-3BD7A7D7DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2880" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
@@ -1410,7 +1410,7 @@
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>208</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1461,8 +1461,24 @@
       <c r="H2" s="14" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="str">
+        <f>_xlfn.TEXTAFTER(H2,"image/")</f>
+        <v>82441</v>
+      </c>
+      <c r="K2" t="str">
+        <f>_xlfn.TEXTAFTER(B2,"pem")</f>
+        <v>82441_aquit</v>
+      </c>
+      <c r="L2" t="str">
+        <f>_xlfn.TEXTBEFORE(K2,"_")</f>
+        <v>82441</v>
+      </c>
+      <c r="M2" t="b">
+        <f>IF(J2=L2, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1490,8 +1506,24 @@
       <c r="H3" s="14" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="3">_xlfn.TEXTAFTER(H3,"image/")</f>
+        <v>85041</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="4">_xlfn.TEXTAFTER(B3,"pem")</f>
+        <v>85041_square</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L66" si="5">_xlfn.TEXTBEFORE(K3,"_")</f>
+        <v>85041</v>
+      </c>
+      <c r="M3" t="b">
+        <f t="shared" ref="M3:M66" si="6">IF(J3=L3, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1519,8 +1551,24 @@
       <c r="H4" s="14" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
+        <v>56766</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>56766_aquit</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>56766</v>
+      </c>
+      <c r="M4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1548,8 +1596,24 @@
       <c r="H5" s="14" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>84909</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>84909_square</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>84909</v>
+      </c>
+      <c r="M5" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1577,8 +1641,24 @@
       <c r="H6" s="14" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>84540</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>84540_aquit</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>84540</v>
+      </c>
+      <c r="M6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1606,8 +1686,24 @@
       <c r="H7" s="14" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>84623</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>84623_aquit</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>84623</v>
+      </c>
+      <c r="M7" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1638,8 +1734,24 @@
       <c r="I8" s="8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>84873</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>84873_square</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>84873</v>
+      </c>
+      <c r="M8" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1667,8 +1779,24 @@
       <c r="H9" s="15" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>84614</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>84614_aquit</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>84614</v>
+      </c>
+      <c r="M9" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1696,8 +1824,24 @@
       <c r="H10" s="15" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>84548</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>84548_aquit</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>84548</v>
+      </c>
+      <c r="M10" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1725,8 +1869,24 @@
       <c r="H11" s="14" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>84882</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>84882_square</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>84882</v>
+      </c>
+      <c r="M11" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1754,8 +1914,24 @@
       <c r="H12" s="15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>84878</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>84878_square</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>84878</v>
+      </c>
+      <c r="M12" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1786,8 +1962,24 @@
       <c r="I13" s="8" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>86239</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>86239_square</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>86239</v>
+      </c>
+      <c r="M13" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1815,8 +2007,24 @@
       <c r="H14" s="15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>84630</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>84630_aquit</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>84630</v>
+      </c>
+      <c r="M14" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1844,8 +2052,24 @@
       <c r="H15" s="15" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>84881</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>84881_square</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>84881</v>
+      </c>
+      <c r="M15" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1873,8 +2097,24 @@
       <c r="H16" s="15" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>84534</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>84534_aquit</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>84534</v>
+      </c>
+      <c r="M16" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1902,8 +2142,24 @@
       <c r="H17" s="11" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>84863</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="4"/>
+        <v>84863_square</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="5"/>
+        <v>84863</v>
+      </c>
+      <c r="M17" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1931,8 +2187,24 @@
       <c r="H18" s="11" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>83892</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>83892_aquit</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>83892</v>
+      </c>
+      <c r="M18" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1960,8 +2232,24 @@
       <c r="H19" s="11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>85059</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>85059_square</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>85059</v>
+      </c>
+      <c r="M19" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1989,8 +2277,24 @@
       <c r="H20" s="11" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>84600</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>84600_aquit</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>84600</v>
+      </c>
+      <c r="M20" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2018,8 +2322,24 @@
       <c r="H21" s="11" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J21" t="str">
+        <f t="shared" si="3"/>
+        <v>83880</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>83880_aquit</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>83880</v>
+      </c>
+      <c r="M21" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2047,8 +2367,24 @@
       <c r="H22" s="11" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>84880</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>84880_square</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>84880</v>
+      </c>
+      <c r="M22" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2076,8 +2412,24 @@
       <c r="H23" s="12" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="str">
+        <f t="shared" si="3"/>
+        <v>84580</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>84580_aquit</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>84580</v>
+      </c>
+      <c r="M23" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2105,8 +2457,24 @@
       <c r="H24" s="9" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>85056</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>85056_square</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>85056</v>
+      </c>
+      <c r="M24" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2134,8 +2502,24 @@
       <c r="H25" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>83911</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>83911_aquit</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>83911</v>
+      </c>
+      <c r="M25" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2163,8 +2547,24 @@
       <c r="H26" s="11" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J26" t="str">
+        <f t="shared" si="3"/>
+        <v>84665</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>84665_aquit</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>84665</v>
+      </c>
+      <c r="M26" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2195,8 +2595,24 @@
       <c r="I27" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="str">
+        <f t="shared" si="3"/>
+        <v>84905</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>84905_square</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>84905</v>
+      </c>
+      <c r="M27" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2224,8 +2640,24 @@
       <c r="H28" s="14" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>84532</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>84532_aquit</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>84532</v>
+      </c>
+      <c r="M28" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2253,8 +2685,24 @@
       <c r="H29" s="11" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="str">
+        <f t="shared" si="3"/>
+        <v>84919</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>84919_square</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>84919</v>
+      </c>
+      <c r="M29" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2282,8 +2730,24 @@
       <c r="H30" s="14" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J30" t="str">
+        <f t="shared" si="3"/>
+        <v>84595</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>84595_aquit</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>84595</v>
+      </c>
+      <c r="M30" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2311,8 +2775,24 @@
       <c r="H31" s="11" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J31" t="str">
+        <f t="shared" si="3"/>
+        <v>84872</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>84872_square</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>84872</v>
+      </c>
+      <c r="M31" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2339,6 +2819,22 @@
       </c>
       <c r="H32" s="11" t="s">
         <v>250</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="3"/>
+        <v>84666</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>84666_aquit</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>84666</v>
+      </c>
+      <c r="M32" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2369,6 +2865,22 @@
       <c r="H33" s="11" t="s">
         <v>251</v>
       </c>
+      <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>84874</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>84874_square</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>84874</v>
+      </c>
+      <c r="M33" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -2398,6 +2910,22 @@
       <c r="H34" s="11" t="s">
         <v>252</v>
       </c>
+      <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>76616</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="4"/>
+        <v>76616_aquit</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="5"/>
+        <v>76616</v>
+      </c>
+      <c r="M34" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -2427,6 +2955,22 @@
       <c r="H35" s="11" t="s">
         <v>253</v>
       </c>
+      <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>119191</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="4"/>
+        <v>11919_aquit</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="5"/>
+        <v>11919</v>
+      </c>
+      <c r="M35" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -2456,6 +3000,22 @@
       <c r="H36" s="11" t="s">
         <v>254</v>
       </c>
+      <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>84924</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="4"/>
+        <v>84924_square</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="5"/>
+        <v>84924</v>
+      </c>
+      <c r="M36" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -2485,6 +3045,22 @@
       <c r="H37" s="11" t="s">
         <v>255</v>
       </c>
+      <c r="J37" t="str">
+        <f t="shared" si="3"/>
+        <v>84057</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="4"/>
+        <v>84057_aquit</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="5"/>
+        <v>84057</v>
+      </c>
+      <c r="M37" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
@@ -2517,10 +3093,22 @@
       <c r="I38" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
+      <c r="J38" t="str">
+        <f t="shared" si="3"/>
+        <v>85065</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="4"/>
+        <v>85065_square</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="5"/>
+        <v>85065</v>
+      </c>
+      <c r="M38" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -2550,6 +3138,22 @@
       <c r="H39" s="11" t="s">
         <v>257</v>
       </c>
+      <c r="J39" t="str">
+        <f t="shared" si="3"/>
+        <v>83876</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="4"/>
+        <v>83876_aquit</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="5"/>
+        <v>83876</v>
+      </c>
+      <c r="M39" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2579,6 +3183,22 @@
       <c r="H40" s="11" t="s">
         <v>258</v>
       </c>
+      <c r="J40" t="str">
+        <f t="shared" si="3"/>
+        <v>85073</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="4"/>
+        <v>85073_square</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="5"/>
+        <v>85073</v>
+      </c>
+      <c r="M40" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -2608,6 +3228,22 @@
       <c r="H41" s="11" t="s">
         <v>259</v>
       </c>
+      <c r="J41" t="str">
+        <f t="shared" si="3"/>
+        <v>83869</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="4"/>
+        <v>83869_aquit</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="5"/>
+        <v>83869</v>
+      </c>
+      <c r="M41" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2637,6 +3273,22 @@
       <c r="H42" s="11" t="s">
         <v>260</v>
       </c>
+      <c r="J42" t="str">
+        <f t="shared" si="3"/>
+        <v>84946</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="4"/>
+        <v>84946_square</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="5"/>
+        <v>84946</v>
+      </c>
+      <c r="M42" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -2666,6 +3318,22 @@
       <c r="H43" s="11" t="s">
         <v>261</v>
       </c>
+      <c r="J43" t="str">
+        <f t="shared" si="3"/>
+        <v>84570</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="4"/>
+        <v>84570_aquit</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="5"/>
+        <v>84570</v>
+      </c>
+      <c r="M43" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -2695,6 +3363,22 @@
       <c r="H44" s="11" t="s">
         <v>262</v>
       </c>
+      <c r="J44" t="str">
+        <f t="shared" si="3"/>
+        <v>85037</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="4"/>
+        <v>85037_square</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="5"/>
+        <v>85037</v>
+      </c>
+      <c r="M44" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2724,6 +3408,22 @@
       <c r="H45" s="11" t="s">
         <v>263</v>
       </c>
+      <c r="J45" t="str">
+        <f t="shared" si="3"/>
+        <v>85014</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="4"/>
+        <v>85014_aquit</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="5"/>
+        <v>85014</v>
+      </c>
+      <c r="M45" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -2753,6 +3453,22 @@
       <c r="H46" s="11" t="s">
         <v>264</v>
       </c>
+      <c r="J46" t="str">
+        <f t="shared" si="3"/>
+        <v>71059</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="4"/>
+        <v>71059_square</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="5"/>
+        <v>71059</v>
+      </c>
+      <c r="M46" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2782,6 +3498,22 @@
       <c r="H47" s="11" t="s">
         <v>265</v>
       </c>
+      <c r="J47" t="str">
+        <f t="shared" si="3"/>
+        <v>85026</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="4"/>
+        <v>85026_aquit</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="5"/>
+        <v>85026</v>
+      </c>
+      <c r="M47" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2814,8 +3546,24 @@
       <c r="I48" s="8" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J48" t="str">
+        <f t="shared" si="3"/>
+        <v>71210</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="4"/>
+        <v>71210_square</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="5"/>
+        <v>71210</v>
+      </c>
+      <c r="M48" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2843,8 +3591,24 @@
       <c r="H49" s="11" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J49" t="str">
+        <f t="shared" si="3"/>
+        <v>85972</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="4"/>
+        <v>85972_square</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="5"/>
+        <v>85972</v>
+      </c>
+      <c r="M49" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2872,8 +3636,24 @@
       <c r="H50" s="11" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J50" t="str">
+        <f t="shared" si="3"/>
+        <v>86078</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="4"/>
+        <v>86078_square</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="5"/>
+        <v>86078</v>
+      </c>
+      <c r="M50" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -2901,8 +3681,24 @@
       <c r="H51" s="11" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J51" t="str">
+        <f t="shared" si="3"/>
+        <v>85023</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="4"/>
+        <v>85023_square</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="5"/>
+        <v>85023</v>
+      </c>
+      <c r="M51" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2930,8 +3726,24 @@
       <c r="H52" s="11" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J52" t="str">
+        <f t="shared" si="3"/>
+        <v>80113</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="4"/>
+        <v>80113_aquit</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="5"/>
+        <v>80113</v>
+      </c>
+      <c r="M52" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -2959,8 +3771,24 @@
       <c r="H53" s="11" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J53" t="str">
+        <f t="shared" si="3"/>
+        <v>71112</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="4"/>
+        <v>71112_square</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="5"/>
+        <v>71112</v>
+      </c>
+      <c r="M53" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -2988,8 +3816,24 @@
       <c r="H54" s="11" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J54" t="str">
+        <f t="shared" si="3"/>
+        <v>80209</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="4"/>
+        <v>80209_aquit</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="5"/>
+        <v>80209</v>
+      </c>
+      <c r="M54" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -3020,8 +3864,24 @@
       <c r="I55" s="8" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="J55" t="str">
+        <f t="shared" si="3"/>
+        <v>71032</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="4"/>
+        <v>71032_square</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="5"/>
+        <v>71032</v>
+      </c>
+      <c r="M55" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -3049,8 +3909,24 @@
       <c r="H56" s="10" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J56" t="str">
+        <f>_xlfn.TEXTAFTER(H56,"image/")</f>
+        <v>80148; https://pemdatabase.eu/image/80149</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="4"/>
+        <v>80148-80149_aquit</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="5"/>
+        <v>80148-80149</v>
+      </c>
+      <c r="M56" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -3078,8 +3954,24 @@
       <c r="H57" s="11" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J57" t="str">
+        <f t="shared" si="3"/>
+        <v>71205</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="4"/>
+        <v>71205_square</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="5"/>
+        <v>71205</v>
+      </c>
+      <c r="M57" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -3107,8 +3999,24 @@
       <c r="H58" s="11" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J58" t="str">
+        <f t="shared" si="3"/>
+        <v>86046</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="4"/>
+        <v>86046_aquit</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="5"/>
+        <v>86046</v>
+      </c>
+      <c r="M58" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -3136,8 +4044,24 @@
       <c r="H59" s="11" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" t="str">
+        <f t="shared" si="3"/>
+        <v>85997</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="4"/>
+        <v>85997_square</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="5"/>
+        <v>85997</v>
+      </c>
+      <c r="M59" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -3165,8 +4089,24 @@
       <c r="H60" s="14" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J60" t="str">
+        <f t="shared" si="3"/>
+        <v>80028</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="4"/>
+        <v>80028_aquit</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="5"/>
+        <v>80028</v>
+      </c>
+      <c r="M60" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -3197,8 +4137,24 @@
       <c r="I61" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J61" t="str">
+        <f t="shared" si="3"/>
+        <v>71128</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="4"/>
+        <v>71128_square</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="5"/>
+        <v>71128</v>
+      </c>
+      <c r="M61" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -3226,8 +4182,24 @@
       <c r="H62" s="11" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J62" t="str">
+        <f t="shared" si="3"/>
+        <v>85921</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="4"/>
+        <v>85921_square</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="5"/>
+        <v>85921</v>
+      </c>
+      <c r="M62" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -3255,8 +4227,24 @@
       <c r="H63" s="11" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J63" t="str">
+        <f t="shared" si="3"/>
+        <v>86009</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="4"/>
+        <v>86009_square</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="5"/>
+        <v>86009</v>
+      </c>
+      <c r="M63" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -3284,8 +4272,24 @@
       <c r="H64" s="11" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" t="str">
+        <f t="shared" si="3"/>
+        <v>84967</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="4"/>
+        <v>84967_square</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="5"/>
+        <v>84967</v>
+      </c>
+      <c r="M64" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -3313,8 +4317,24 @@
       <c r="H65" s="14" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J65" t="str">
+        <f t="shared" si="3"/>
+        <v>84633</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="4"/>
+        <v>84633_aquit</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="5"/>
+        <v>84633</v>
+      </c>
+      <c r="M65" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -3345,8 +4365,24 @@
       <c r="I66" s="8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J66" t="str">
+        <f t="shared" si="3"/>
+        <v>85642</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="4"/>
+        <v>85642_square</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="5"/>
+        <v>85642</v>
+      </c>
+      <c r="M66" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -3360,22 +4396,38 @@
         <v>206</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E103" si="3">RIGHT(B67, 6)</f>
+        <f t="shared" ref="E67:E103" si="7">RIGHT(B67, 6)</f>
         <v>square</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F103" si="4">IF(E67="square","-notation square","")</f>
+        <f t="shared" ref="F67:F103" si="8">IF(E67="square","-notation square","")</f>
         <v>-notation square</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G103" si="5">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
+        <f t="shared" ref="G67:G103" si="9">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
       <c r="H67" s="11" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J103" si="10">_xlfn.TEXTAFTER(H67,"image/")</f>
+        <v>71108</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K103" si="11">_xlfn.TEXTAFTER(B67,"pem")</f>
+        <v>71108_square</v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L103" si="12">_xlfn.TEXTBEFORE(K67,"_")</f>
+        <v>71108</v>
+      </c>
+      <c r="M67" t="b">
+        <f t="shared" ref="M67:M103" si="13">IF(J67=L67, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3389,22 +4441,38 @@
         <v>207</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
       <c r="H68" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J68" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M68" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3418,22 +4486,38 @@
         <v>207</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
       <c r="H69" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J69" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M69" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -3447,22 +4531,38 @@
         <v>207</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
       <c r="H70" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J70" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M70" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -3476,22 +4576,38 @@
         <v>207</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J71" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M71" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -3505,22 +4621,38 @@
         <v>207</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
       <c r="H72" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J72" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M72" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -3534,22 +4666,38 @@
         <v>207</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J73" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M73" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -3563,22 +4711,38 @@
         <v>207</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
       <c r="H74" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J74" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M74" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -3592,15 +4756,15 @@
         <v>207</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
       <c r="H75" s="11" t="s">
@@ -3609,8 +4773,24 @@
       <c r="I75" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J75" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M75" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3624,22 +4804,38 @@
         <v>207</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
       <c r="H76" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J76" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M76" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -3653,22 +4849,38 @@
         <v>207</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H77" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J77" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M77" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -3682,22 +4894,38 @@
         <v>207</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
       <c r="H78" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J78" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M78" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -3711,22 +4939,38 @@
         <v>207</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H79" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J79" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M79" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -3740,22 +4984,38 @@
         <v>207</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
       <c r="H80" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J80" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M80" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>67</v>
       </c>
@@ -3769,22 +5029,38 @@
         <v>207</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H81" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J81" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L81" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M81" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -3798,22 +5074,38 @@
         <v>207</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
       <c r="H82" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J82" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M82" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>67</v>
       </c>
@@ -3827,22 +5119,38 @@
         <v>207</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
       <c r="H83" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J83" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M83" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>67</v>
       </c>
@@ -3856,22 +5164,38 @@
         <v>207</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
       <c r="H84" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J84" t="str">
+        <f t="shared" si="10"/>
+        <v>92154</v>
+      </c>
+      <c r="K84" t="str">
+        <f t="shared" si="11"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="12"/>
+        <v>92154</v>
+      </c>
+      <c r="M84" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>67</v>
       </c>
@@ -3885,22 +5209,38 @@
         <v>207</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
       <c r="H85" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J85" t="str">
+        <f t="shared" si="10"/>
+        <v>71010</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" si="11"/>
+        <v>71010_square</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="12"/>
+        <v>71010</v>
+      </c>
+      <c r="M85" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -3914,22 +5254,38 @@
         <v>207</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
       <c r="H86" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J86" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K86" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M86" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -3943,22 +5299,38 @@
         <v>207</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
       <c r="H87" s="11" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J87" t="str">
+        <f t="shared" si="10"/>
+        <v>71012</v>
+      </c>
+      <c r="K87" t="str">
+        <f t="shared" si="11"/>
+        <v>71012_square</v>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="12"/>
+        <v>71012</v>
+      </c>
+      <c r="M87" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>67</v>
       </c>
@@ -3972,22 +5344,38 @@
         <v>207</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
       <c r="H88" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J88" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K88" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M88" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>67</v>
       </c>
@@ -4001,22 +5389,38 @@
         <v>207</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J89" t="str">
+        <f t="shared" si="10"/>
+        <v>71012</v>
+      </c>
+      <c r="K89" t="str">
+        <f t="shared" si="11"/>
+        <v>71012_square</v>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="12"/>
+        <v>71012</v>
+      </c>
+      <c r="M89" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>67</v>
       </c>
@@ -4030,22 +5434,38 @@
         <v>207</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
       <c r="H90" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J90" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K90" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M90" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>67</v>
       </c>
@@ -4059,22 +5479,38 @@
         <v>207</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J91" t="str">
+        <f t="shared" si="10"/>
+        <v>71012</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="11"/>
+        <v>71012_square</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="12"/>
+        <v>71012</v>
+      </c>
+      <c r="M91" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>67</v>
       </c>
@@ -4088,22 +5524,38 @@
         <v>207</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
       <c r="H92" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J92" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K92" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M92" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>67</v>
       </c>
@@ -4117,22 +5569,38 @@
         <v>207</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J93" t="str">
+        <f t="shared" si="10"/>
+        <v>71012</v>
+      </c>
+      <c r="K93" t="str">
+        <f t="shared" si="11"/>
+        <v>71012_square</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="12"/>
+        <v>71012</v>
+      </c>
+      <c r="M93" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>67</v>
       </c>
@@ -4146,22 +5614,38 @@
         <v>207</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
       <c r="H94" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J94" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K94" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M94" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>67</v>
       </c>
@@ -4175,22 +5659,38 @@
         <v>207</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
       <c r="H95" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J95" t="str">
+        <f t="shared" si="10"/>
+        <v>71013</v>
+      </c>
+      <c r="K95" t="str">
+        <f t="shared" si="11"/>
+        <v>71013_square</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" si="12"/>
+        <v>71013</v>
+      </c>
+      <c r="M95" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>67</v>
       </c>
@@ -4204,22 +5704,38 @@
         <v>207</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
       <c r="H96" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J96" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K96" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L96" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M96" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>67</v>
       </c>
@@ -4233,22 +5749,38 @@
         <v>207</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
       <c r="H97" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J97" t="str">
+        <f t="shared" si="10"/>
+        <v>71013</v>
+      </c>
+      <c r="K97" t="str">
+        <f t="shared" si="11"/>
+        <v>71013_square</v>
+      </c>
+      <c r="L97" t="str">
+        <f t="shared" si="12"/>
+        <v>71013</v>
+      </c>
+      <c r="M97" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>67</v>
       </c>
@@ -4262,22 +5794,38 @@
         <v>207</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
       <c r="H98" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J98" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K98" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L98" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M98" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>67</v>
       </c>
@@ -4291,22 +5839,38 @@
         <v>207</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
       <c r="H99" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J99" t="str">
+        <f t="shared" si="10"/>
+        <v>71013</v>
+      </c>
+      <c r="K99" t="str">
+        <f t="shared" si="11"/>
+        <v>71013_square</v>
+      </c>
+      <c r="L99" t="str">
+        <f t="shared" si="12"/>
+        <v>71013</v>
+      </c>
+      <c r="M99" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>67</v>
       </c>
@@ -4320,22 +5884,38 @@
         <v>207</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
       <c r="H100" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J100" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K100" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L100" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M100" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>67</v>
       </c>
@@ -4349,22 +5929,38 @@
         <v>207</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
       <c r="H101" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J101" t="str">
+        <f t="shared" si="10"/>
+        <v>71013</v>
+      </c>
+      <c r="K101" t="str">
+        <f t="shared" si="11"/>
+        <v>71013_square</v>
+      </c>
+      <c r="L101" t="str">
+        <f t="shared" si="12"/>
+        <v>71013</v>
+      </c>
+      <c r="M101" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>67</v>
       </c>
@@ -4378,22 +5974,38 @@
         <v>207</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>_aquit</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
       <c r="H102" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J102" t="str">
+        <f t="shared" si="10"/>
+        <v>80159</v>
+      </c>
+      <c r="K102" t="str">
+        <f t="shared" si="11"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="L102" t="str">
+        <f t="shared" si="12"/>
+        <v>80159</v>
+      </c>
+      <c r="M102" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>67</v>
       </c>
@@ -4407,22 +6019,38 @@
         <v>207</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>square</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-notation square</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
       <c r="H103" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J103" t="str">
+        <f t="shared" si="10"/>
+        <v>71013</v>
+      </c>
+      <c r="K103" t="str">
+        <f t="shared" si="11"/>
+        <v>71013_square</v>
+      </c>
+      <c r="L103" t="str">
+        <f t="shared" si="12"/>
+        <v>71013</v>
+      </c>
+      <c r="M103" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H104" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Highlight when filename don't match the link
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531921FA-A736-0D4E-A24A-3BD7A7D7DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28C204-63E2-E64A-B826-37E367FDD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2880" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="1260" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="292">
   <si>
     <t>01_benedicte-omnes_pem82441_aquit</t>
   </si>
@@ -938,12 +938,15 @@
   <si>
     <t>https://pemdatabase.eu/image/71013</t>
   </si>
+  <si>
+    <t>Evaluation of links vs. filenames</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -973,6 +976,14 @@
       <sz val="12"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1020,7 +1031,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1043,12 +1054,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1058,27 +1084,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1388,13 +1443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CAB5ED-65C4-C540-BBD9-8DBFB51E3378}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:M1048576"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,9 +1463,12 @@
     <col min="7" max="7" width="214" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>208</v>
       </c>
@@ -1432,8 +1490,14 @@
       <c r="G1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1461,24 +1525,24 @@
       <c r="H2" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H2,"image/")</f>
         <v>82441</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" s="18" t="str">
         <f>_xlfn.TEXTAFTER(B2,"pem")</f>
         <v>82441_aquit</v>
       </c>
-      <c r="L2" t="str">
-        <f>_xlfn.TEXTBEFORE(K2,"_")</f>
+      <c r="M2" s="18" t="str">
+        <f>_xlfn.TEXTBEFORE(L2,"_")</f>
         <v>82441</v>
       </c>
-      <c r="M2" t="b">
-        <f>IF(J2=L2, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="20" t="b">
+        <f>IF(K2=M2, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1506,24 +1570,24 @@
       <c r="H3" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="3">_xlfn.TEXTAFTER(H3,"image/")</f>
+      <c r="K3" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H3,"image/")</f>
         <v>85041</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K66" si="4">_xlfn.TEXTAFTER(B3,"pem")</f>
+      <c r="L3" s="18" t="str">
+        <f t="shared" ref="L3:L66" si="3">_xlfn.TEXTAFTER(B3,"pem")</f>
         <v>85041_square</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L66" si="5">_xlfn.TEXTBEFORE(K3,"_")</f>
+      <c r="M3" s="18" t="str">
+        <f t="shared" ref="M3:M66" si="4">_xlfn.TEXTBEFORE(L3,"_")</f>
         <v>85041</v>
       </c>
-      <c r="M3" t="b">
-        <f t="shared" ref="M3:M66" si="6">IF(J3=L3, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="20" t="b">
+        <f t="shared" ref="N3:N66" si="5">IF(K3=M3, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1551,24 +1615,24 @@
       <c r="H4" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H4,"image/")</f>
+        <v>56766</v>
+      </c>
+      <c r="L4" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>56766_aquit</v>
+      </c>
+      <c r="M4" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>56766</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" si="4"/>
-        <v>56766_aquit</v>
-      </c>
-      <c r="L4" t="str">
+      <c r="N4" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>56766</v>
-      </c>
-      <c r="M4" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1596,24 +1660,24 @@
       <c r="H5" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H5,"image/")</f>
+        <v>84909</v>
+      </c>
+      <c r="L5" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84909_square</v>
+      </c>
+      <c r="M5" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84909</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>84909_square</v>
-      </c>
-      <c r="L5" t="str">
+      <c r="N5" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84909</v>
-      </c>
-      <c r="M5" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1641,24 +1705,24 @@
       <c r="H6" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H6,"image/")</f>
+        <v>84540</v>
+      </c>
+      <c r="L6" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84540_aquit</v>
+      </c>
+      <c r="M6" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84540</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" si="4"/>
-        <v>84540_aquit</v>
-      </c>
-      <c r="L6" t="str">
+      <c r="N6" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84540</v>
-      </c>
-      <c r="M6" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1686,24 +1750,24 @@
       <c r="H7" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H7,"image/")</f>
+        <v>84623</v>
+      </c>
+      <c r="L7" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84623_aquit</v>
+      </c>
+      <c r="M7" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84623</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v>84623_aquit</v>
-      </c>
-      <c r="L7" t="str">
+      <c r="N7" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84623</v>
-      </c>
-      <c r="M7" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1734,24 +1798,24 @@
       <c r="I8" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H8,"image/")</f>
+        <v>84873</v>
+      </c>
+      <c r="L8" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84873_square</v>
+      </c>
+      <c r="M8" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84873</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v>84873_square</v>
-      </c>
-      <c r="L8" t="str">
+      <c r="N8" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84873</v>
-      </c>
-      <c r="M8" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1779,24 +1843,24 @@
       <c r="H9" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H9,"image/")</f>
+        <v>84614</v>
+      </c>
+      <c r="L9" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84614_aquit</v>
+      </c>
+      <c r="M9" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84614</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" si="4"/>
-        <v>84614_aquit</v>
-      </c>
-      <c r="L9" t="str">
+      <c r="N9" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84614</v>
-      </c>
-      <c r="M9" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1824,24 +1888,24 @@
       <c r="H10" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H10,"image/")</f>
+        <v>84548</v>
+      </c>
+      <c r="L10" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84548_aquit</v>
+      </c>
+      <c r="M10" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84548</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" si="4"/>
-        <v>84548_aquit</v>
-      </c>
-      <c r="L10" t="str">
+      <c r="N10" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84548</v>
-      </c>
-      <c r="M10" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1869,24 +1933,24 @@
       <c r="H11" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H11,"image/")</f>
+        <v>84882</v>
+      </c>
+      <c r="L11" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84882_square</v>
+      </c>
+      <c r="M11" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84882</v>
       </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v>84882_square</v>
-      </c>
-      <c r="L11" t="str">
+      <c r="N11" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84882</v>
-      </c>
-      <c r="M11" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1914,24 +1978,24 @@
       <c r="H12" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H12,"image/")</f>
+        <v>84878</v>
+      </c>
+      <c r="L12" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84878_square</v>
+      </c>
+      <c r="M12" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84878</v>
       </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>84878_square</v>
-      </c>
-      <c r="L12" t="str">
+      <c r="N12" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84878</v>
-      </c>
-      <c r="M12" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1962,24 +2026,24 @@
       <c r="I13" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H13,"image/")</f>
+        <v>86239</v>
+      </c>
+      <c r="L13" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>86239_square</v>
+      </c>
+      <c r="M13" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>86239</v>
       </c>
-      <c r="K13" t="str">
-        <f t="shared" si="4"/>
-        <v>86239_square</v>
-      </c>
-      <c r="L13" t="str">
+      <c r="N13" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>86239</v>
-      </c>
-      <c r="M13" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2007,24 +2071,24 @@
       <c r="H14" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H14,"image/")</f>
+        <v>84630</v>
+      </c>
+      <c r="L14" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84630_aquit</v>
+      </c>
+      <c r="M14" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84630</v>
       </c>
-      <c r="K14" t="str">
-        <f t="shared" si="4"/>
-        <v>84630_aquit</v>
-      </c>
-      <c r="L14" t="str">
+      <c r="N14" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84630</v>
-      </c>
-      <c r="M14" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2052,24 +2116,24 @@
       <c r="H15" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H15,"image/")</f>
+        <v>84881</v>
+      </c>
+      <c r="L15" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84881_square</v>
+      </c>
+      <c r="M15" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84881</v>
       </c>
-      <c r="K15" t="str">
-        <f t="shared" si="4"/>
-        <v>84881_square</v>
-      </c>
-      <c r="L15" t="str">
+      <c r="N15" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84881</v>
-      </c>
-      <c r="M15" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2097,24 +2161,24 @@
       <c r="H16" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H16,"image/")</f>
+        <v>84534</v>
+      </c>
+      <c r="L16" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84534_aquit</v>
+      </c>
+      <c r="M16" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84534</v>
       </c>
-      <c r="K16" t="str">
-        <f t="shared" si="4"/>
-        <v>84534_aquit</v>
-      </c>
-      <c r="L16" t="str">
+      <c r="N16" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84534</v>
-      </c>
-      <c r="M16" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -2142,24 +2206,24 @@
       <c r="H17" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H17,"image/")</f>
+        <v>84863</v>
+      </c>
+      <c r="L17" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84863_square</v>
+      </c>
+      <c r="M17" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84863</v>
       </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v>84863_square</v>
-      </c>
-      <c r="L17" t="str">
+      <c r="N17" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84863</v>
-      </c>
-      <c r="M17" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2187,24 +2251,24 @@
       <c r="H18" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H18,"image/")</f>
+        <v>83892</v>
+      </c>
+      <c r="L18" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>83892_aquit</v>
+      </c>
+      <c r="M18" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>83892</v>
       </c>
-      <c r="K18" t="str">
-        <f t="shared" si="4"/>
-        <v>83892_aquit</v>
-      </c>
-      <c r="L18" t="str">
+      <c r="N18" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>83892</v>
-      </c>
-      <c r="M18" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2232,24 +2296,24 @@
       <c r="H19" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H19,"image/")</f>
+        <v>85059</v>
+      </c>
+      <c r="L19" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85059_square</v>
+      </c>
+      <c r="M19" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85059</v>
       </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v>85059_square</v>
-      </c>
-      <c r="L19" t="str">
+      <c r="N19" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85059</v>
-      </c>
-      <c r="M19" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2277,24 +2341,24 @@
       <c r="H20" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H20,"image/")</f>
+        <v>84600</v>
+      </c>
+      <c r="L20" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84600_aquit</v>
+      </c>
+      <c r="M20" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84600</v>
       </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>84600_aquit</v>
-      </c>
-      <c r="L20" t="str">
+      <c r="N20" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84600</v>
-      </c>
-      <c r="M20" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2322,24 +2386,24 @@
       <c r="H21" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="J21" t="str">
+      <c r="K21" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H21,"image/")</f>
+        <v>83880</v>
+      </c>
+      <c r="L21" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>83880_aquit</v>
+      </c>
+      <c r="M21" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>83880</v>
       </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
-        <v>83880_aquit</v>
-      </c>
-      <c r="L21" t="str">
+      <c r="N21" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>83880</v>
-      </c>
-      <c r="M21" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2367,24 +2431,24 @@
       <c r="H22" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="J22" t="str">
+      <c r="K22" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H22,"image/")</f>
+        <v>84880</v>
+      </c>
+      <c r="L22" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84880_square</v>
+      </c>
+      <c r="M22" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84880</v>
       </c>
-      <c r="K22" t="str">
-        <f t="shared" si="4"/>
-        <v>84880_square</v>
-      </c>
-      <c r="L22" t="str">
+      <c r="N22" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84880</v>
-      </c>
-      <c r="M22" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2412,24 +2476,24 @@
       <c r="H23" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="J23" t="str">
+      <c r="K23" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H23,"image/")</f>
+        <v>84580</v>
+      </c>
+      <c r="L23" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84580_aquit</v>
+      </c>
+      <c r="M23" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84580</v>
       </c>
-      <c r="K23" t="str">
-        <f t="shared" si="4"/>
-        <v>84580_aquit</v>
-      </c>
-      <c r="L23" t="str">
+      <c r="N23" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84580</v>
-      </c>
-      <c r="M23" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2457,24 +2521,24 @@
       <c r="H24" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="J24" t="str">
+      <c r="K24" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H24,"image/")</f>
+        <v>85056</v>
+      </c>
+      <c r="L24" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85056_square</v>
+      </c>
+      <c r="M24" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85056</v>
       </c>
-      <c r="K24" t="str">
-        <f t="shared" si="4"/>
-        <v>85056_square</v>
-      </c>
-      <c r="L24" t="str">
+      <c r="N24" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85056</v>
-      </c>
-      <c r="M24" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2502,24 +2566,24 @@
       <c r="H25" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="J25" t="str">
+      <c r="K25" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H25,"image/")</f>
+        <v>83911</v>
+      </c>
+      <c r="L25" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>83911_aquit</v>
+      </c>
+      <c r="M25" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>83911</v>
       </c>
-      <c r="K25" t="str">
-        <f t="shared" si="4"/>
-        <v>83911_aquit</v>
-      </c>
-      <c r="L25" t="str">
+      <c r="N25" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>83911</v>
-      </c>
-      <c r="M25" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2547,24 +2611,24 @@
       <c r="H26" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="J26" t="str">
+      <c r="K26" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H26,"image/")</f>
+        <v>84665</v>
+      </c>
+      <c r="L26" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84665_aquit</v>
+      </c>
+      <c r="M26" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84665</v>
       </c>
-      <c r="K26" t="str">
-        <f t="shared" si="4"/>
-        <v>84665_aquit</v>
-      </c>
-      <c r="L26" t="str">
+      <c r="N26" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84665</v>
-      </c>
-      <c r="M26" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2595,24 +2659,24 @@
       <c r="I27" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="J27" t="str">
+      <c r="K27" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H27,"image/")</f>
+        <v>84905</v>
+      </c>
+      <c r="L27" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84905_square</v>
+      </c>
+      <c r="M27" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84905</v>
       </c>
-      <c r="K27" t="str">
-        <f t="shared" si="4"/>
-        <v>84905_square</v>
-      </c>
-      <c r="L27" t="str">
+      <c r="N27" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84905</v>
-      </c>
-      <c r="M27" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2640,24 +2704,24 @@
       <c r="H28" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="J28" t="str">
+      <c r="K28" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H28,"image/")</f>
+        <v>84532</v>
+      </c>
+      <c r="L28" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84532_aquit</v>
+      </c>
+      <c r="M28" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84532</v>
       </c>
-      <c r="K28" t="str">
-        <f t="shared" si="4"/>
-        <v>84532_aquit</v>
-      </c>
-      <c r="L28" t="str">
+      <c r="N28" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84532</v>
-      </c>
-      <c r="M28" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2685,24 +2749,24 @@
       <c r="H29" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J29" t="str">
+      <c r="K29" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H29,"image/")</f>
+        <v>84919</v>
+      </c>
+      <c r="L29" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84919_square</v>
+      </c>
+      <c r="M29" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84919</v>
       </c>
-      <c r="K29" t="str">
-        <f t="shared" si="4"/>
-        <v>84919_square</v>
-      </c>
-      <c r="L29" t="str">
+      <c r="N29" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84919</v>
-      </c>
-      <c r="M29" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2730,24 +2794,24 @@
       <c r="H30" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="J30" t="str">
+      <c r="K30" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H30,"image/")</f>
+        <v>84595</v>
+      </c>
+      <c r="L30" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84595_aquit</v>
+      </c>
+      <c r="M30" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84595</v>
       </c>
-      <c r="K30" t="str">
-        <f t="shared" si="4"/>
-        <v>84595_aquit</v>
-      </c>
-      <c r="L30" t="str">
+      <c r="N30" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84595</v>
-      </c>
-      <c r="M30" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2775,24 +2839,24 @@
       <c r="H31" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="J31" t="str">
+      <c r="K31" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H31,"image/")</f>
+        <v>84872</v>
+      </c>
+      <c r="L31" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84872_square</v>
+      </c>
+      <c r="M31" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84872</v>
       </c>
-      <c r="K31" t="str">
-        <f t="shared" si="4"/>
-        <v>84872_square</v>
-      </c>
-      <c r="L31" t="str">
+      <c r="N31" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84872</v>
-      </c>
-      <c r="M31" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2820,24 +2884,24 @@
       <c r="H32" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J32" t="str">
+      <c r="K32" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H32,"image/")</f>
+        <v>84666</v>
+      </c>
+      <c r="L32" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84666_aquit</v>
+      </c>
+      <c r="M32" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84666</v>
       </c>
-      <c r="K32" t="str">
-        <f t="shared" si="4"/>
-        <v>84666_aquit</v>
-      </c>
-      <c r="L32" t="str">
+      <c r="N32" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84666</v>
-      </c>
-      <c r="M32" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2865,24 +2929,24 @@
       <c r="H33" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="J33" t="str">
+      <c r="K33" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H33,"image/")</f>
+        <v>84874</v>
+      </c>
+      <c r="L33" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84874_square</v>
+      </c>
+      <c r="M33" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84874</v>
       </c>
-      <c r="K33" t="str">
-        <f t="shared" si="4"/>
-        <v>84874_square</v>
-      </c>
-      <c r="L33" t="str">
+      <c r="N33" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84874</v>
-      </c>
-      <c r="M33" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2910,24 +2974,24 @@
       <c r="H34" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="J34" t="str">
+      <c r="K34" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H34,"image/")</f>
+        <v>76616</v>
+      </c>
+      <c r="L34" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>76616_aquit</v>
+      </c>
+      <c r="M34" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>76616</v>
       </c>
-      <c r="K34" t="str">
-        <f t="shared" si="4"/>
-        <v>76616_aquit</v>
-      </c>
-      <c r="L34" t="str">
+      <c r="N34" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>76616</v>
-      </c>
-      <c r="M34" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2955,24 +3019,24 @@
       <c r="H35" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="J35" t="str">
+      <c r="K35" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H35,"image/")</f>
+        <v>119191</v>
+      </c>
+      <c r="L35" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>119191</v>
-      </c>
-      <c r="K35" t="str">
+        <v>11919_aquit</v>
+      </c>
+      <c r="M35" s="18" t="str">
         <f t="shared" si="4"/>
-        <v>11919_aquit</v>
-      </c>
-      <c r="L35" t="str">
+        <v>11919</v>
+      </c>
+      <c r="N35" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>11919</v>
-      </c>
-      <c r="M35" t="b">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3000,24 +3064,24 @@
       <c r="H36" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="J36" t="str">
+      <c r="K36" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H36,"image/")</f>
+        <v>84924</v>
+      </c>
+      <c r="L36" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84924_square</v>
+      </c>
+      <c r="M36" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84924</v>
       </c>
-      <c r="K36" t="str">
-        <f t="shared" si="4"/>
-        <v>84924_square</v>
-      </c>
-      <c r="L36" t="str">
+      <c r="N36" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84924</v>
-      </c>
-      <c r="M36" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -3045,24 +3109,24 @@
       <c r="H37" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="J37" t="str">
+      <c r="K37" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H37,"image/")</f>
+        <v>84057</v>
+      </c>
+      <c r="L37" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84057_aquit</v>
+      </c>
+      <c r="M37" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84057</v>
       </c>
-      <c r="K37" t="str">
-        <f t="shared" si="4"/>
-        <v>84057_aquit</v>
-      </c>
-      <c r="L37" t="str">
+      <c r="N37" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84057</v>
-      </c>
-      <c r="M37" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
@@ -3093,24 +3157,25 @@
       <c r="I38" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="J38" t="str">
+      <c r="J38" s="17"/>
+      <c r="K38" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H38,"image/")</f>
+        <v>85065</v>
+      </c>
+      <c r="L38" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85065_square</v>
+      </c>
+      <c r="M38" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85065</v>
       </c>
-      <c r="K38" t="str">
-        <f t="shared" si="4"/>
-        <v>85065_square</v>
-      </c>
-      <c r="L38" t="str">
+      <c r="N38" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85065</v>
-      </c>
-      <c r="M38" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -3138,24 +3203,24 @@
       <c r="H39" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="J39" t="str">
+      <c r="K39" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H39,"image/")</f>
+        <v>83876</v>
+      </c>
+      <c r="L39" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>83876_aquit</v>
+      </c>
+      <c r="M39" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>83876</v>
       </c>
-      <c r="K39" t="str">
-        <f t="shared" si="4"/>
-        <v>83876_aquit</v>
-      </c>
-      <c r="L39" t="str">
+      <c r="N39" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>83876</v>
-      </c>
-      <c r="M39" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3183,24 +3248,24 @@
       <c r="H40" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="J40" t="str">
+      <c r="K40" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H40,"image/")</f>
+        <v>85073</v>
+      </c>
+      <c r="L40" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85073_square</v>
+      </c>
+      <c r="M40" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85073</v>
       </c>
-      <c r="K40" t="str">
-        <f t="shared" si="4"/>
-        <v>85073_square</v>
-      </c>
-      <c r="L40" t="str">
+      <c r="N40" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85073</v>
-      </c>
-      <c r="M40" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -3228,24 +3293,24 @@
       <c r="H41" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="J41" t="str">
+      <c r="K41" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H41,"image/")</f>
+        <v>83869</v>
+      </c>
+      <c r="L41" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>83869_aquit</v>
+      </c>
+      <c r="M41" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>83869</v>
       </c>
-      <c r="K41" t="str">
-        <f t="shared" si="4"/>
-        <v>83869_aquit</v>
-      </c>
-      <c r="L41" t="str">
+      <c r="N41" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>83869</v>
-      </c>
-      <c r="M41" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3273,24 +3338,24 @@
       <c r="H42" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="J42" t="str">
+      <c r="K42" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H42,"image/")</f>
+        <v>84946</v>
+      </c>
+      <c r="L42" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84946_square</v>
+      </c>
+      <c r="M42" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84946</v>
       </c>
-      <c r="K42" t="str">
-        <f t="shared" si="4"/>
-        <v>84946_square</v>
-      </c>
-      <c r="L42" t="str">
+      <c r="N42" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84946</v>
-      </c>
-      <c r="M42" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -3318,24 +3383,24 @@
       <c r="H43" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="J43" t="str">
+      <c r="K43" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H43,"image/")</f>
+        <v>84570</v>
+      </c>
+      <c r="L43" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84570_aquit</v>
+      </c>
+      <c r="M43" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84570</v>
       </c>
-      <c r="K43" t="str">
-        <f t="shared" si="4"/>
-        <v>84570_aquit</v>
-      </c>
-      <c r="L43" t="str">
+      <c r="N43" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84570</v>
-      </c>
-      <c r="M43" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3363,24 +3428,24 @@
       <c r="H44" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="J44" t="str">
+      <c r="K44" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H44,"image/")</f>
+        <v>85037</v>
+      </c>
+      <c r="L44" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85037_square</v>
+      </c>
+      <c r="M44" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85037</v>
       </c>
-      <c r="K44" t="str">
-        <f t="shared" si="4"/>
-        <v>85037_square</v>
-      </c>
-      <c r="L44" t="str">
+      <c r="N44" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85037</v>
-      </c>
-      <c r="M44" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3408,24 +3473,24 @@
       <c r="H45" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="J45" t="str">
+      <c r="K45" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H45,"image/")</f>
+        <v>85014</v>
+      </c>
+      <c r="L45" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85014_aquit</v>
+      </c>
+      <c r="M45" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85014</v>
       </c>
-      <c r="K45" t="str">
-        <f t="shared" si="4"/>
-        <v>85014_aquit</v>
-      </c>
-      <c r="L45" t="str">
+      <c r="N45" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85014</v>
-      </c>
-      <c r="M45" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -3453,24 +3518,24 @@
       <c r="H46" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="J46" t="str">
+      <c r="K46" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H46,"image/")</f>
+        <v>71059</v>
+      </c>
+      <c r="L46" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71059_square</v>
+      </c>
+      <c r="M46" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71059</v>
       </c>
-      <c r="K46" t="str">
-        <f t="shared" si="4"/>
-        <v>71059_square</v>
-      </c>
-      <c r="L46" t="str">
+      <c r="N46" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71059</v>
-      </c>
-      <c r="M46" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -3498,24 +3563,24 @@
       <c r="H47" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="J47" t="str">
+      <c r="K47" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H47,"image/")</f>
+        <v>85026</v>
+      </c>
+      <c r="L47" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85026_aquit</v>
+      </c>
+      <c r="M47" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85026</v>
       </c>
-      <c r="K47" t="str">
-        <f t="shared" si="4"/>
-        <v>85026_aquit</v>
-      </c>
-      <c r="L47" t="str">
+      <c r="N47" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85026</v>
-      </c>
-      <c r="M47" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -3546,24 +3611,24 @@
       <c r="I48" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J48" t="str">
+      <c r="K48" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H48,"image/")</f>
+        <v>71210</v>
+      </c>
+      <c r="L48" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71210_square</v>
+      </c>
+      <c r="M48" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71210</v>
       </c>
-      <c r="K48" t="str">
-        <f t="shared" si="4"/>
-        <v>71210_square</v>
-      </c>
-      <c r="L48" t="str">
+      <c r="N48" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71210</v>
-      </c>
-      <c r="M48" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -3591,24 +3656,24 @@
       <c r="H49" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="J49" t="str">
+      <c r="K49" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H49,"image/")</f>
+        <v>85972</v>
+      </c>
+      <c r="L49" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85972_square</v>
+      </c>
+      <c r="M49" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85972</v>
       </c>
-      <c r="K49" t="str">
-        <f t="shared" si="4"/>
-        <v>85972_square</v>
-      </c>
-      <c r="L49" t="str">
+      <c r="N49" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85972</v>
-      </c>
-      <c r="M49" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -3636,24 +3701,24 @@
       <c r="H50" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="J50" t="str">
+      <c r="K50" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H50,"image/")</f>
+        <v>86078</v>
+      </c>
+      <c r="L50" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>86078_square</v>
+      </c>
+      <c r="M50" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>86078</v>
       </c>
-      <c r="K50" t="str">
-        <f t="shared" si="4"/>
-        <v>86078_square</v>
-      </c>
-      <c r="L50" t="str">
+      <c r="N50" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>86078</v>
-      </c>
-      <c r="M50" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -3681,24 +3746,24 @@
       <c r="H51" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="J51" t="str">
+      <c r="K51" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H51,"image/")</f>
+        <v>85023</v>
+      </c>
+      <c r="L51" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85023_square</v>
+      </c>
+      <c r="M51" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85023</v>
       </c>
-      <c r="K51" t="str">
-        <f t="shared" si="4"/>
-        <v>85023_square</v>
-      </c>
-      <c r="L51" t="str">
+      <c r="N51" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85023</v>
-      </c>
-      <c r="M51" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -3726,24 +3791,24 @@
       <c r="H52" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="J52" t="str">
+      <c r="K52" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H52,"image/")</f>
+        <v>80113</v>
+      </c>
+      <c r="L52" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>80113_aquit</v>
+      </c>
+      <c r="M52" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>80113</v>
       </c>
-      <c r="K52" t="str">
-        <f t="shared" si="4"/>
-        <v>80113_aquit</v>
-      </c>
-      <c r="L52" t="str">
+      <c r="N52" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>80113</v>
-      </c>
-      <c r="M52" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -3771,24 +3836,24 @@
       <c r="H53" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="J53" t="str">
+      <c r="K53" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H53,"image/")</f>
+        <v>71112</v>
+      </c>
+      <c r="L53" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71112_square</v>
+      </c>
+      <c r="M53" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71112</v>
       </c>
-      <c r="K53" t="str">
-        <f t="shared" si="4"/>
-        <v>71112_square</v>
-      </c>
-      <c r="L53" t="str">
+      <c r="N53" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71112</v>
-      </c>
-      <c r="M53" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -3816,24 +3881,24 @@
       <c r="H54" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="J54" t="str">
+      <c r="K54" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H54,"image/")</f>
+        <v>80209</v>
+      </c>
+      <c r="L54" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>80209_aquit</v>
+      </c>
+      <c r="M54" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>80209</v>
       </c>
-      <c r="K54" t="str">
-        <f t="shared" si="4"/>
-        <v>80209_aquit</v>
-      </c>
-      <c r="L54" t="str">
+      <c r="N54" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>80209</v>
-      </c>
-      <c r="M54" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -3864,24 +3929,24 @@
       <c r="I55" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J55" t="str">
+      <c r="K55" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H55,"image/")</f>
+        <v>71032</v>
+      </c>
+      <c r="L55" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71032_square</v>
+      </c>
+      <c r="M55" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71032</v>
       </c>
-      <c r="K55" t="str">
-        <f t="shared" si="4"/>
-        <v>71032_square</v>
-      </c>
-      <c r="L55" t="str">
+      <c r="N55" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71032</v>
-      </c>
-      <c r="M55" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -3909,24 +3974,24 @@
       <c r="H56" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="J56" t="str">
+      <c r="K56" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H56,"image/")</f>
         <v>80148; https://pemdatabase.eu/image/80149</v>
       </c>
-      <c r="K56" t="str">
+      <c r="L56" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>80148-80149_aquit</v>
+      </c>
+      <c r="M56" s="18" t="str">
         <f t="shared" si="4"/>
-        <v>80148-80149_aquit</v>
-      </c>
-      <c r="L56" t="str">
+        <v>80148-80149</v>
+      </c>
+      <c r="N56" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>80148-80149</v>
-      </c>
-      <c r="M56" t="b">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -3954,24 +4019,24 @@
       <c r="H57" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="J57" t="str">
+      <c r="K57" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H57,"image/")</f>
+        <v>71205</v>
+      </c>
+      <c r="L57" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71205_square</v>
+      </c>
+      <c r="M57" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71205</v>
       </c>
-      <c r="K57" t="str">
-        <f t="shared" si="4"/>
-        <v>71205_square</v>
-      </c>
-      <c r="L57" t="str">
+      <c r="N57" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71205</v>
-      </c>
-      <c r="M57" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -3999,24 +4064,24 @@
       <c r="H58" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="J58" t="str">
+      <c r="K58" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H58,"image/")</f>
+        <v>86046</v>
+      </c>
+      <c r="L58" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>86046_aquit</v>
+      </c>
+      <c r="M58" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>86046</v>
       </c>
-      <c r="K58" t="str">
-        <f t="shared" si="4"/>
-        <v>86046_aquit</v>
-      </c>
-      <c r="L58" t="str">
+      <c r="N58" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>86046</v>
-      </c>
-      <c r="M58" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -4044,24 +4109,24 @@
       <c r="H59" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="J59" t="str">
+      <c r="K59" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H59,"image/")</f>
+        <v>85997</v>
+      </c>
+      <c r="L59" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85997_square</v>
+      </c>
+      <c r="M59" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85997</v>
       </c>
-      <c r="K59" t="str">
-        <f t="shared" si="4"/>
-        <v>85997_square</v>
-      </c>
-      <c r="L59" t="str">
+      <c r="N59" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85997</v>
-      </c>
-      <c r="M59" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -4089,24 +4154,24 @@
       <c r="H60" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="J60" t="str">
+      <c r="K60" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H60,"image/")</f>
+        <v>80028</v>
+      </c>
+      <c r="L60" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>80028_aquit</v>
+      </c>
+      <c r="M60" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>80028</v>
       </c>
-      <c r="K60" t="str">
-        <f t="shared" si="4"/>
-        <v>80028_aquit</v>
-      </c>
-      <c r="L60" t="str">
+      <c r="N60" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>80028</v>
-      </c>
-      <c r="M60" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -4137,24 +4202,24 @@
       <c r="I61" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="J61" t="str">
+      <c r="K61" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H61,"image/")</f>
+        <v>71128</v>
+      </c>
+      <c r="L61" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>71128_square</v>
+      </c>
+      <c r="M61" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>71128</v>
       </c>
-      <c r="K61" t="str">
-        <f t="shared" si="4"/>
-        <v>71128_square</v>
-      </c>
-      <c r="L61" t="str">
+      <c r="N61" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>71128</v>
-      </c>
-      <c r="M61" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -4182,24 +4247,24 @@
       <c r="H62" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J62" t="str">
+      <c r="K62" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H62,"image/")</f>
+        <v>85921</v>
+      </c>
+      <c r="L62" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85921_square</v>
+      </c>
+      <c r="M62" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85921</v>
       </c>
-      <c r="K62" t="str">
-        <f t="shared" si="4"/>
-        <v>85921_square</v>
-      </c>
-      <c r="L62" t="str">
+      <c r="N62" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85921</v>
-      </c>
-      <c r="M62" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -4227,24 +4292,24 @@
       <c r="H63" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="J63" t="str">
+      <c r="K63" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H63,"image/")</f>
+        <v>86009</v>
+      </c>
+      <c r="L63" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>86009_square</v>
+      </c>
+      <c r="M63" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>86009</v>
       </c>
-      <c r="K63" t="str">
-        <f t="shared" si="4"/>
-        <v>86009_square</v>
-      </c>
-      <c r="L63" t="str">
+      <c r="N63" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>86009</v>
-      </c>
-      <c r="M63" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -4272,24 +4337,24 @@
       <c r="H64" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="J64" t="str">
+      <c r="K64" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H64,"image/")</f>
+        <v>84967</v>
+      </c>
+      <c r="L64" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84967_square</v>
+      </c>
+      <c r="M64" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84967</v>
       </c>
-      <c r="K64" t="str">
-        <f t="shared" si="4"/>
-        <v>84967_square</v>
-      </c>
-      <c r="L64" t="str">
+      <c r="N64" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84967</v>
-      </c>
-      <c r="M64" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -4317,24 +4382,24 @@
       <c r="H65" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J65" t="str">
+      <c r="K65" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H65,"image/")</f>
+        <v>84633</v>
+      </c>
+      <c r="L65" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>84633_aquit</v>
+      </c>
+      <c r="M65" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>84633</v>
       </c>
-      <c r="K65" t="str">
-        <f t="shared" si="4"/>
-        <v>84633_aquit</v>
-      </c>
-      <c r="L65" t="str">
+      <c r="N65" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>84633</v>
-      </c>
-      <c r="M65" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -4365,24 +4430,24 @@
       <c r="I66" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J66" t="str">
+      <c r="K66" s="18" t="str">
+        <f>_xlfn.TEXTAFTER(H66,"image/")</f>
+        <v>85642</v>
+      </c>
+      <c r="L66" s="18" t="str">
         <f t="shared" si="3"/>
+        <v>85642_square</v>
+      </c>
+      <c r="M66" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>85642</v>
       </c>
-      <c r="K66" t="str">
-        <f t="shared" si="4"/>
-        <v>85642_square</v>
-      </c>
-      <c r="L66" t="str">
+      <c r="N66" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>85642</v>
-      </c>
-      <c r="M66" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -4396,38 +4461,38 @@
         <v>206</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E103" si="7">RIGHT(B67, 6)</f>
+        <f t="shared" ref="E67:E103" si="6">RIGHT(B67, 6)</f>
         <v>square</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F103" si="8">IF(E67="square","-notation square","")</f>
+        <f t="shared" ref="F67:F103" si="7">IF(E67="square","-notation square","")</f>
         <v>-notation square</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G103" si="9">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
+        <f t="shared" ref="G67:G103" si="8">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
       <c r="H67" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="J67" t="str">
-        <f t="shared" ref="J67:J103" si="10">_xlfn.TEXTAFTER(H67,"image/")</f>
+      <c r="K67" s="18" t="str">
+        <f t="shared" ref="K67:K103" si="9">_xlfn.TEXTAFTER(H67,"image/")</f>
         <v>71108</v>
       </c>
-      <c r="K67" t="str">
-        <f t="shared" ref="K67:K103" si="11">_xlfn.TEXTAFTER(B67,"pem")</f>
+      <c r="L67" s="18" t="str">
+        <f t="shared" ref="L67:L103" si="10">_xlfn.TEXTAFTER(B67,"pem")</f>
         <v>71108_square</v>
       </c>
-      <c r="L67" t="str">
-        <f t="shared" ref="L67:L103" si="12">_xlfn.TEXTBEFORE(K67,"_")</f>
+      <c r="M67" s="18" t="str">
+        <f t="shared" ref="M67:M103" si="11">_xlfn.TEXTBEFORE(L67,"_")</f>
         <v>71108</v>
       </c>
-      <c r="M67" t="b">
-        <f t="shared" ref="M67:M103" si="13">IF(J67=L67, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N67" s="20" t="b">
+        <f t="shared" ref="N67:N103" si="12">IF(K67=M67, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -4441,38 +4506,38 @@
         <v>207</v>
       </c>
       <c r="E68" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F68" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F68" t="str">
+        <v/>
+      </c>
+      <c r="G68" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G68" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
       <c r="H68" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J68" t="str">
+      <c r="K68" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L68" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M68" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K68" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L68" t="str">
+      <c r="N68" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M68" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -4486,38 +4551,38 @@
         <v>207</v>
       </c>
       <c r="E69" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F69" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F69" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G69" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G69" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
       <c r="H69" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J69" t="str">
+      <c r="K69" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L69" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M69" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K69" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L69" t="str">
+      <c r="N69" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M69" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -4531,38 +4596,38 @@
         <v>207</v>
       </c>
       <c r="E70" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F70" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F70" t="str">
+        <v/>
+      </c>
+      <c r="G70" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G70" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
       <c r="H70" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J70" t="str">
+      <c r="K70" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L70" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M70" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K70" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L70" t="str">
+      <c r="N70" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M70" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -4576,38 +4641,38 @@
         <v>207</v>
       </c>
       <c r="E71" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F71" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F71" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G71" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G71" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J71" t="str">
+      <c r="K71" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L71" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M71" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K71" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L71" t="str">
+      <c r="N71" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M71" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -4621,38 +4686,38 @@
         <v>207</v>
       </c>
       <c r="E72" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F72" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F72" t="str">
+        <v/>
+      </c>
+      <c r="G72" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G72" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
       <c r="H72" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J72" t="str">
+      <c r="K72" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L72" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M72" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K72" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L72" t="str">
+      <c r="N72" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M72" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -4666,38 +4731,38 @@
         <v>207</v>
       </c>
       <c r="E73" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F73" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F73" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G73" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G73" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J73" t="str">
+      <c r="K73" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L73" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M73" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K73" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L73" t="str">
+      <c r="N73" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M73" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -4711,38 +4776,38 @@
         <v>207</v>
       </c>
       <c r="E74" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F74" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F74" t="str">
+        <v/>
+      </c>
+      <c r="G74" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G74" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
       <c r="H74" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J74" t="str">
+      <c r="K74" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L74" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M74" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K74" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L74" t="str">
+      <c r="N74" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M74" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -4756,15 +4821,15 @@
         <v>207</v>
       </c>
       <c r="E75" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F75" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F75" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G75" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G75" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
       <c r="H75" s="11" t="s">
@@ -4773,24 +4838,24 @@
       <c r="I75" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="J75" t="str">
+      <c r="K75" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L75" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M75" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K75" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L75" t="str">
+      <c r="N75" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M75" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -4804,38 +4869,38 @@
         <v>207</v>
       </c>
       <c r="E76" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F76" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F76" t="str">
+        <v/>
+      </c>
+      <c r="G76" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G76" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
       <c r="H76" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J76" t="str">
+      <c r="K76" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L76" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M76" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K76" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L76" t="str">
+      <c r="N76" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M76" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -4849,38 +4914,38 @@
         <v>207</v>
       </c>
       <c r="E77" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F77" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F77" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G77" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G77" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H77" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J77" t="str">
+      <c r="K77" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L77" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M77" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K77" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L77" t="str">
+      <c r="N77" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M77" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -4894,38 +4959,38 @@
         <v>207</v>
       </c>
       <c r="E78" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F78" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F78" t="str">
+        <v/>
+      </c>
+      <c r="G78" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G78" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
       <c r="H78" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J78" t="str">
+      <c r="K78" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L78" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M78" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K78" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L78" t="str">
+      <c r="N78" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M78" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -4939,38 +5004,38 @@
         <v>207</v>
       </c>
       <c r="E79" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F79" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F79" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G79" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G79" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H79" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J79" t="str">
+      <c r="K79" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L79" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M79" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K79" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L79" t="str">
+      <c r="N79" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M79" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -4984,38 +5049,38 @@
         <v>207</v>
       </c>
       <c r="E80" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F80" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F80" t="str">
+        <v/>
+      </c>
+      <c r="G80" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G80" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
       <c r="H80" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J80" t="str">
+      <c r="K80" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L80" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M80" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K80" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L80" t="str">
+      <c r="N80" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M80" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>67</v>
       </c>
@@ -5029,38 +5094,38 @@
         <v>207</v>
       </c>
       <c r="E81" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F81" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F81" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G81" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G81" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H81" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J81" t="str">
+      <c r="K81" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L81" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M81" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K81" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L81" t="str">
+      <c r="N81" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M81" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -5074,38 +5139,38 @@
         <v>207</v>
       </c>
       <c r="E82" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F82" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F82" t="str">
+        <v/>
+      </c>
+      <c r="G82" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G82" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
       <c r="H82" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J82" t="str">
+      <c r="K82" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L82" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M82" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K82" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L82" t="str">
+      <c r="N82" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M82" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>67</v>
       </c>
@@ -5119,38 +5184,38 @@
         <v>207</v>
       </c>
       <c r="E83" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F83" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F83" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G83" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G83" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
       <c r="H83" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J83" t="str">
+      <c r="K83" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L83" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M83" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K83" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L83" t="str">
+      <c r="N83" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M83" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>67</v>
       </c>
@@ -5164,38 +5229,38 @@
         <v>207</v>
       </c>
       <c r="E84" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F84" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F84" t="str">
+        <v/>
+      </c>
+      <c r="G84" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G84" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
       <c r="H84" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="J84" t="str">
+      <c r="K84" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>92154</v>
+      </c>
+      <c r="L84" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>92154_aquit</v>
+      </c>
+      <c r="M84" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>92154</v>
       </c>
-      <c r="K84" t="str">
-        <f t="shared" si="11"/>
-        <v>92154_aquit</v>
-      </c>
-      <c r="L84" t="str">
+      <c r="N84" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>92154</v>
-      </c>
-      <c r="M84" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>67</v>
       </c>
@@ -5209,38 +5274,38 @@
         <v>207</v>
       </c>
       <c r="E85" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F85" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F85" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G85" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G85" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
       <c r="H85" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="J85" t="str">
+      <c r="K85" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71010</v>
+      </c>
+      <c r="L85" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71010_square</v>
+      </c>
+      <c r="M85" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71010</v>
       </c>
-      <c r="K85" t="str">
-        <f t="shared" si="11"/>
-        <v>71010_square</v>
-      </c>
-      <c r="L85" t="str">
+      <c r="N85" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71010</v>
-      </c>
-      <c r="M85" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -5254,38 +5319,38 @@
         <v>207</v>
       </c>
       <c r="E86" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F86" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F86" t="str">
+        <v/>
+      </c>
+      <c r="G86" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G86" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
       <c r="H86" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J86" t="str">
+      <c r="K86" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L86" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M86" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K86" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L86" t="str">
+      <c r="N86" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M86" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -5299,38 +5364,38 @@
         <v>207</v>
       </c>
       <c r="E87" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F87" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F87" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G87" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G87" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
       <c r="H87" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="J87" t="str">
+      <c r="K87" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71012</v>
+      </c>
+      <c r="L87" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71012_square</v>
+      </c>
+      <c r="M87" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71012</v>
       </c>
-      <c r="K87" t="str">
-        <f t="shared" si="11"/>
-        <v>71012_square</v>
-      </c>
-      <c r="L87" t="str">
+      <c r="N87" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71012</v>
-      </c>
-      <c r="M87" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>67</v>
       </c>
@@ -5344,38 +5409,38 @@
         <v>207</v>
       </c>
       <c r="E88" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F88" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F88" t="str">
+        <v/>
+      </c>
+      <c r="G88" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G88" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
       <c r="H88" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J88" t="str">
+      <c r="K88" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L88" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M88" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K88" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L88" t="str">
+      <c r="N88" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M88" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>67</v>
       </c>
@@ -5389,38 +5454,38 @@
         <v>207</v>
       </c>
       <c r="E89" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F89" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F89" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G89" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G89" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="J89" t="str">
+      <c r="K89" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71012</v>
+      </c>
+      <c r="L89" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71012_square</v>
+      </c>
+      <c r="M89" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71012</v>
       </c>
-      <c r="K89" t="str">
-        <f t="shared" si="11"/>
-        <v>71012_square</v>
-      </c>
-      <c r="L89" t="str">
+      <c r="N89" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71012</v>
-      </c>
-      <c r="M89" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>67</v>
       </c>
@@ -5434,38 +5499,38 @@
         <v>207</v>
       </c>
       <c r="E90" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F90" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F90" t="str">
+        <v/>
+      </c>
+      <c r="G90" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G90" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
       <c r="H90" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J90" t="str">
+      <c r="K90" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L90" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M90" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K90" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L90" t="str">
+      <c r="N90" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M90" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>67</v>
       </c>
@@ -5479,38 +5544,38 @@
         <v>207</v>
       </c>
       <c r="E91" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F91" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F91" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G91" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G91" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="J91" t="str">
+      <c r="K91" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71012</v>
+      </c>
+      <c r="L91" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71012_square</v>
+      </c>
+      <c r="M91" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71012</v>
       </c>
-      <c r="K91" t="str">
-        <f t="shared" si="11"/>
-        <v>71012_square</v>
-      </c>
-      <c r="L91" t="str">
+      <c r="N91" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71012</v>
-      </c>
-      <c r="M91" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>67</v>
       </c>
@@ -5524,38 +5589,38 @@
         <v>207</v>
       </c>
       <c r="E92" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F92" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F92" t="str">
+        <v/>
+      </c>
+      <c r="G92" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G92" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
       <c r="H92" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J92" t="str">
+      <c r="K92" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L92" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M92" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K92" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L92" t="str">
+      <c r="N92" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M92" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>67</v>
       </c>
@@ -5569,38 +5634,38 @@
         <v>207</v>
       </c>
       <c r="E93" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F93" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F93" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G93" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G93" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="J93" t="str">
+      <c r="K93" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71012</v>
+      </c>
+      <c r="L93" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71012_square</v>
+      </c>
+      <c r="M93" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71012</v>
       </c>
-      <c r="K93" t="str">
-        <f t="shared" si="11"/>
-        <v>71012_square</v>
-      </c>
-      <c r="L93" t="str">
+      <c r="N93" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71012</v>
-      </c>
-      <c r="M93" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>67</v>
       </c>
@@ -5614,38 +5679,38 @@
         <v>207</v>
       </c>
       <c r="E94" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F94" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F94" t="str">
+        <v/>
+      </c>
+      <c r="G94" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G94" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
       <c r="H94" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J94" t="str">
+      <c r="K94" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L94" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M94" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K94" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L94" t="str">
+      <c r="N94" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M94" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>67</v>
       </c>
@@ -5659,38 +5724,38 @@
         <v>207</v>
       </c>
       <c r="E95" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F95" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F95" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G95" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G95" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
       <c r="H95" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J95" t="str">
+      <c r="K95" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71013</v>
+      </c>
+      <c r="L95" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71013_square</v>
+      </c>
+      <c r="M95" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71013</v>
       </c>
-      <c r="K95" t="str">
-        <f t="shared" si="11"/>
-        <v>71013_square</v>
-      </c>
-      <c r="L95" t="str">
+      <c r="N95" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71013</v>
-      </c>
-      <c r="M95" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>67</v>
       </c>
@@ -5704,38 +5769,38 @@
         <v>207</v>
       </c>
       <c r="E96" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F96" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F96" t="str">
+        <v/>
+      </c>
+      <c r="G96" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G96" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
       <c r="H96" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="J96" t="str">
+      <c r="K96" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L96" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M96" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K96" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L96" t="str">
+      <c r="N96" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M96" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>67</v>
       </c>
@@ -5749,38 +5814,38 @@
         <v>207</v>
       </c>
       <c r="E97" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F97" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F97" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G97" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G97" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
       <c r="H97" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J97" t="str">
+      <c r="K97" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71013</v>
+      </c>
+      <c r="L97" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71013_square</v>
+      </c>
+      <c r="M97" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71013</v>
       </c>
-      <c r="K97" t="str">
-        <f t="shared" si="11"/>
-        <v>71013_square</v>
-      </c>
-      <c r="L97" t="str">
+      <c r="N97" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71013</v>
-      </c>
-      <c r="M97" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>67</v>
       </c>
@@ -5794,38 +5859,38 @@
         <v>207</v>
       </c>
       <c r="E98" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F98" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F98" t="str">
+        <v/>
+      </c>
+      <c r="G98" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G98" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
       <c r="H98" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="J98" t="str">
+      <c r="K98" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L98" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M98" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K98" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L98" t="str">
+      <c r="N98" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M98" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>67</v>
       </c>
@@ -5839,38 +5904,38 @@
         <v>207</v>
       </c>
       <c r="E99" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F99" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F99" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G99" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G99" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
       <c r="H99" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J99" t="str">
+      <c r="K99" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71013</v>
+      </c>
+      <c r="L99" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71013_square</v>
+      </c>
+      <c r="M99" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71013</v>
       </c>
-      <c r="K99" t="str">
-        <f t="shared" si="11"/>
-        <v>71013_square</v>
-      </c>
-      <c r="L99" t="str">
+      <c r="N99" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71013</v>
-      </c>
-      <c r="M99" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>67</v>
       </c>
@@ -5884,38 +5949,38 @@
         <v>207</v>
       </c>
       <c r="E100" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F100" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F100" t="str">
+        <v/>
+      </c>
+      <c r="G100" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G100" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
       <c r="H100" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="J100" t="str">
+      <c r="K100" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L100" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M100" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K100" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L100" t="str">
+      <c r="N100" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M100" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>67</v>
       </c>
@@ -5929,38 +5994,38 @@
         <v>207</v>
       </c>
       <c r="E101" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F101" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F101" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G101" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G101" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
       <c r="H101" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J101" t="str">
+      <c r="K101" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71013</v>
+      </c>
+      <c r="L101" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71013_square</v>
+      </c>
+      <c r="M101" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71013</v>
       </c>
-      <c r="K101" t="str">
-        <f t="shared" si="11"/>
-        <v>71013_square</v>
-      </c>
-      <c r="L101" t="str">
+      <c r="N101" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71013</v>
-      </c>
-      <c r="M101" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>67</v>
       </c>
@@ -5974,38 +6039,38 @@
         <v>207</v>
       </c>
       <c r="E102" t="str">
+        <f t="shared" si="6"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F102" t="str">
         <f t="shared" si="7"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F102" t="str">
+        <v/>
+      </c>
+      <c r="G102" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G102" t="str">
-        <f t="shared" si="9"/>
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
       <c r="H102" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="J102" t="str">
+      <c r="K102" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>80159</v>
+      </c>
+      <c r="L102" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>80159_aquit</v>
+      </c>
+      <c r="M102" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>80159</v>
       </c>
-      <c r="K102" t="str">
-        <f t="shared" si="11"/>
-        <v>80159_aquit</v>
-      </c>
-      <c r="L102" t="str">
+      <c r="N102" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>80159</v>
-      </c>
-      <c r="M102" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>67</v>
       </c>
@@ -6019,42 +6084,50 @@
         <v>207</v>
       </c>
       <c r="E103" t="str">
+        <f t="shared" si="6"/>
+        <v>square</v>
+      </c>
+      <c r="F103" t="str">
         <f t="shared" si="7"/>
-        <v>square</v>
-      </c>
-      <c r="F103" t="str">
+        <v>-notation square</v>
+      </c>
+      <c r="G103" t="str">
         <f t="shared" si="8"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G103" t="str">
-        <f t="shared" si="9"/>
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
       <c r="H103" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J103" t="str">
+      <c r="K103" s="18" t="str">
+        <f t="shared" si="9"/>
+        <v>71013</v>
+      </c>
+      <c r="L103" s="18" t="str">
         <f t="shared" si="10"/>
+        <v>71013_square</v>
+      </c>
+      <c r="M103" s="18" t="str">
+        <f t="shared" si="11"/>
         <v>71013</v>
       </c>
-      <c r="K103" t="str">
-        <f t="shared" si="11"/>
-        <v>71013_square</v>
-      </c>
-      <c r="L103" t="str">
+      <c r="N103" s="20" t="b">
         <f t="shared" si="12"/>
-        <v>71013</v>
-      </c>
-      <c r="M103" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H104" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="N2:N103">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{DB9705ED-1102-844D-8A04-BCDD8E8E1C9A}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{D77C11A9-E4F8-DB40-9661-517579200867}"/>

</xml_diff>

<commit_message>
All filenames now match the links (see table)
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28C204-63E2-E64A-B826-37E367FDD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A2AEAA-A51D-E44E-ABAF-BA67946C64B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
@@ -684,9 +684,6 @@
   </si>
   <si>
     <t>34_deo-nostro_pem71013_square</t>
-  </si>
-  <si>
-    <t>34_qui-manducat--panem_pem11919_aquit</t>
   </si>
   <si>
     <t>accid</t>
@@ -940,6 +937,9 @@
   </si>
   <si>
     <t>Evaluation of links vs. filenames</t>
+  </si>
+  <si>
+    <t>34_qui-manducat--panem_pem119191_aquit</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1446,10 @@
   <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1491,7 @@
         <v>214</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -1523,7 +1523,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K2" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H2,"image/")</f>
@@ -1568,7 +1568,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K3" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H3,"image/")</f>
@@ -1613,7 +1613,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/03_de-fructu-operum_pem56766_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.mei </v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K4" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H4,"image/")</f>
@@ -1658,7 +1658,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/04_de-fructu-operum_pem84909_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.mei -notation square</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K5" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H5,"image/")</f>
@@ -1703,7 +1703,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/05_dicit-dominus_pem84540_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.mei </v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K6" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H6,"image/")</f>
@@ -1748,7 +1748,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/06_dicit-dominus_pem84623_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.mei </v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K7" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H7,"image/")</f>
@@ -1793,10 +1793,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K8" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H8,"image/")</f>
@@ -1841,7 +1841,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/08_ecce-virgo_pem84614_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.mei </v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K9" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H9,"image/")</f>
@@ -1886,7 +1886,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/09_ecce-virgo_pem84548_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.mei </v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K10" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H10,"image/")</f>
@@ -1931,7 +1931,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/10_ecce-virgo_pem84882_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.mei -notation square</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K11" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H11,"image/")</f>
@@ -1976,7 +1976,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/11_jerusalem-surge_pem84878_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.mei -notation square</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K12" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H12,"image/")</f>
@@ -2021,10 +2021,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K13" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H13,"image/")</f>
@@ -2069,7 +2069,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/13_factus-est-repente_pem84630_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.mei </v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K14" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H14,"image/")</f>
@@ -2114,7 +2114,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/14_factus-est-repente_pem84881_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.mei -notation square</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K15" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H15,"image/")</f>
@@ -2159,7 +2159,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K16" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H16,"image/")</f>
@@ -2204,7 +2204,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K17" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H17,"image/")</f>
@@ -2249,7 +2249,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K18" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H18,"image/")</f>
@@ -2294,7 +2294,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K19" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H19,"image/")</f>
@@ -2339,7 +2339,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K20" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H20,"image/")</f>
@@ -2384,7 +2384,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K21" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H21,"image/")</f>
@@ -2429,7 +2429,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K22" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H22,"image/")</f>
@@ -2474,7 +2474,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K23" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H23,"image/")</f>
@@ -2519,7 +2519,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K24" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H24,"image/")</f>
@@ -2564,7 +2564,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K25" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H25,"image/")</f>
@@ -2609,7 +2609,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K26" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H26,"image/")</f>
@@ -2654,10 +2654,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K27" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H27,"image/")</f>
@@ -2702,7 +2702,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K28" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H28,"image/")</f>
@@ -2747,7 +2747,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K29" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H29,"image/")</f>
@@ -2792,7 +2792,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K30" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H30,"image/")</f>
@@ -2837,7 +2837,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K31" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H31,"image/")</f>
@@ -2882,7 +2882,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K32" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H32,"image/")</f>
@@ -2927,7 +2927,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K33" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H33,"image/")</f>
@@ -2972,7 +2972,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K34" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H34,"image/")</f>
@@ -2996,7 +2996,7 @@
         <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>216</v>
+        <v>291</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>136</v>
@@ -3014,10 +3014,10 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/34_qui-manducat--panem_pem11919_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem11919_aquit.mei </v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/34_qui-manducat--panem_pem119191_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.mei </v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K35" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H35,"image/")</f>
@@ -3025,15 +3025,15 @@
       </c>
       <c r="L35" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>11919_aquit</v>
+        <v>119191_aquit</v>
       </c>
       <c r="M35" s="18" t="str">
         <f t="shared" si="4"/>
-        <v>11919</v>
+        <v>119191</v>
       </c>
       <c r="N35" s="20" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3062,7 +3062,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K36" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H36,"image/")</f>
@@ -3107,7 +3107,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K37" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H37,"image/")</f>
@@ -3152,10 +3152,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="18" t="str">
@@ -3201,7 +3201,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K39" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H39,"image/")</f>
@@ -3246,7 +3246,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K40" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H40,"image/")</f>
@@ -3291,7 +3291,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K41" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H41,"image/")</f>
@@ -3336,7 +3336,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K42" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H42,"image/")</f>
@@ -3381,7 +3381,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K43" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H43,"image/")</f>
@@ -3426,7 +3426,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K44" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H44,"image/")</f>
@@ -3471,7 +3471,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K45" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H45,"image/")</f>
@@ -3516,7 +3516,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K46" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H46,"image/")</f>
@@ -3561,7 +3561,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K47" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H47,"image/")</f>
@@ -3606,10 +3606,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K48" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H48,"image/")</f>
@@ -3654,7 +3654,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/05_o-crux_pem85972_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.mei -notation square</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K49" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H49,"image/")</f>
@@ -3699,7 +3699,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/06_o-crux_pem86078_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.mei -notation square</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K50" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H50,"image/")</f>
@@ -3744,7 +3744,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/07_o-crux_pem85023_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.mei -notation square</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K51" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H51,"image/")</f>
@@ -3789,7 +3789,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/08_ihesum_pem80113_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.mei </v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K52" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H52,"image/")</f>
@@ -3834,7 +3834,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/09_ihesum_pem71112_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.mei -notation square</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K53" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H53,"image/")</f>
@@ -3879,7 +3879,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/10_tunc-invocabis_pem80209_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.mei </v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K54" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H54,"image/")</f>
@@ -3924,10 +3924,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K55" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H55,"image/")</f>
@@ -3972,7 +3972,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/12_si-offers_pem80148-80149_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.mei </v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K56" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H56,"image/")</f>
@@ -4017,7 +4017,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/13_si-offers_pem71205_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.mei -notation square</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K57" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H57,"image/")</f>
@@ -4062,7 +4062,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/14_isti-sunt_pem86046_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.mei </v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K58" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H58,"image/")</f>
@@ -4107,7 +4107,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/15_isti-sunt_pem85997_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.mei -notation square</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K59" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H59,"image/")</f>
@@ -4152,7 +4152,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/16_mercennarius_pem80028_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.mei </v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K60" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H60,"image/")</f>
@@ -4197,10 +4197,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K61" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H61,"image/")</f>
@@ -4245,7 +4245,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/18_o-lux_pem85921_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.mei -notation square</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K62" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H62,"image/")</f>
@@ -4290,7 +4290,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/19_o-lux_pem86009_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.mei -notation square</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K63" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H63,"image/")</f>
@@ -4335,7 +4335,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/20_o-lux_pem84967_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.mei -notation square</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K64" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H64,"image/")</f>
@@ -4380,7 +4380,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/21_vespere_pem84633_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.mei </v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K65" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H65,"image/")</f>
@@ -4425,10 +4425,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K66" s="18" t="str">
         <f>_xlfn.TEXTAFTER(H66,"image/")</f>
@@ -4473,7 +4473,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K67" s="18" t="str">
         <f t="shared" ref="K67:K103" si="9">_xlfn.TEXTAFTER(H67,"image/")</f>
@@ -4518,7 +4518,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K68" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4563,7 +4563,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K69" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4608,7 +4608,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K70" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4653,7 +4653,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K71" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4698,7 +4698,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K72" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4743,7 +4743,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K73" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4788,7 +4788,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K74" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4833,10 +4833,10 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K75" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4881,7 +4881,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K76" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4926,7 +4926,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K77" s="18" t="str">
         <f t="shared" si="9"/>
@@ -4971,7 +4971,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K78" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5016,7 +5016,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K79" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5061,7 +5061,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K80" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5106,7 +5106,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K81" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5151,7 +5151,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K82" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5196,7 +5196,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K83" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5241,7 +5241,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K84" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5286,7 +5286,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K85" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5331,7 +5331,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K86" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5376,7 +5376,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K87" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5421,7 +5421,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K88" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5466,7 +5466,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K89" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5511,7 +5511,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K90" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5556,7 +5556,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K91" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5601,7 +5601,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K92" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5646,7 +5646,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K93" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5691,7 +5691,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K94" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5736,7 +5736,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K95" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5781,7 +5781,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
       <c r="H96" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K96" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5826,7 +5826,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K97" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5871,7 +5871,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
       <c r="H98" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K98" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5916,7 +5916,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K99" s="18" t="str">
         <f t="shared" si="9"/>
@@ -5961,7 +5961,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K100" s="18" t="str">
         <f t="shared" si="9"/>
@@ -6006,7 +6006,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K101" s="18" t="str">
         <f t="shared" si="9"/>
@@ -6051,7 +6051,7 @@
         <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K102" s="18" t="str">
         <f t="shared" si="9"/>
@@ -6096,7 +6096,7 @@
         <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K103" s="18" t="str">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
Change file names and fix the name of Pieces 01 and 02
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marthae.thomae/Downloads/temp/GABCtoMEI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A2AEAA-A51D-E44E-ABAF-BA67946C64B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E60CCAC-0D0E-2C42-B9C8-3DC16BFF4262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="740" windowWidth="28740" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="2920" yWindow="6060" windowWidth="48280" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1074,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1094,35 +1094,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1446,10 +1433,10 @@
   <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N35" sqref="N35"/>
+      <selection pane="bottomRight" activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,11 +1448,11 @@
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="214" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="21"/>
+    <col min="14" max="14" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1490,12 +1477,12 @@
       <c r="G1" t="s">
         <v>214</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1519,25 +1506,25 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A2,"/",B2,".gabc MEI_outfiles/", A2, "/", C2, "_", D2, B2, ".mei ",F2)</f>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
-      </c>
-      <c r="H2" s="14" t="s">
+        <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A2,"/",C2,"_",D2,B2,".gabc MEI_outfiles/", A2, "/", C2, "_", D2, B2, ".mei ",F2)</f>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H2,"image/")</f>
+      <c r="K2" s="15" t="str">
+        <f t="shared" ref="K2:K33" si="0">_xlfn.TEXTAFTER(H2,"image/")</f>
         <v>82441</v>
       </c>
-      <c r="L2" s="18" t="str">
+      <c r="L2" s="15" t="str">
         <f>_xlfn.TEXTAFTER(B2,"pem")</f>
         <v>82441_aquit</v>
       </c>
-      <c r="M2" s="18" t="str">
+      <c r="M2" s="15" t="str">
         <f>_xlfn.TEXTBEFORE(L2,"_")</f>
         <v>82441</v>
       </c>
-      <c r="N2" s="20" t="b">
+      <c r="N2" s="16" t="b">
         <f>IF(K2=M2, TRUE, FALSE)</f>
         <v>1</v>
       </c>
@@ -1556,33 +1543,33 @@
         <v>205</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">RIGHT(B3, 6)</f>
+        <f t="shared" ref="E3:E66" si="1">RIGHT(B3, 6)</f>
         <v>square</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="1">IF(E3="square","-notation square","")</f>
+        <f t="shared" ref="F3:F66" si="2">IF(E3="square","-notation square","")</f>
         <v>-notation square</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" si="2">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A3,"/",B3,".gabc MEI_outfiles/", A3, "/", C3, "_", D3, B3, ".mei ",F3)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
-      </c>
-      <c r="H3" s="14" t="s">
+        <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A3,"/",C3,"_",D3,B3,".gabc MEI_outfiles/", A3, "/", C3, "_", D3, B3, ".mei ",F3)</f>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="K3" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H3,"image/")</f>
+      <c r="K3" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>85041</v>
       </c>
-      <c r="L3" s="18" t="str">
+      <c r="L3" s="15" t="str">
         <f t="shared" ref="L3:L66" si="3">_xlfn.TEXTAFTER(B3,"pem")</f>
         <v>85041_square</v>
       </c>
-      <c r="M3" s="18" t="str">
+      <c r="M3" s="15" t="str">
         <f t="shared" ref="M3:M66" si="4">_xlfn.TEXTBEFORE(L3,"_")</f>
         <v>85041</v>
       </c>
-      <c r="N3" s="20" t="b">
+      <c r="N3" s="16" t="b">
         <f t="shared" ref="N3:N66" si="5">IF(K3=M3, TRUE, FALSE)</f>
         <v>1</v>
       </c>
@@ -1601,33 +1588,33 @@
         <v>205</v>
       </c>
       <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G67" si="6">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A4,"/",C4,"_",D4,B4,".gabc MEI_outfiles/", A4, "/", C4, "_", D4, B4, ".mei ",F4)</f>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.mei </v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/03_de-fructu-operum_pem56766_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.mei </v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="K4" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H4,"image/")</f>
         <v>56766</v>
       </c>
-      <c r="L4" s="18" t="str">
+      <c r="L4" s="15" t="str">
         <f t="shared" si="3"/>
         <v>56766_aquit</v>
       </c>
-      <c r="M4" s="18" t="str">
+      <c r="M4" s="15" t="str">
         <f t="shared" si="4"/>
         <v>56766</v>
       </c>
-      <c r="N4" s="20" t="b">
+      <c r="N4" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1646,33 +1633,33 @@
         <v>205</v>
       </c>
       <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>square</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>-notation square</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.mei -notation square</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="K5" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>square</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="1"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/04_de-fructu-operum_pem84909_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.mei -notation square</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="K5" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H5,"image/")</f>
         <v>84909</v>
       </c>
-      <c r="L5" s="18" t="str">
+      <c r="L5" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84909_square</v>
       </c>
-      <c r="M5" s="18" t="str">
+      <c r="M5" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84909</v>
       </c>
-      <c r="N5" s="20" t="b">
+      <c r="N5" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1691,33 +1678,33 @@
         <v>205</v>
       </c>
       <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.mei </v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/05_dicit-dominus_pem84540_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.mei </v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="K6" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H6,"image/")</f>
         <v>84540</v>
       </c>
-      <c r="L6" s="18" t="str">
+      <c r="L6" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84540_aquit</v>
       </c>
-      <c r="M6" s="18" t="str">
+      <c r="M6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84540</v>
       </c>
-      <c r="N6" s="20" t="b">
+      <c r="N6" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1736,33 +1723,33 @@
         <v>205</v>
       </c>
       <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.mei </v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="K7" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/06_dicit-dominus_pem84623_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.mei </v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="K7" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H7,"image/")</f>
         <v>84623</v>
       </c>
-      <c r="L7" s="18" t="str">
+      <c r="L7" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84623_aquit</v>
       </c>
-      <c r="M7" s="18" t="str">
+      <c r="M7" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84623</v>
       </c>
-      <c r="N7" s="20" t="b">
+      <c r="N7" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1781,36 +1768,36 @@
         <v>205</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
-      </c>
-      <c r="H8" s="15" t="s">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>225</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="K8" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H8,"image/")</f>
+      <c r="K8" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84873</v>
       </c>
-      <c r="L8" s="18" t="str">
+      <c r="L8" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84873_square</v>
       </c>
-      <c r="M8" s="18" t="str">
+      <c r="M8" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84873</v>
       </c>
-      <c r="N8" s="20" t="b">
+      <c r="N8" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1829,33 +1816,33 @@
         <v>205</v>
       </c>
       <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.mei </v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="K9" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/08_ecce-virgo_pem84614_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.mei </v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="K9" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H9,"image/")</f>
         <v>84614</v>
       </c>
-      <c r="L9" s="18" t="str">
+      <c r="L9" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84614_aquit</v>
       </c>
-      <c r="M9" s="18" t="str">
+      <c r="M9" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84614</v>
       </c>
-      <c r="N9" s="20" t="b">
+      <c r="N9" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1874,33 +1861,33 @@
         <v>205</v>
       </c>
       <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.mei </v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="K10" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/09_ecce-virgo_pem84548_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.mei </v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="K10" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H10,"image/")</f>
         <v>84548</v>
       </c>
-      <c r="L10" s="18" t="str">
+      <c r="L10" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84548_aquit</v>
       </c>
-      <c r="M10" s="18" t="str">
+      <c r="M10" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84548</v>
       </c>
-      <c r="N10" s="20" t="b">
+      <c r="N10" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1919,33 +1906,33 @@
         <v>205</v>
       </c>
       <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>square</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>-notation square</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.mei -notation square</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="K11" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>square</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/10_ecce-virgo_pem84882_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.mei -notation square</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="K11" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H11,"image/")</f>
         <v>84882</v>
       </c>
-      <c r="L11" s="18" t="str">
+      <c r="L11" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84882_square</v>
       </c>
-      <c r="M11" s="18" t="str">
+      <c r="M11" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84882</v>
       </c>
-      <c r="N11" s="20" t="b">
+      <c r="N11" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1964,33 +1951,33 @@
         <v>205</v>
       </c>
       <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>square</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>-notation square</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.mei -notation square</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>square</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/11_jerusalem-surge_pem84878_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.mei -notation square</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="K12" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H12,"image/")</f>
         <v>84878</v>
       </c>
-      <c r="L12" s="18" t="str">
+      <c r="L12" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84878_square</v>
       </c>
-      <c r="M12" s="18" t="str">
+      <c r="M12" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84878</v>
       </c>
-      <c r="N12" s="20" t="b">
+      <c r="N12" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2009,36 +1996,36 @@
         <v>205</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
-      </c>
-      <c r="H13" s="15" t="s">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>230</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K13" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H13,"image/")</f>
+      <c r="K13" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>86239</v>
       </c>
-      <c r="L13" s="18" t="str">
+      <c r="L13" s="15" t="str">
         <f t="shared" si="3"/>
         <v>86239_square</v>
       </c>
-      <c r="M13" s="18" t="str">
+      <c r="M13" s="15" t="str">
         <f t="shared" si="4"/>
         <v>86239</v>
       </c>
-      <c r="N13" s="20" t="b">
+      <c r="N13" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2057,33 +2044,33 @@
         <v>205</v>
       </c>
       <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.mei </v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="K14" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/13_factus-est-repente_pem84630_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.mei </v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="K14" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H14,"image/")</f>
         <v>84630</v>
       </c>
-      <c r="L14" s="18" t="str">
+      <c r="L14" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84630_aquit</v>
       </c>
-      <c r="M14" s="18" t="str">
+      <c r="M14" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84630</v>
       </c>
-      <c r="N14" s="20" t="b">
+      <c r="N14" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2102,33 +2089,33 @@
         <v>205</v>
       </c>
       <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>square</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>-notation square</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.mei -notation square</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="K15" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>square</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>-notation square</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/14_factus-est-repente_pem84881_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.mei -notation square</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="K15" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H15,"image/")</f>
         <v>84881</v>
       </c>
-      <c r="L15" s="18" t="str">
+      <c r="L15" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84881_square</v>
       </c>
-      <c r="M15" s="18" t="str">
+      <c r="M15" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84881</v>
       </c>
-      <c r="N15" s="20" t="b">
+      <c r="N15" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2147,33 +2134,33 @@
         <v>205</v>
       </c>
       <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="K16" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="K16" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H16,"image/")</f>
         <v>84534</v>
       </c>
-      <c r="L16" s="18" t="str">
+      <c r="L16" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84534_aquit</v>
       </c>
-      <c r="M16" s="18" t="str">
+      <c r="M16" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84534</v>
       </c>
-      <c r="N16" s="20" t="b">
+      <c r="N16" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2192,33 +2179,33 @@
         <v>205</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="K17" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H17,"image/")</f>
+      <c r="K17" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84863</v>
       </c>
-      <c r="L17" s="18" t="str">
+      <c r="L17" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84863_square</v>
       </c>
-      <c r="M17" s="18" t="str">
+      <c r="M17" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84863</v>
       </c>
-      <c r="N17" s="20" t="b">
+      <c r="N17" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2237,33 +2224,33 @@
         <v>205</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
       </c>
       <c r="H18" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="K18" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H18,"image/")</f>
+      <c r="K18" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>83892</v>
       </c>
-      <c r="L18" s="18" t="str">
+      <c r="L18" s="15" t="str">
         <f t="shared" si="3"/>
         <v>83892_aquit</v>
       </c>
-      <c r="M18" s="18" t="str">
+      <c r="M18" s="15" t="str">
         <f t="shared" si="4"/>
         <v>83892</v>
       </c>
-      <c r="N18" s="20" t="b">
+      <c r="N18" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2282,33 +2269,33 @@
         <v>205</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="K19" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H19,"image/")</f>
+      <c r="K19" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>85059</v>
       </c>
-      <c r="L19" s="18" t="str">
+      <c r="L19" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85059_square</v>
       </c>
-      <c r="M19" s="18" t="str">
+      <c r="M19" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85059</v>
       </c>
-      <c r="N19" s="20" t="b">
+      <c r="N19" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2327,33 +2314,33 @@
         <v>205</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
       </c>
       <c r="H20" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="K20" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H20,"image/")</f>
+      <c r="K20" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84600</v>
       </c>
-      <c r="L20" s="18" t="str">
+      <c r="L20" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84600_aquit</v>
       </c>
-      <c r="M20" s="18" t="str">
+      <c r="M20" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84600</v>
       </c>
-      <c r="N20" s="20" t="b">
+      <c r="N20" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2372,33 +2359,33 @@
         <v>205</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
       </c>
       <c r="H21" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="K21" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H21,"image/")</f>
+      <c r="K21" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>83880</v>
       </c>
-      <c r="L21" s="18" t="str">
+      <c r="L21" s="15" t="str">
         <f t="shared" si="3"/>
         <v>83880_aquit</v>
       </c>
-      <c r="M21" s="18" t="str">
+      <c r="M21" s="15" t="str">
         <f t="shared" si="4"/>
         <v>83880</v>
       </c>
-      <c r="N21" s="20" t="b">
+      <c r="N21" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2417,33 +2404,33 @@
         <v>205</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="K22" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H22,"image/")</f>
+      <c r="K22" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84880</v>
       </c>
-      <c r="L22" s="18" t="str">
+      <c r="L22" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84880_square</v>
       </c>
-      <c r="M22" s="18" t="str">
+      <c r="M22" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84880</v>
       </c>
-      <c r="N22" s="20" t="b">
+      <c r="N22" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2462,33 +2449,33 @@
         <v>205</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
       </c>
       <c r="H23" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="K23" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H23,"image/")</f>
+      <c r="K23" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84580</v>
       </c>
-      <c r="L23" s="18" t="str">
+      <c r="L23" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84580_aquit</v>
       </c>
-      <c r="M23" s="18" t="str">
+      <c r="M23" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84580</v>
       </c>
-      <c r="N23" s="20" t="b">
+      <c r="N23" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2507,33 +2494,33 @@
         <v>205</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="K24" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H24,"image/")</f>
+      <c r="K24" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>85056</v>
       </c>
-      <c r="L24" s="18" t="str">
+      <c r="L24" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85056_square</v>
       </c>
-      <c r="M24" s="18" t="str">
+      <c r="M24" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85056</v>
       </c>
-      <c r="N24" s="20" t="b">
+      <c r="N24" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2552,33 +2539,33 @@
         <v>205</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
       </c>
       <c r="H25" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="K25" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H25,"image/")</f>
+      <c r="K25" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>83911</v>
       </c>
-      <c r="L25" s="18" t="str">
+      <c r="L25" s="15" t="str">
         <f t="shared" si="3"/>
         <v>83911_aquit</v>
       </c>
-      <c r="M25" s="18" t="str">
+      <c r="M25" s="15" t="str">
         <f t="shared" si="4"/>
         <v>83911</v>
       </c>
-      <c r="N25" s="20" t="b">
+      <c r="N25" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2597,33 +2584,33 @@
         <v>205</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
       </c>
       <c r="H26" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="K26" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H26,"image/")</f>
+      <c r="K26" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84665</v>
       </c>
-      <c r="L26" s="18" t="str">
+      <c r="L26" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84665_aquit</v>
       </c>
-      <c r="M26" s="18" t="str">
+      <c r="M26" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84665</v>
       </c>
-      <c r="N26" s="20" t="b">
+      <c r="N26" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2642,16 +2629,16 @@
         <v>205</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>244</v>
@@ -2659,19 +2646,19 @@
       <c r="I27" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="K27" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H27,"image/")</f>
+      <c r="K27" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84905</v>
       </c>
-      <c r="L27" s="18" t="str">
+      <c r="L27" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84905_square</v>
       </c>
-      <c r="M27" s="18" t="str">
+      <c r="M27" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84905</v>
       </c>
-      <c r="N27" s="20" t="b">
+      <c r="N27" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2690,33 +2677,33 @@
         <v>205</v>
       </c>
       <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="K28" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="K28" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H28,"image/")</f>
         <v>84532</v>
       </c>
-      <c r="L28" s="18" t="str">
+      <c r="L28" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84532_aquit</v>
       </c>
-      <c r="M28" s="18" t="str">
+      <c r="M28" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84532</v>
       </c>
-      <c r="N28" s="20" t="b">
+      <c r="N28" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2735,33 +2722,33 @@
         <v>205</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="K29" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H29,"image/")</f>
+      <c r="K29" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84919</v>
       </c>
-      <c r="L29" s="18" t="str">
+      <c r="L29" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84919_square</v>
       </c>
-      <c r="M29" s="18" t="str">
+      <c r="M29" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84919</v>
       </c>
-      <c r="N29" s="20" t="b">
+      <c r="N29" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2780,33 +2767,33 @@
         <v>205</v>
       </c>
       <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>_aquit</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="K30" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>_aquit</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="K30" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H30,"image/")</f>
         <v>84595</v>
       </c>
-      <c r="L30" s="18" t="str">
+      <c r="L30" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84595_aquit</v>
       </c>
-      <c r="M30" s="18" t="str">
+      <c r="M30" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84595</v>
       </c>
-      <c r="N30" s="20" t="b">
+      <c r="N30" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2825,33 +2812,33 @@
         <v>205</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="K31" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H31,"image/")</f>
+      <c r="K31" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84872</v>
       </c>
-      <c r="L31" s="18" t="str">
+      <c r="L31" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84872_square</v>
       </c>
-      <c r="M31" s="18" t="str">
+      <c r="M31" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84872</v>
       </c>
-      <c r="N31" s="20" t="b">
+      <c r="N31" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2870,33 +2857,33 @@
         <v>205</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
       </c>
       <c r="H32" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="K32" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H32,"image/")</f>
+      <c r="K32" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84666</v>
       </c>
-      <c r="L32" s="18" t="str">
+      <c r="L32" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84666_aquit</v>
       </c>
-      <c r="M32" s="18" t="str">
+      <c r="M32" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84666</v>
       </c>
-      <c r="N32" s="20" t="b">
+      <c r="N32" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2915,33 +2902,33 @@
         <v>205</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="K33" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H33,"image/")</f>
+      <c r="K33" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>84874</v>
       </c>
-      <c r="L33" s="18" t="str">
+      <c r="L33" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84874_square</v>
       </c>
-      <c r="M33" s="18" t="str">
+      <c r="M33" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84874</v>
       </c>
-      <c r="N33" s="20" t="b">
+      <c r="N33" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2960,33 +2947,33 @@
         <v>205</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
       </c>
       <c r="H34" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="K34" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H34,"image/")</f>
+      <c r="K34" s="15" t="str">
+        <f t="shared" ref="K34:K66" si="7">_xlfn.TEXTAFTER(H34,"image/")</f>
         <v>76616</v>
       </c>
-      <c r="L34" s="18" t="str">
+      <c r="L34" s="15" t="str">
         <f t="shared" si="3"/>
         <v>76616_aquit</v>
       </c>
-      <c r="M34" s="18" t="str">
+      <c r="M34" s="15" t="str">
         <f t="shared" si="4"/>
         <v>76616</v>
       </c>
-      <c r="N34" s="20" t="b">
+      <c r="N34" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3005,33 +2992,33 @@
         <v>205</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/34_qui-manducat--panem_pem119191_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.mei </v>
       </c>
       <c r="H35" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="K35" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H35,"image/")</f>
+      <c r="K35" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>119191</v>
       </c>
-      <c r="L35" s="18" t="str">
+      <c r="L35" s="15" t="str">
         <f t="shared" si="3"/>
         <v>119191_aquit</v>
       </c>
-      <c r="M35" s="18" t="str">
+      <c r="M35" s="15" t="str">
         <f t="shared" si="4"/>
         <v>119191</v>
       </c>
-      <c r="N35" s="20" t="b">
+      <c r="N35" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3050,33 +3037,33 @@
         <v>205</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="K36" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H36,"image/")</f>
+      <c r="K36" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84924</v>
       </c>
-      <c r="L36" s="18" t="str">
+      <c r="L36" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84924_square</v>
       </c>
-      <c r="M36" s="18" t="str">
+      <c r="M36" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84924</v>
       </c>
-      <c r="N36" s="20" t="b">
+      <c r="N36" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3095,33 +3082,33 @@
         <v>205</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
       </c>
       <c r="H37" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K37" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H37,"image/")</f>
+      <c r="K37" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84057</v>
       </c>
-      <c r="L37" s="18" t="str">
+      <c r="L37" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84057_aquit</v>
       </c>
-      <c r="M37" s="18" t="str">
+      <c r="M37" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84057</v>
       </c>
-      <c r="N37" s="20" t="b">
+      <c r="N37" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3140,16 +3127,16 @@
         <v>205</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
-      <c r="G38" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
+      <c r="G38" t="str">
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>255</v>
@@ -3157,20 +3144,19 @@
       <c r="I38" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="J38" s="17"/>
-      <c r="K38" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H38,"image/")</f>
+      <c r="K38" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85065</v>
       </c>
-      <c r="L38" s="18" t="str">
+      <c r="L38" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85065_square</v>
       </c>
-      <c r="M38" s="18" t="str">
+      <c r="M38" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85065</v>
       </c>
-      <c r="N38" s="20" t="b">
+      <c r="N38" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3189,33 +3175,33 @@
         <v>205</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
       </c>
       <c r="H39" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="K39" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H39,"image/")</f>
+      <c r="K39" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>83876</v>
       </c>
-      <c r="L39" s="18" t="str">
+      <c r="L39" s="15" t="str">
         <f t="shared" si="3"/>
         <v>83876_aquit</v>
       </c>
-      <c r="M39" s="18" t="str">
+      <c r="M39" s="15" t="str">
         <f t="shared" si="4"/>
         <v>83876</v>
       </c>
-      <c r="N39" s="20" t="b">
+      <c r="N39" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3234,33 +3220,33 @@
         <v>205</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="K40" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H40,"image/")</f>
+      <c r="K40" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85073</v>
       </c>
-      <c r="L40" s="18" t="str">
+      <c r="L40" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85073_square</v>
       </c>
-      <c r="M40" s="18" t="str">
+      <c r="M40" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85073</v>
       </c>
-      <c r="N40" s="20" t="b">
+      <c r="N40" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3279,33 +3265,33 @@
         <v>205</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
       </c>
       <c r="H41" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="K41" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H41,"image/")</f>
+      <c r="K41" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>83869</v>
       </c>
-      <c r="L41" s="18" t="str">
+      <c r="L41" s="15" t="str">
         <f t="shared" si="3"/>
         <v>83869_aquit</v>
       </c>
-      <c r="M41" s="18" t="str">
+      <c r="M41" s="15" t="str">
         <f t="shared" si="4"/>
         <v>83869</v>
       </c>
-      <c r="N41" s="20" t="b">
+      <c r="N41" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3324,33 +3310,33 @@
         <v>205</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="K42" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H42,"image/")</f>
+      <c r="K42" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84946</v>
       </c>
-      <c r="L42" s="18" t="str">
+      <c r="L42" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84946_square</v>
       </c>
-      <c r="M42" s="18" t="str">
+      <c r="M42" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84946</v>
       </c>
-      <c r="N42" s="20" t="b">
+      <c r="N42" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3369,33 +3355,33 @@
         <v>205</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
       </c>
       <c r="H43" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="K43" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H43,"image/")</f>
+      <c r="K43" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84570</v>
       </c>
-      <c r="L43" s="18" t="str">
+      <c r="L43" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84570_aquit</v>
       </c>
-      <c r="M43" s="18" t="str">
+      <c r="M43" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84570</v>
       </c>
-      <c r="N43" s="20" t="b">
+      <c r="N43" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3414,33 +3400,33 @@
         <v>205</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
       </c>
       <c r="H44" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="K44" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H44,"image/")</f>
+      <c r="K44" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85037</v>
       </c>
-      <c r="L44" s="18" t="str">
+      <c r="L44" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85037_square</v>
       </c>
-      <c r="M44" s="18" t="str">
+      <c r="M44" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85037</v>
       </c>
-      <c r="N44" s="20" t="b">
+      <c r="N44" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3459,33 +3445,33 @@
         <v>206</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
       </c>
       <c r="H45" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="K45" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H45,"image/")</f>
+      <c r="K45" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85014</v>
       </c>
-      <c r="L45" s="18" t="str">
+      <c r="L45" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85014_aquit</v>
       </c>
-      <c r="M45" s="18" t="str">
+      <c r="M45" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85014</v>
       </c>
-      <c r="N45" s="20" t="b">
+      <c r="N45" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3504,33 +3490,33 @@
         <v>206</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="K46" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H46,"image/")</f>
+      <c r="K46" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71059</v>
       </c>
-      <c r="L46" s="18" t="str">
+      <c r="L46" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71059_square</v>
       </c>
-      <c r="M46" s="18" t="str">
+      <c r="M46" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71059</v>
       </c>
-      <c r="N46" s="20" t="b">
+      <c r="N46" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3549,33 +3535,33 @@
         <v>206</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
       </c>
       <c r="H47" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="K47" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H47,"image/")</f>
+      <c r="K47" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85026</v>
       </c>
-      <c r="L47" s="18" t="str">
+      <c r="L47" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85026_aquit</v>
       </c>
-      <c r="M47" s="18" t="str">
+      <c r="M47" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85026</v>
       </c>
-      <c r="N47" s="20" t="b">
+      <c r="N47" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3594,16 +3580,16 @@
         <v>206</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>265</v>
@@ -3611,19 +3597,19 @@
       <c r="I48" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K48" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H48,"image/")</f>
+      <c r="K48" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71210</v>
       </c>
-      <c r="L48" s="18" t="str">
+      <c r="L48" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71210_square</v>
       </c>
-      <c r="M48" s="18" t="str">
+      <c r="M48" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71210</v>
       </c>
-      <c r="N48" s="20" t="b">
+      <c r="N48" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3642,33 +3628,33 @@
         <v>206</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/05_o-crux_pem85972_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.mei -notation square</v>
       </c>
       <c r="H49" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="K49" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H49,"image/")</f>
+      <c r="K49" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85972</v>
       </c>
-      <c r="L49" s="18" t="str">
+      <c r="L49" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85972_square</v>
       </c>
-      <c r="M49" s="18" t="str">
+      <c r="M49" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85972</v>
       </c>
-      <c r="N49" s="20" t="b">
+      <c r="N49" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3687,33 +3673,33 @@
         <v>206</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/06_o-crux_pem86078_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.mei -notation square</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="K50" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H50,"image/")</f>
+      <c r="K50" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>86078</v>
       </c>
-      <c r="L50" s="18" t="str">
+      <c r="L50" s="15" t="str">
         <f t="shared" si="3"/>
         <v>86078_square</v>
       </c>
-      <c r="M50" s="18" t="str">
+      <c r="M50" s="15" t="str">
         <f t="shared" si="4"/>
         <v>86078</v>
       </c>
-      <c r="N50" s="20" t="b">
+      <c r="N50" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3732,33 +3718,33 @@
         <v>206</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/07_o-crux_pem85023_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.mei -notation square</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="K51" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H51,"image/")</f>
+      <c r="K51" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85023</v>
       </c>
-      <c r="L51" s="18" t="str">
+      <c r="L51" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85023_square</v>
       </c>
-      <c r="M51" s="18" t="str">
+      <c r="M51" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85023</v>
       </c>
-      <c r="N51" s="20" t="b">
+      <c r="N51" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3777,33 +3763,33 @@
         <v>206</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/08_ihesum_pem80113_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.mei </v>
       </c>
       <c r="H52" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="K52" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H52,"image/")</f>
+      <c r="K52" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>80113</v>
       </c>
-      <c r="L52" s="18" t="str">
+      <c r="L52" s="15" t="str">
         <f t="shared" si="3"/>
         <v>80113_aquit</v>
       </c>
-      <c r="M52" s="18" t="str">
+      <c r="M52" s="15" t="str">
         <f t="shared" si="4"/>
         <v>80113</v>
       </c>
-      <c r="N52" s="20" t="b">
+      <c r="N52" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3822,33 +3808,33 @@
         <v>206</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/09_ihesum_pem71112_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.mei -notation square</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="K53" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H53,"image/")</f>
+      <c r="K53" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71112</v>
       </c>
-      <c r="L53" s="18" t="str">
+      <c r="L53" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71112_square</v>
       </c>
-      <c r="M53" s="18" t="str">
+      <c r="M53" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71112</v>
       </c>
-      <c r="N53" s="20" t="b">
+      <c r="N53" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3867,33 +3853,33 @@
         <v>206</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/10_tunc-invocabis_pem80209_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.mei </v>
       </c>
       <c r="H54" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="K54" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H54,"image/")</f>
+      <c r="K54" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>80209</v>
       </c>
-      <c r="L54" s="18" t="str">
+      <c r="L54" s="15" t="str">
         <f t="shared" si="3"/>
         <v>80209_aquit</v>
       </c>
-      <c r="M54" s="18" t="str">
+      <c r="M54" s="15" t="str">
         <f t="shared" si="4"/>
         <v>80209</v>
       </c>
-      <c r="N54" s="20" t="b">
+      <c r="N54" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3912,16 +3898,16 @@
         <v>206</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>272</v>
@@ -3929,19 +3915,19 @@
       <c r="I55" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="K55" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H55,"image/")</f>
+      <c r="K55" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71032</v>
       </c>
-      <c r="L55" s="18" t="str">
+      <c r="L55" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71032_square</v>
       </c>
-      <c r="M55" s="18" t="str">
+      <c r="M55" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71032</v>
       </c>
-      <c r="N55" s="20" t="b">
+      <c r="N55" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3960,33 +3946,33 @@
         <v>206</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/12_si-offers_pem80148-80149_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.mei </v>
       </c>
       <c r="H56" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="K56" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H56,"image/")</f>
+      <c r="K56" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>80148; https://pemdatabase.eu/image/80149</v>
       </c>
-      <c r="L56" s="18" t="str">
+      <c r="L56" s="15" t="str">
         <f t="shared" si="3"/>
         <v>80148-80149_aquit</v>
       </c>
-      <c r="M56" s="18" t="str">
+      <c r="M56" s="15" t="str">
         <f t="shared" si="4"/>
         <v>80148-80149</v>
       </c>
-      <c r="N56" s="20" t="b">
+      <c r="N56" s="16" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -4005,33 +3991,33 @@
         <v>206</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/13_si-offers_pem71205_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.mei -notation square</v>
       </c>
       <c r="H57" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="K57" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H57,"image/")</f>
+      <c r="K57" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71205</v>
       </c>
-      <c r="L57" s="18" t="str">
+      <c r="L57" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71205_square</v>
       </c>
-      <c r="M57" s="18" t="str">
+      <c r="M57" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71205</v>
       </c>
-      <c r="N57" s="20" t="b">
+      <c r="N57" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4050,33 +4036,33 @@
         <v>206</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/14_isti-sunt_pem86046_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.mei </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.mei </v>
       </c>
       <c r="H58" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="K58" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H58,"image/")</f>
+      <c r="K58" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>86046</v>
       </c>
-      <c r="L58" s="18" t="str">
+      <c r="L58" s="15" t="str">
         <f t="shared" si="3"/>
         <v>86046_aquit</v>
       </c>
-      <c r="M58" s="18" t="str">
+      <c r="M58" s="15" t="str">
         <f t="shared" si="4"/>
         <v>86046</v>
       </c>
-      <c r="N58" s="20" t="b">
+      <c r="N58" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4095,33 +4081,33 @@
         <v>206</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/15_isti-sunt_pem85997_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.mei -notation square</v>
       </c>
       <c r="H59" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="K59" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H59,"image/")</f>
+      <c r="K59" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85997</v>
       </c>
-      <c r="L59" s="18" t="str">
+      <c r="L59" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85997_square</v>
       </c>
-      <c r="M59" s="18" t="str">
+      <c r="M59" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85997</v>
       </c>
-      <c r="N59" s="20" t="b">
+      <c r="N59" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4140,33 +4126,33 @@
         <v>206</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/16_mercennarius_pem80028_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.mei </v>
-      </c>
-      <c r="H60" s="14" t="s">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.mei </v>
+      </c>
+      <c r="H60" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="K60" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H60,"image/")</f>
+      <c r="K60" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>80028</v>
       </c>
-      <c r="L60" s="18" t="str">
+      <c r="L60" s="15" t="str">
         <f t="shared" si="3"/>
         <v>80028_aquit</v>
       </c>
-      <c r="M60" s="18" t="str">
+      <c r="M60" s="15" t="str">
         <f t="shared" si="4"/>
         <v>80028</v>
       </c>
-      <c r="N60" s="20" t="b">
+      <c r="N60" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4185,16 +4171,16 @@
         <v>206</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
       <c r="H61" s="11" t="s">
         <v>278</v>
@@ -4202,19 +4188,19 @@
       <c r="I61" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="K61" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H61,"image/")</f>
+      <c r="K61" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>71128</v>
       </c>
-      <c r="L61" s="18" t="str">
+      <c r="L61" s="15" t="str">
         <f t="shared" si="3"/>
         <v>71128_square</v>
       </c>
-      <c r="M61" s="18" t="str">
+      <c r="M61" s="15" t="str">
         <f t="shared" si="4"/>
         <v>71128</v>
       </c>
-      <c r="N61" s="20" t="b">
+      <c r="N61" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4233,33 +4219,33 @@
         <v>206</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/18_o-lux_pem85921_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.mei -notation square</v>
       </c>
       <c r="H62" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="K62" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H62,"image/")</f>
+      <c r="K62" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85921</v>
       </c>
-      <c r="L62" s="18" t="str">
+      <c r="L62" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85921_square</v>
       </c>
-      <c r="M62" s="18" t="str">
+      <c r="M62" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85921</v>
       </c>
-      <c r="N62" s="20" t="b">
+      <c r="N62" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4278,33 +4264,33 @@
         <v>206</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/19_o-lux_pem86009_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.mei -notation square</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K63" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H63,"image/")</f>
+      <c r="K63" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>86009</v>
       </c>
-      <c r="L63" s="18" t="str">
+      <c r="L63" s="15" t="str">
         <f t="shared" si="3"/>
         <v>86009_square</v>
       </c>
-      <c r="M63" s="18" t="str">
+      <c r="M63" s="15" t="str">
         <f t="shared" si="4"/>
         <v>86009</v>
       </c>
-      <c r="N63" s="20" t="b">
+      <c r="N63" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4323,33 +4309,33 @@
         <v>206</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/20_o-lux_pem84967_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.mei -notation square</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="K64" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H64,"image/")</f>
+      <c r="K64" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84967</v>
       </c>
-      <c r="L64" s="18" t="str">
+      <c r="L64" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84967_square</v>
       </c>
-      <c r="M64" s="18" t="str">
+      <c r="M64" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84967</v>
       </c>
-      <c r="N64" s="20" t="b">
+      <c r="N64" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4368,33 +4354,33 @@
         <v>206</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>_aquit</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/21_vespere_pem84633_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.mei </v>
-      </c>
-      <c r="H65" s="14" t="s">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.mei </v>
+      </c>
+      <c r="H65" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="K65" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H65,"image/")</f>
+      <c r="K65" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>84633</v>
       </c>
-      <c r="L65" s="18" t="str">
+      <c r="L65" s="15" t="str">
         <f t="shared" si="3"/>
         <v>84633_aquit</v>
       </c>
-      <c r="M65" s="18" t="str">
+      <c r="M65" s="15" t="str">
         <f t="shared" si="4"/>
         <v>84633</v>
       </c>
-      <c r="N65" s="20" t="b">
+      <c r="N65" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4413,16 +4399,16 @@
         <v>206</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>square</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-notation square</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="2"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
       </c>
       <c r="H66" s="11" t="s">
         <v>283</v>
@@ -4430,19 +4416,19 @@
       <c r="I66" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="K66" s="18" t="str">
-        <f>_xlfn.TEXTAFTER(H66,"image/")</f>
+      <c r="K66" s="15" t="str">
+        <f t="shared" si="7"/>
         <v>85642</v>
       </c>
-      <c r="L66" s="18" t="str">
+      <c r="L66" s="15" t="str">
         <f t="shared" si="3"/>
         <v>85642_square</v>
       </c>
-      <c r="M66" s="18" t="str">
+      <c r="M66" s="15" t="str">
         <f t="shared" si="4"/>
         <v>85642</v>
       </c>
-      <c r="N66" s="20" t="b">
+      <c r="N66" s="16" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -4461,34 +4447,34 @@
         <v>206</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E103" si="6">RIGHT(B67, 6)</f>
+        <f t="shared" ref="E67:E103" si="8">RIGHT(B67, 6)</f>
         <v>square</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F103" si="7">IF(E67="square","-notation square","")</f>
+        <f t="shared" ref="F67:F103" si="9">IF(E67="square","-notation square","")</f>
         <v>-notation square</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G103" si="8">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A67,"/",B67,".gabc MEI_outfiles/", A67, "/", C67, "_", D67, B67, ".mei ",F67)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
+        <f t="shared" si="6"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
       <c r="H67" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="K67" s="18" t="str">
-        <f t="shared" ref="K67:K103" si="9">_xlfn.TEXTAFTER(H67,"image/")</f>
+      <c r="K67" s="15" t="str">
+        <f t="shared" ref="K67:K103" si="10">_xlfn.TEXTAFTER(H67,"image/")</f>
         <v>71108</v>
       </c>
-      <c r="L67" s="18" t="str">
-        <f t="shared" ref="L67:L103" si="10">_xlfn.TEXTAFTER(B67,"pem")</f>
+      <c r="L67" s="15" t="str">
+        <f t="shared" ref="L67:L103" si="11">_xlfn.TEXTAFTER(B67,"pem")</f>
         <v>71108_square</v>
       </c>
-      <c r="M67" s="18" t="str">
-        <f t="shared" ref="M67:M103" si="11">_xlfn.TEXTBEFORE(L67,"_")</f>
+      <c r="M67" s="15" t="str">
+        <f t="shared" ref="M67:M103" si="12">_xlfn.TEXTBEFORE(L67,"_")</f>
         <v>71108</v>
       </c>
-      <c r="N67" s="20" t="b">
-        <f t="shared" ref="N67:N103" si="12">IF(K67=M67, TRUE, FALSE)</f>
+      <c r="N67" s="16" t="b">
+        <f t="shared" ref="N67:N103" si="13">IF(K67=M67, TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -4506,34 +4492,34 @@
         <v>207</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
+        <f t="shared" ref="G68:G103" si="14">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A68,"/",C68,"_",D68,B68,".gabc MEI_outfiles/", A68, "/", C68, "_", D68, B68, ".mei ",F68)</f>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
       <c r="H68" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K68" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K68" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L68" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L68" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M68" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M68" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N68" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N68" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4551,34 +4537,34 @@
         <v>207</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
       <c r="H69" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K69" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K69" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L69" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L69" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M69" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M69" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N69" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N69" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4596,34 +4582,34 @@
         <v>207</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
       <c r="H70" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K70" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K70" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L70" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L70" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M70" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M70" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N70" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N70" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4641,34 +4627,34 @@
         <v>207</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K71" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K71" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L71" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L71" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M71" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M71" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N71" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N71" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4686,34 +4672,34 @@
         <v>207</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
       <c r="H72" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K72" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K72" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L72" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L72" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M72" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M72" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N72" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N72" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4731,34 +4717,34 @@
         <v>207</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K73" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K73" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L73" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L73" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M73" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M73" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N73" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N73" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4776,34 +4762,34 @@
         <v>207</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
       <c r="H74" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K74" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K74" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L74" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L74" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M74" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M74" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N74" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N74" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4821,16 +4807,16 @@
         <v>207</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
       <c r="H75" s="11" t="s">
         <v>286</v>
@@ -4838,20 +4824,20 @@
       <c r="I75" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="K75" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K75" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L75" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L75" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M75" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M75" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N75" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N75" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4869,34 +4855,34 @@
         <v>207</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
       <c r="H76" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K76" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K76" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L76" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L76" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M76" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M76" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N76" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N76" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4914,34 +4900,34 @@
         <v>207</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H77" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K77" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K77" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L77" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L77" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M77" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M77" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N77" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N77" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4959,34 +4945,34 @@
         <v>207</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
       <c r="H78" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K78" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K78" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L78" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L78" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M78" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M78" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N78" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N78" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5004,34 +4990,34 @@
         <v>207</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H79" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K79" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K79" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L79" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L79" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M79" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M79" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N79" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N79" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5049,34 +5035,34 @@
         <v>207</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
       <c r="H80" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K80" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K80" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L80" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L80" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M80" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M80" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N80" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N80" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5094,34 +5080,34 @@
         <v>207</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H81" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K81" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K81" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L81" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L81" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M81" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M81" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N81" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N81" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5139,34 +5125,34 @@
         <v>207</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
       <c r="H82" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K82" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K82" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L82" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L82" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M82" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M82" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N82" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N82" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5184,34 +5170,34 @@
         <v>207</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
       <c r="H83" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K83" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K83" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L83" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L83" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M83" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M83" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N83" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N83" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5229,34 +5215,34 @@
         <v>207</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
       <c r="H84" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="K84" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K84" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>92154</v>
       </c>
-      <c r="L84" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L84" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>92154_aquit</v>
       </c>
-      <c r="M84" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M84" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>92154</v>
       </c>
-      <c r="N84" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N84" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5274,34 +5260,34 @@
         <v>207</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
       <c r="H85" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="K85" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K85" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71010</v>
       </c>
-      <c r="L85" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L85" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71010_square</v>
       </c>
-      <c r="M85" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M85" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71010</v>
       </c>
-      <c r="N85" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N85" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5319,34 +5305,34 @@
         <v>207</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
       <c r="H86" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="K86" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K86" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L86" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L86" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M86" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M86" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N86" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N86" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5364,34 +5350,34 @@
         <v>207</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
       <c r="H87" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="K87" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K87" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71012</v>
       </c>
-      <c r="L87" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L87" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71012_square</v>
       </c>
-      <c r="M87" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M87" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71012</v>
       </c>
-      <c r="N87" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N87" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5409,34 +5395,34 @@
         <v>207</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
       <c r="H88" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="K88" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K88" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L88" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L88" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M88" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M88" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N88" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N88" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5454,34 +5440,34 @@
         <v>207</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="K89" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K89" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71012</v>
       </c>
-      <c r="L89" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L89" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71012_square</v>
       </c>
-      <c r="M89" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M89" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71012</v>
       </c>
-      <c r="N89" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N89" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5499,34 +5485,34 @@
         <v>207</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
       <c r="H90" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="K90" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K90" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L90" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L90" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M90" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M90" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N90" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N90" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5544,34 +5530,34 @@
         <v>207</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="K91" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K91" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71012</v>
       </c>
-      <c r="L91" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L91" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71012_square</v>
       </c>
-      <c r="M91" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M91" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71012</v>
       </c>
-      <c r="N91" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N91" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5589,34 +5575,34 @@
         <v>207</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
       <c r="H92" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="K92" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K92" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L92" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L92" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M92" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M92" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N92" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N92" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5634,34 +5620,34 @@
         <v>207</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="K93" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K93" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71012</v>
       </c>
-      <c r="L93" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L93" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71012_square</v>
       </c>
-      <c r="M93" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M93" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71012</v>
       </c>
-      <c r="N93" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N93" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5679,34 +5665,34 @@
         <v>207</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
       <c r="H94" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="K94" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K94" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L94" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L94" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M94" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M94" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N94" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N94" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5724,34 +5710,34 @@
         <v>207</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
       <c r="H95" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="K95" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K95" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71013</v>
       </c>
-      <c r="L95" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L95" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71013_square</v>
       </c>
-      <c r="M95" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M95" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71013</v>
       </c>
-      <c r="N95" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N95" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5769,34 +5755,34 @@
         <v>207</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
       <c r="H96" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="K96" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K96" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L96" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L96" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M96" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M96" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N96" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N96" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5814,34 +5800,34 @@
         <v>207</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
       <c r="H97" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="K97" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K97" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71013</v>
       </c>
-      <c r="L97" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L97" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71013_square</v>
       </c>
-      <c r="M97" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M97" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71013</v>
       </c>
-      <c r="N97" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N97" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5859,34 +5845,34 @@
         <v>207</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
       <c r="H98" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="K98" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K98" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L98" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L98" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M98" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M98" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N98" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N98" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5904,34 +5890,34 @@
         <v>207</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
       <c r="H99" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="K99" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K99" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71013</v>
       </c>
-      <c r="L99" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L99" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71013_square</v>
       </c>
-      <c r="M99" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M99" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71013</v>
       </c>
-      <c r="N99" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N99" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5949,34 +5935,34 @@
         <v>207</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
       <c r="H100" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="K100" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K100" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L100" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L100" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M100" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M100" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N100" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N100" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -5994,34 +5980,34 @@
         <v>207</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
       <c r="H101" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="K101" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K101" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71013</v>
       </c>
-      <c r="L101" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L101" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71013_square</v>
       </c>
-      <c r="M101" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M101" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71013</v>
       </c>
-      <c r="N101" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N101" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -6039,34 +6025,34 @@
         <v>207</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>_aquit</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
       <c r="H102" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="K102" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K102" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>80159</v>
       </c>
-      <c r="L102" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L102" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>80159_aquit</v>
       </c>
-      <c r="M102" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M102" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>80159</v>
       </c>
-      <c r="N102" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N102" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -6084,34 +6070,34 @@
         <v>207</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>square</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-notation square</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="8"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
+        <f t="shared" si="14"/>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
       <c r="H103" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="K103" s="18" t="str">
-        <f t="shared" si="9"/>
+      <c r="K103" s="15" t="str">
+        <f t="shared" si="10"/>
         <v>71013</v>
       </c>
-      <c r="L103" s="18" t="str">
-        <f t="shared" si="10"/>
+      <c r="L103" s="15" t="str">
+        <f t="shared" si="11"/>
         <v>71013_square</v>
       </c>
-      <c r="M103" s="18" t="str">
-        <f t="shared" si="11"/>
+      <c r="M103" s="15" t="str">
+        <f t="shared" si="12"/>
         <v>71013</v>
       </c>
-      <c r="N103" s="20" t="b">
-        <f t="shared" si="12"/>
+      <c r="N103" s="16" t="b">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix spreadsheet now seems to be good
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D24D47A-6E66-8A4E-82F8-7BF4ED509204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1268545D-0F86-A740-BB6E-1855A2DF3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18320" yWindow="11700" windowWidth="48280" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="25560" yWindow="4280" windowWidth="48280" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="292">
   <si>
     <t>antiphonae_ad_communionem</t>
   </si>
@@ -636,17 +636,317 @@
     <t>Evaluation of links vs. filenames</t>
   </si>
   <si>
-    <t>01_benedicite-omnes_pem82441_aquit</t>
-  </si>
-  <si>
-    <t>02_benedicite-omnes_pem85041_square</t>
+    <t>01_benedicte-omnes_pem82441_aquit</t>
+  </si>
+  <si>
+    <t>02_benedicte-omnes_pem85041_square</t>
+  </si>
+  <si>
+    <t>03_de-fructu-operum_pem56766_aquit</t>
+  </si>
+  <si>
+    <t>04_de-fructu-operum_pem84909_square</t>
+  </si>
+  <si>
+    <t>05_dicit-dominus_pem84540_aquit</t>
+  </si>
+  <si>
+    <t>06_dicit-dominus_pem84623_aquit</t>
+  </si>
+  <si>
+    <t>07_dicit-dominus_pem84873_square</t>
+  </si>
+  <si>
+    <t>08_ecce-virgo_pem84614_aquit</t>
+  </si>
+  <si>
+    <t>09_ecce-virgo_pem84548_aquit</t>
+  </si>
+  <si>
+    <t>10_ecce-virgo_pem84882_square</t>
+  </si>
+  <si>
+    <t>11_jerusalem-surge_pem84878_square</t>
+  </si>
+  <si>
+    <t>12_jerusalem-surge_pem86239_square</t>
+  </si>
+  <si>
+    <t>13_factus-est-repente_pem84630_aquit</t>
+  </si>
+  <si>
+    <t>14_factus-est-repente_pem84881_square</t>
+  </si>
+  <si>
+    <t>15_fili-quid_pem84534_aquit</t>
+  </si>
+  <si>
+    <t>16_fili-quid_pem84863_square</t>
+  </si>
+  <si>
+    <t>17_justorum-animae_pem83892_aquit</t>
+  </si>
+  <si>
+    <t>18_justorum-animae_pem85059_square</t>
+  </si>
+  <si>
+    <t>19_manducaverunt_pem84600_aquit</t>
+  </si>
+  <si>
+    <t>20_manducaverunt_pem83880_aquit</t>
+  </si>
+  <si>
+    <t>21_manducaverunt_pem84880_square</t>
+  </si>
+  <si>
+    <t>22_martinus-abrahe_pem84580_aquit</t>
+  </si>
+  <si>
+    <t>23_martinus-abrahe_pem85056_square</t>
+  </si>
+  <si>
+    <t>24_mitte-manum_pem83911_aquit</t>
+  </si>
+  <si>
+    <t>25_mitte-manum_pem84665_aquit</t>
+  </si>
+  <si>
+    <t>26_mitte-manum_pem84905_square</t>
+  </si>
+  <si>
+    <t>27_panem-de-caelo_pem84532_aquit</t>
+  </si>
+  <si>
+    <t>28_panem-de-caelo_pem84919_square</t>
+  </si>
+  <si>
+    <t>29_pater-si-non_pem84595_aquit</t>
+  </si>
+  <si>
+    <t>30_pater-si-non_pem84872_square</t>
+  </si>
+  <si>
+    <t>31_psallite-domino_pem84666_aquit</t>
+  </si>
+  <si>
+    <t>32_psallite-domino_pem84874_square</t>
+  </si>
+  <si>
+    <t>33_qui-manducat--carnem_pem76616_aquit</t>
+  </si>
+  <si>
+    <t>34_qui-manducat--panem_pem119191_aquit</t>
+  </si>
+  <si>
+    <t>35_qui-manducat_pem84924_square</t>
+  </si>
+  <si>
+    <t>36_qui-vult_pem84057_aquit</t>
+  </si>
+  <si>
+    <t>37_qui-vult_pem85065_square</t>
+  </si>
+  <si>
+    <t>38_tu-es-petrus_pem83876_aquit</t>
+  </si>
+  <si>
+    <t>39_tu-es-petrus_pem85073_square</t>
+  </si>
+  <si>
+    <t>40_tu-mandasti_pem83869_aquit</t>
+  </si>
+  <si>
+    <t>41_tu-mandasti_pem84946_square</t>
+  </si>
+  <si>
+    <t>42_vos-qui-secuti_pem84570_aquit</t>
+  </si>
+  <si>
+    <t>43_vos-qui-secuti_pem85037_square</t>
+  </si>
+  <si>
+    <t>01_nemo-te_pem85014_aquit</t>
+  </si>
+  <si>
+    <t>02_nemo-te_pem71059_square</t>
+  </si>
+  <si>
+    <t>03_serve-nequam_pem85026_aquit</t>
+  </si>
+  <si>
+    <t>04_serve-nequam_pem71210_square</t>
+  </si>
+  <si>
+    <t>05_o-crux_pem85972_square</t>
+  </si>
+  <si>
+    <t>06_o-crux_pem86078_square</t>
+  </si>
+  <si>
+    <t>07_o-crux_pem85023_square</t>
+  </si>
+  <si>
+    <t>08_ihesum_pem80113_aquit</t>
+  </si>
+  <si>
+    <t>09_ihesum_pem71112_square</t>
+  </si>
+  <si>
+    <t>10_tunc-invocabis_pem80209_aquit</t>
+  </si>
+  <si>
+    <t>11_tunc-invocabis_pem71032_square</t>
+  </si>
+  <si>
+    <t>12_si-offers_pem80148-80149_aquit</t>
+  </si>
+  <si>
+    <t>13_si-offers_pem71205_square</t>
+  </si>
+  <si>
+    <t>14_isti-sunt_pem86046_aquit</t>
+  </si>
+  <si>
+    <t>15_isti-sunt_pem85997_square</t>
+  </si>
+  <si>
+    <t>16_mercennarius_pem80028_aquit</t>
+  </si>
+  <si>
+    <t>17_mercennarius_pem71128_square</t>
+  </si>
+  <si>
+    <t>18_o-lux_pem85921_square</t>
+  </si>
+  <si>
+    <t>19_o-lux_pem86009_square</t>
+  </si>
+  <si>
+    <t>20_o-lux_pem84967_square</t>
+  </si>
+  <si>
+    <t>21_vespere_pem84633_aquit</t>
+  </si>
+  <si>
+    <t>22_vespere_pem85642_square</t>
+  </si>
+  <si>
+    <t>23_vespere_pem71108_square</t>
+  </si>
+  <si>
+    <t>01_tibi-soli-peccavi_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>02_tibi-soli-peccavi_pem71010_square</t>
+  </si>
+  <si>
+    <t>03_domine-refugium_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>04_domine-refugium_pem71010_square</t>
+  </si>
+  <si>
+    <t>05_in-matutinis_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>06_in-matutinis_pem71010_square</t>
+  </si>
+  <si>
+    <t>07_cantemus-domino_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>08_cantemus-domino_pem71010_square</t>
+  </si>
+  <si>
+    <t>09_in-sanctis-ejus_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>10_in-sanctis-ejus_pem71010_square</t>
+  </si>
+  <si>
+    <t>11_in-sanctitate-serviamus_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>12_in-sanctitate-serviamus_pem71010_square</t>
+  </si>
+  <si>
+    <t>13_et-omnis_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>14_et-omnis_pem71010_square</t>
+  </si>
+  <si>
+    <t>15_ecce-quam-bonum_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>16_ecce-quam-bonum_pem71010_square</t>
+  </si>
+  <si>
+    <t>17_laudate-nomen_pem92154_aquit</t>
+  </si>
+  <si>
+    <t>18_laudate-nomen_pem71010_square</t>
+  </si>
+  <si>
+    <t>19_metuant-dominum_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>20_metuant-dominum_pem71012_square</t>
+  </si>
+  <si>
+    <t>21_et-in-servis_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>22_et-in-servis_pem71012_square</t>
+  </si>
+  <si>
+    <t>23_in-cimbalis_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>24_in-cimbalis_pem71012_square</t>
+  </si>
+  <si>
+    <t>25_in-viam_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>26_in-viam_pem71012_square</t>
+  </si>
+  <si>
+    <t>27_benedictus_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>28_benedictus_pem71013_square</t>
+  </si>
+  <si>
+    <t>29_per-singulos_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>30_per-singulos_pem71013_square</t>
+  </si>
+  <si>
+    <t>31_laudabo_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>32_laudabo_pem71013_square</t>
+  </si>
+  <si>
+    <t>33_deo-nostro_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>34_deo-nostro_pem71013_square</t>
+  </si>
+  <si>
+    <t>35_benedixit_pem80159_aquit</t>
+  </si>
+  <si>
+    <t>36_benedixit_pem71013_square</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -703,6 +1003,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -769,7 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -798,6 +1103,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1130,7 +1436,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3:B103"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1507,7 @@
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A2,"/",C2,"_",D2,B2,".gabc MEI_outfiles/", A2, "/", C2, "_", D2, B2, ".mei ",F2)</f>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/001_C01_benedicite-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicite-omnes_pem82441_aquit.mei </v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
       </c>
       <c r="H2" s="12" t="s">
         <v>118</v>
@@ -1246,7 +1552,7 @@
       </c>
       <c r="G3" t="str">
         <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A3,"/",C3,"_",D3,B3,".gabc MEI_outfiles/", A3, "/", C3, "_", D3, B3, ".mei ",F3)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/002_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>119</v>
@@ -1273,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1283,15 +1589,15 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G4" t="str">
         <f t="shared" ref="G4:G67" si="6">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A4,"/",C4,"_",D4,B4,".gabc MEI_outfiles/", A4, "/", C4, "_", D4, B4, ".mei ",F4)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/003_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/003_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/003_C03_de-fructu-operum_pem56766_aquit.mei </v>
       </c>
       <c r="H4" s="12" t="s">
         <v>120</v>
@@ -1302,15 +1608,15 @@
       </c>
       <c r="L4" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>56766_aquit</v>
       </c>
       <c r="M4" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>56766</v>
       </c>
       <c r="N4" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1318,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1336,7 +1642,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/004_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.gabc MEI_outfiles/antiphonae_ad_communionem/004_C04_de-fructu-operum_pem84909_square.mei -notation square</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>121</v>
@@ -1347,15 +1653,15 @@
       </c>
       <c r="L5" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84909_square</v>
       </c>
       <c r="M5" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84909</v>
       </c>
       <c r="N5" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1363,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1373,15 +1679,15 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/005_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/005_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/005_C05_dicit-dominus_pem84540_aquit.mei </v>
       </c>
       <c r="H6" s="12" t="s">
         <v>122</v>
@@ -1392,15 +1698,15 @@
       </c>
       <c r="L6" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84540_aquit</v>
       </c>
       <c r="M6" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84540</v>
       </c>
       <c r="N6" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1408,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -1418,15 +1724,15 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/006_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/006_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/006_C06_dicit-dominus_pem84623_aquit.mei </v>
       </c>
       <c r="H7" s="12" t="s">
         <v>123</v>
@@ -1437,15 +1743,15 @@
       </c>
       <c r="L7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84623_aquit</v>
       </c>
       <c r="M7" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84623</v>
       </c>
       <c r="N7" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1453,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1471,7 +1777,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/007_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.gabc MEI_outfiles/antiphonae_ad_communionem/007_C07_dicit-dominus_pem84873_square.mei -notation square</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>124</v>
@@ -1485,15 +1791,15 @@
       </c>
       <c r="L8" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84873_square</v>
       </c>
       <c r="M8" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84873</v>
       </c>
       <c r="N8" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1501,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1511,15 +1817,15 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/008_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/008_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/008_C08_ecce-virgo_pem84614_aquit.mei </v>
       </c>
       <c r="H9" s="13" t="s">
         <v>125</v>
@@ -1530,15 +1836,15 @@
       </c>
       <c r="L9" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84614_aquit</v>
       </c>
       <c r="M9" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84614</v>
       </c>
       <c r="N9" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1546,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
@@ -1556,15 +1862,15 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/009_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/009_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/009_C09_ecce-virgo_pem84548_aquit.mei </v>
       </c>
       <c r="H10" s="13" t="s">
         <v>126</v>
@@ -1575,15 +1881,15 @@
       </c>
       <c r="L10" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84548_aquit</v>
       </c>
       <c r="M10" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84548</v>
       </c>
       <c r="N10" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1591,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -1609,7 +1915,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/010_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.gabc MEI_outfiles/antiphonae_ad_communionem/010_C10_ecce-virgo_pem84882_square.mei -notation square</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>127</v>
@@ -1620,15 +1926,15 @@
       </c>
       <c r="L11" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84882_square</v>
       </c>
       <c r="M11" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84882</v>
       </c>
       <c r="N11" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1636,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
@@ -1654,7 +1960,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/011_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.gabc MEI_outfiles/antiphonae_ad_communionem/011_C11_jerusalem-surge_pem84878_square.mei -notation square</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>128</v>
@@ -1665,15 +1971,15 @@
       </c>
       <c r="L12" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84878_square</v>
       </c>
       <c r="M12" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84878</v>
       </c>
       <c r="N12" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1681,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
@@ -1699,7 +2005,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/012_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.gabc MEI_outfiles/antiphonae_ad_communionem/012_C12_jerusalem-surge_pem86239_square.mei -notation square</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>129</v>
@@ -1713,15 +2019,15 @@
       </c>
       <c r="L13" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>86239_square</v>
       </c>
       <c r="M13" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>86239</v>
       </c>
       <c r="N13" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1729,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -1739,15 +2045,15 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/013_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/013_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/013_C13_factus-est-repente_pem84630_aquit.mei </v>
       </c>
       <c r="H14" s="13" t="s">
         <v>130</v>
@@ -1758,15 +2064,15 @@
       </c>
       <c r="L14" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84630_aquit</v>
       </c>
       <c r="M14" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84630</v>
       </c>
       <c r="N14" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1774,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -1792,7 +2098,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/014_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.gabc MEI_outfiles/antiphonae_ad_communionem/014_C14_factus-est-repente_pem84881_square.mei -notation square</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>131</v>
@@ -1803,15 +2109,15 @@
       </c>
       <c r="L15" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84881_square</v>
       </c>
       <c r="M15" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84881</v>
       </c>
       <c r="N15" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1819,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -1829,15 +2135,15 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/015_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/015_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/015_C15_fili-quid_pem84534_aquit.mei </v>
       </c>
       <c r="H16" s="13" t="s">
         <v>132</v>
@@ -1848,15 +2154,15 @@
       </c>
       <c r="L16" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84534_aquit</v>
       </c>
       <c r="M16" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84534</v>
       </c>
       <c r="N16" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1864,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1882,7 +2188,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/016_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.gabc MEI_outfiles/antiphonae_ad_communionem/016_C16_fili-quid_pem84863_square.mei -notation square</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>133</v>
@@ -1893,15 +2199,15 @@
       </c>
       <c r="L17" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84863_square</v>
       </c>
       <c r="M17" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84863</v>
       </c>
       <c r="N17" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1909,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
@@ -1919,15 +2225,15 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/017_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/017_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/017_C17_justorum-animae_pem83892_aquit.mei </v>
       </c>
       <c r="H18" s="10" t="s">
         <v>134</v>
@@ -1938,15 +2244,15 @@
       </c>
       <c r="L18" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>83892_aquit</v>
       </c>
       <c r="M18" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>83892</v>
       </c>
       <c r="N18" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1954,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
@@ -1972,7 +2278,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/018_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.gabc MEI_outfiles/antiphonae_ad_communionem/018_C18_justorum-animae_pem85059_square.mei -notation square</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>135</v>
@@ -1983,15 +2289,15 @@
       </c>
       <c r="L19" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85059_square</v>
       </c>
       <c r="M19" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85059</v>
       </c>
       <c r="N19" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -1999,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -2009,15 +2315,15 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/019_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/019_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/019_C19_manducaverunt_pem84600_aquit.mei </v>
       </c>
       <c r="H20" s="10" t="s">
         <v>136</v>
@@ -2028,15 +2334,15 @@
       </c>
       <c r="L20" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84600_aquit</v>
       </c>
       <c r="M20" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84600</v>
       </c>
       <c r="N20" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2044,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -2054,15 +2360,15 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/020_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/020_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/020_C20_manducaverunt_pem83880_aquit.mei </v>
       </c>
       <c r="H21" s="10" t="s">
         <v>137</v>
@@ -2073,15 +2379,15 @@
       </c>
       <c r="L21" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>83880_aquit</v>
       </c>
       <c r="M21" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>83880</v>
       </c>
       <c r="N21" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2089,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -2107,7 +2413,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/021_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.gabc MEI_outfiles/antiphonae_ad_communionem/021_C21_manducaverunt_pem84880_square.mei -notation square</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>138</v>
@@ -2118,15 +2424,15 @@
       </c>
       <c r="L22" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84880_square</v>
       </c>
       <c r="M22" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84880</v>
       </c>
       <c r="N22" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2134,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
@@ -2144,15 +2450,15 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/022_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/022_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/022_C22_martinus-abrahe_pem84580_aquit.mei </v>
       </c>
       <c r="H23" s="11" t="s">
         <v>139</v>
@@ -2163,15 +2469,15 @@
       </c>
       <c r="L23" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84580_aquit</v>
       </c>
       <c r="M23" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84580</v>
       </c>
       <c r="N23" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -2179,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -2197,7 +2503,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/023_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.gabc MEI_outfiles/antiphonae_ad_communionem/023_C23_martinus-abrahe_pem85056_square.mei -notation square</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>140</v>
@@ -2208,15 +2514,15 @@
       </c>
       <c r="L24" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85056_square</v>
       </c>
       <c r="M24" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85056</v>
       </c>
       <c r="N24" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -2224,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -2234,15 +2540,15 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/024_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/024_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/024_C24_mitte-manum_pem83911_aquit.mei </v>
       </c>
       <c r="H25" s="8" t="s">
         <v>141</v>
@@ -2253,15 +2559,15 @@
       </c>
       <c r="L25" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>83911_aquit</v>
       </c>
       <c r="M25" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>83911</v>
       </c>
       <c r="N25" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2269,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -2279,15 +2585,15 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/025_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/025_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/025_C25_mitte-manum_pem84665_aquit.mei </v>
       </c>
       <c r="H26" s="10" t="s">
         <v>142</v>
@@ -2298,15 +2604,15 @@
       </c>
       <c r="L26" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84665_aquit</v>
       </c>
       <c r="M26" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84665</v>
       </c>
       <c r="N26" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2314,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>28</v>
@@ -2332,7 +2638,7 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/026_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.gabc MEI_outfiles/antiphonae_ad_communionem/026_C26_mitte-manum_pem84905_square.mei -notation square</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>143</v>
@@ -2346,15 +2652,15 @@
       </c>
       <c r="L27" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84905_square</v>
       </c>
       <c r="M27" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84905</v>
       </c>
       <c r="N27" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -2362,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>29</v>
@@ -2372,15 +2678,15 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/027_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/027_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/027_C27_panem-de-caelo_pem84532_aquit.mei </v>
       </c>
       <c r="H28" s="12" t="s">
         <v>144</v>
@@ -2391,15 +2697,15 @@
       </c>
       <c r="L28" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84532_aquit</v>
       </c>
       <c r="M28" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84532</v>
       </c>
       <c r="N28" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2407,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>30</v>
@@ -2425,7 +2731,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/028_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.gabc MEI_outfiles/antiphonae_ad_communionem/028_C28_panem-de-caelo_pem84919_square.mei -notation square</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>145</v>
@@ -2436,15 +2742,15 @@
       </c>
       <c r="L29" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84919_square</v>
       </c>
       <c r="M29" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84919</v>
       </c>
       <c r="N29" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -2452,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>31</v>
@@ -2462,15 +2768,15 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/029_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/029_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/029_C29_pater-si-non_pem84595_aquit.mei </v>
       </c>
       <c r="H30" s="12" t="s">
         <v>146</v>
@@ -2481,15 +2787,15 @@
       </c>
       <c r="L30" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84595_aquit</v>
       </c>
       <c r="M30" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84595</v>
       </c>
       <c r="N30" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2497,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>32</v>
@@ -2515,7 +2821,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/030_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.gabc MEI_outfiles/antiphonae_ad_communionem/030_C30_pater-si-non_pem84872_square.mei -notation square</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>147</v>
@@ -2526,15 +2832,15 @@
       </c>
       <c r="L31" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84872_square</v>
       </c>
       <c r="M31" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84872</v>
       </c>
       <c r="N31" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2542,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>33</v>
@@ -2552,15 +2858,15 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/031_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/031_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/031_C31_psallite-domino_pem84666_aquit.mei </v>
       </c>
       <c r="H32" s="10" t="s">
         <v>148</v>
@@ -2571,15 +2877,15 @@
       </c>
       <c r="L32" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84666_aquit</v>
       </c>
       <c r="M32" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84666</v>
       </c>
       <c r="N32" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2587,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>34</v>
@@ -2605,7 +2911,7 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/032_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.gabc MEI_outfiles/antiphonae_ad_communionem/032_C32_psallite-domino_pem84874_square.mei -notation square</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>149</v>
@@ -2616,15 +2922,15 @@
       </c>
       <c r="L33" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84874_square</v>
       </c>
       <c r="M33" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84874</v>
       </c>
       <c r="N33" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2632,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>35</v>
@@ -2642,15 +2948,15 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/033_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/033_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/033_C33_qui-manducat--carnem_pem76616_aquit.mei </v>
       </c>
       <c r="H34" s="10" t="s">
         <v>150</v>
@@ -2661,15 +2967,15 @@
       </c>
       <c r="L34" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>76616_aquit</v>
       </c>
       <c r="M34" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>76616</v>
       </c>
       <c r="N34" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2677,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>36</v>
@@ -2687,15 +2993,15 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/034_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/034_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/034_C34_qui-manducat--panem_pem119191_aquit.mei </v>
       </c>
       <c r="H35" s="10" t="s">
         <v>151</v>
@@ -2706,15 +3012,15 @@
       </c>
       <c r="L35" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>119191_aquit</v>
       </c>
       <c r="M35" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>119191</v>
       </c>
       <c r="N35" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2722,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>37</v>
@@ -2740,7 +3046,7 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/035_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.gabc MEI_outfiles/antiphonae_ad_communionem/035_C35_qui-manducat_pem84924_square.mei -notation square</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>152</v>
@@ -2751,15 +3057,15 @@
       </c>
       <c r="L36" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84924_square</v>
       </c>
       <c r="M36" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84924</v>
       </c>
       <c r="N36" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2767,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>38</v>
@@ -2777,15 +3083,15 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/036_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/036_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/036_C36_qui-vult_pem84057_aquit.mei </v>
       </c>
       <c r="H37" s="10" t="s">
         <v>153</v>
@@ -2796,23 +3102,23 @@
       </c>
       <c r="L37" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84057_aquit</v>
       </c>
       <c r="M37" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84057</v>
       </c>
       <c r="N37" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>191</v>
+      <c r="B38" s="18" t="s">
+        <v>226</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>39</v>
@@ -2830,7 +3136,7 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/037_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.gabc MEI_outfiles/antiphonae_ad_communionem/037_C37_qui-vult_pem85065_square.mei -notation square</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>154</v>
@@ -2844,15 +3150,15 @@
       </c>
       <c r="L38" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85065_square</v>
       </c>
       <c r="M38" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85065</v>
       </c>
       <c r="N38" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2860,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>40</v>
@@ -2870,15 +3176,15 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/038_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/038_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/038_C38_tu-es-petrus_pem83876_aquit.mei </v>
       </c>
       <c r="H39" s="10" t="s">
         <v>155</v>
@@ -2889,15 +3195,15 @@
       </c>
       <c r="L39" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>83876_aquit</v>
       </c>
       <c r="M39" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>83876</v>
       </c>
       <c r="N39" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2905,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>41</v>
@@ -2923,7 +3229,7 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/039_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.gabc MEI_outfiles/antiphonae_ad_communionem/039_C39_tu-es-petrus_pem85073_square.mei -notation square</v>
       </c>
       <c r="H40" s="10" t="s">
         <v>156</v>
@@ -2934,15 +3240,15 @@
       </c>
       <c r="L40" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85073_square</v>
       </c>
       <c r="M40" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85073</v>
       </c>
       <c r="N40" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2950,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>42</v>
@@ -2960,15 +3266,15 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/040_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/040_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/040_C40_tu-mandasti_pem83869_aquit.mei </v>
       </c>
       <c r="H41" s="10" t="s">
         <v>157</v>
@@ -2979,15 +3285,15 @@
       </c>
       <c r="L41" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>83869_aquit</v>
       </c>
       <c r="M41" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>83869</v>
       </c>
       <c r="N41" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2995,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>43</v>
@@ -3013,7 +3319,7 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/041_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.gabc MEI_outfiles/antiphonae_ad_communionem/041_C41_tu-mandasti_pem84946_square.mei -notation square</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>158</v>
@@ -3024,15 +3330,15 @@
       </c>
       <c r="L42" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84946_square</v>
       </c>
       <c r="M42" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84946</v>
       </c>
       <c r="N42" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3040,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>44</v>
@@ -3050,15 +3356,15 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/042_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/042_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/042_C42_vos-qui-secuti_pem84570_aquit.mei </v>
       </c>
       <c r="H43" s="10" t="s">
         <v>159</v>
@@ -3069,15 +3375,15 @@
       </c>
       <c r="L43" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84570_aquit</v>
       </c>
       <c r="M43" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84570</v>
       </c>
       <c r="N43" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3085,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>45</v>
@@ -3103,7 +3409,7 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/043_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.gabc MEI_outfiles/antiphonae_ad_communionem/043_C43_vos-qui-secuti_pem85037_square.mei -notation square</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>160</v>
@@ -3114,15 +3420,15 @@
       </c>
       <c r="L44" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85037_square</v>
       </c>
       <c r="M44" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85037</v>
       </c>
       <c r="N44" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3130,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>46</v>
@@ -3140,15 +3446,15 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/044_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/044_M01_nemo-te_pem85014_aquit.mei </v>
       </c>
       <c r="H45" s="10" t="s">
         <v>161</v>
@@ -3159,15 +3465,15 @@
       </c>
       <c r="L45" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85014_aquit</v>
       </c>
       <c r="M45" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85014</v>
       </c>
       <c r="N45" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3175,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>47</v>
@@ -3193,7 +3499,7 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/045_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.gabc MEI_outfiles/antiphonae_ad_magnificat/045_M02_nemo-te_pem71059_square.mei -notation square</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>162</v>
@@ -3204,15 +3510,15 @@
       </c>
       <c r="L46" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71059_square</v>
       </c>
       <c r="M46" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71059</v>
       </c>
       <c r="N46" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3220,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -3230,15 +3536,15 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/046_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/046_M03_serve-nequam_pem85026_aquit.mei </v>
       </c>
       <c r="H47" s="10" t="s">
         <v>163</v>
@@ -3249,15 +3555,15 @@
       </c>
       <c r="L47" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85026_aquit</v>
       </c>
       <c r="M47" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85026</v>
       </c>
       <c r="N47" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3265,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>49</v>
@@ -3283,7 +3589,7 @@
       </c>
       <c r="G48" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/047_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.gabc MEI_outfiles/antiphonae_ad_magnificat/047_M04_serve-nequam_pem71210_square.mei -notation square</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>164</v>
@@ -3297,15 +3603,15 @@
       </c>
       <c r="L48" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71210_square</v>
       </c>
       <c r="M48" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71210</v>
       </c>
       <c r="N48" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3313,7 +3619,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>50</v>
@@ -3331,7 +3637,7 @@
       </c>
       <c r="G49" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/048_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.gabc MEI_outfiles/antiphonae_ad_magnificat/048_M05_o-crux_pem85972_square.mei -notation square</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>165</v>
@@ -3342,15 +3648,15 @@
       </c>
       <c r="L49" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85972_square</v>
       </c>
       <c r="M49" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85972</v>
       </c>
       <c r="N49" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3358,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>51</v>
@@ -3376,7 +3682,7 @@
       </c>
       <c r="G50" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/049_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.gabc MEI_outfiles/antiphonae_ad_magnificat/049_M06_o-crux_pem86078_square.mei -notation square</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>166</v>
@@ -3387,15 +3693,15 @@
       </c>
       <c r="L50" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>86078_square</v>
       </c>
       <c r="M50" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>86078</v>
       </c>
       <c r="N50" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3403,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>52</v>
@@ -3421,7 +3727,7 @@
       </c>
       <c r="G51" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/050_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.gabc MEI_outfiles/antiphonae_ad_magnificat/050_M07_o-crux_pem85023_square.mei -notation square</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>167</v>
@@ -3432,15 +3738,15 @@
       </c>
       <c r="L51" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85023_square</v>
       </c>
       <c r="M51" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85023</v>
       </c>
       <c r="N51" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3448,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>53</v>
@@ -3458,15 +3764,15 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/051_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/051_M08_ihesum_pem80113_aquit.mei </v>
       </c>
       <c r="H52" s="10" t="s">
         <v>168</v>
@@ -3477,15 +3783,15 @@
       </c>
       <c r="L52" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>80113_aquit</v>
       </c>
       <c r="M52" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>80113</v>
       </c>
       <c r="N52" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3493,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>54</v>
@@ -3511,7 +3817,7 @@
       </c>
       <c r="G53" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/052_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.gabc MEI_outfiles/antiphonae_ad_magnificat/052_M09_ihesum_pem71112_square.mei -notation square</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>169</v>
@@ -3522,15 +3828,15 @@
       </c>
       <c r="L53" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71112_square</v>
       </c>
       <c r="M53" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71112</v>
       </c>
       <c r="N53" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3538,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>191</v>
+        <v>242</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>55</v>
@@ -3548,15 +3854,15 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/053_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/053_M10_tunc-invocabis_pem80209_aquit.mei </v>
       </c>
       <c r="H54" s="10" t="s">
         <v>170</v>
@@ -3567,15 +3873,15 @@
       </c>
       <c r="L54" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>80209_aquit</v>
       </c>
       <c r="M54" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>80209</v>
       </c>
       <c r="N54" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3583,7 +3889,7 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>191</v>
+        <v>243</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>56</v>
@@ -3601,7 +3907,7 @@
       </c>
       <c r="G55" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/054_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.gabc MEI_outfiles/antiphonae_ad_magnificat/054_M11_tunc-invocabis_pem71032_square.mei -notation square</v>
       </c>
       <c r="H55" s="10" t="s">
         <v>171</v>
@@ -3615,15 +3921,15 @@
       </c>
       <c r="L55" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71032_square</v>
       </c>
       <c r="M55" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71032</v>
       </c>
       <c r="N55" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="28" x14ac:dyDescent="0.2">
@@ -3631,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>57</v>
@@ -3641,15 +3947,15 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/055_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/055_M12_si-offers_pem80148-80149_aquit.mei </v>
       </c>
       <c r="H56" s="9" t="s">
         <v>172</v>
@@ -3660,11 +3966,11 @@
       </c>
       <c r="L56" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>80148-80149_aquit</v>
       </c>
       <c r="M56" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>80148-80149</v>
       </c>
       <c r="N56" s="15" t="b">
         <f t="shared" si="5"/>
@@ -3676,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>191</v>
+        <v>245</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>58</v>
@@ -3694,7 +4000,7 @@
       </c>
       <c r="G57" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/056_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.gabc MEI_outfiles/antiphonae_ad_magnificat/056_M13_si-offers_pem71205_square.mei -notation square</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>173</v>
@@ -3705,15 +4011,15 @@
       </c>
       <c r="L57" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71205_square</v>
       </c>
       <c r="M57" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71205</v>
       </c>
       <c r="N57" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3721,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>59</v>
@@ -3731,15 +4037,15 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/057_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/057_M14_isti-sunt_pem86046_aquit.mei </v>
       </c>
       <c r="H58" s="10" t="s">
         <v>174</v>
@@ -3750,15 +4056,15 @@
       </c>
       <c r="L58" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>86046_aquit</v>
       </c>
       <c r="M58" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>86046</v>
       </c>
       <c r="N58" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3766,7 +4072,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>60</v>
@@ -3784,7 +4090,7 @@
       </c>
       <c r="G59" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/058_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.gabc MEI_outfiles/antiphonae_ad_magnificat/058_M15_isti-sunt_pem85997_square.mei -notation square</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>175</v>
@@ -3795,15 +4101,15 @@
       </c>
       <c r="L59" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85997_square</v>
       </c>
       <c r="M59" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85997</v>
       </c>
       <c r="N59" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -3811,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>191</v>
+        <v>248</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>61</v>
@@ -3821,15 +4127,15 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/059_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/059_M16_mercennarius_pem80028_aquit.mei </v>
       </c>
       <c r="H60" s="12" t="s">
         <v>176</v>
@@ -3840,15 +4146,15 @@
       </c>
       <c r="L60" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>80028_aquit</v>
       </c>
       <c r="M60" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>80028</v>
       </c>
       <c r="N60" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3856,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>62</v>
@@ -3874,7 +4180,7 @@
       </c>
       <c r="G61" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/060_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.gabc MEI_outfiles/antiphonae_ad_magnificat/060_M17_mercennarius_pem71128_square.mei -notation square</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>177</v>
@@ -3888,15 +4194,15 @@
       </c>
       <c r="L61" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>71128_square</v>
       </c>
       <c r="M61" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>71128</v>
       </c>
       <c r="N61" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3904,7 +4210,7 @@
         <v>1</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>63</v>
@@ -3922,7 +4228,7 @@
       </c>
       <c r="G62" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/061_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.gabc MEI_outfiles/antiphonae_ad_magnificat/061_M18_o-lux_pem85921_square.mei -notation square</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>178</v>
@@ -3933,15 +4239,15 @@
       </c>
       <c r="L62" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85921_square</v>
       </c>
       <c r="M62" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85921</v>
       </c>
       <c r="N62" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3949,7 +4255,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>64</v>
@@ -3967,7 +4273,7 @@
       </c>
       <c r="G63" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/062_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.gabc MEI_outfiles/antiphonae_ad_magnificat/062_M19_o-lux_pem86009_square.mei -notation square</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>179</v>
@@ -3978,15 +4284,15 @@
       </c>
       <c r="L63" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>86009_square</v>
       </c>
       <c r="M63" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>86009</v>
       </c>
       <c r="N63" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -3994,7 +4300,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>65</v>
@@ -4012,7 +4318,7 @@
       </c>
       <c r="G64" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/063_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.gabc MEI_outfiles/antiphonae_ad_magnificat/063_M20_o-lux_pem84967_square.mei -notation square</v>
       </c>
       <c r="H64" s="10" t="s">
         <v>180</v>
@@ -4023,15 +4329,15 @@
       </c>
       <c r="L64" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84967_square</v>
       </c>
       <c r="M64" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84967</v>
       </c>
       <c r="N64" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -4039,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>191</v>
+        <v>253</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>66</v>
@@ -4049,15 +4355,15 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="2"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/064_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.gabc MEI_outfiles/antiphonae_ad_magnificat/064_M21_vespere_pem84633_aquit.mei </v>
       </c>
       <c r="H65" s="12" t="s">
         <v>181</v>
@@ -4068,15 +4374,15 @@
       </c>
       <c r="L65" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>84633_aquit</v>
       </c>
       <c r="M65" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>84633</v>
       </c>
       <c r="N65" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4084,7 +4390,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>191</v>
+        <v>254</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>67</v>
@@ -4102,7 +4408,7 @@
       </c>
       <c r="G66" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/065_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.gabc MEI_outfiles/antiphonae_ad_magnificat/065_M22_vespere_pem85642_square.mei -notation square</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>182</v>
@@ -4116,15 +4422,15 @@
       </c>
       <c r="L66" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>85041_square</v>
+        <v>85642_square</v>
       </c>
       <c r="M66" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>85041</v>
+        <v>85642</v>
       </c>
       <c r="N66" s="15" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4132,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>68</v>
@@ -4150,7 +4456,7 @@
       </c>
       <c r="G67" t="str">
         <f t="shared" si="6"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/066_M02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.gabc MEI_outfiles/antiphonae_ad_magnificat/066_M23_vespere_pem71108_square.mei -notation square</v>
       </c>
       <c r="H67" s="10" t="s">
         <v>183</v>
@@ -4161,15 +4467,15 @@
       </c>
       <c r="L67" s="14" t="str">
         <f t="shared" ref="L67:L103" si="11">_xlfn.TEXTAFTER(B67,"pem")</f>
-        <v>85041_square</v>
+        <v>71108_square</v>
       </c>
       <c r="M67" s="14" t="str">
         <f t="shared" ref="M67:M103" si="12">_xlfn.TEXTBEFORE(L67,"_")</f>
-        <v>85041</v>
+        <v>71108</v>
       </c>
       <c r="N67" s="15" t="b">
         <f t="shared" ref="N67:N103" si="13">IF(K67=M67, TRUE, FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4177,7 +4483,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>191</v>
+        <v>256</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>69</v>
@@ -4187,15 +4493,15 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G103" si="14">_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A68,"/",C68,"_",D68,B68,".gabc MEI_outfiles/", A68, "/", C68, "_", D68, B68, ".mei ",F68)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/067_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/067_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/067_F01_tibi-soli-peccavi_pem92154_aquit.mei </v>
       </c>
       <c r="H68" s="10" t="s">
         <v>184</v>
@@ -4206,15 +4512,15 @@
       </c>
       <c r="L68" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M68" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N68" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4222,7 +4528,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>191</v>
+        <v>257</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>70</v>
@@ -4240,7 +4546,7 @@
       </c>
       <c r="G69" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/068_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/068_F02_tibi-soli-peccavi_pem71010_square.mei -notation square</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>185</v>
@@ -4251,15 +4557,15 @@
       </c>
       <c r="L69" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M69" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N69" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4267,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>191</v>
+        <v>258</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>71</v>
@@ -4277,15 +4583,15 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/069_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/069_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/069_F03_domine-refugium_pem92154_aquit.mei </v>
       </c>
       <c r="H70" s="10" t="s">
         <v>184</v>
@@ -4296,15 +4602,15 @@
       </c>
       <c r="L70" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M70" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N70" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4312,7 +4618,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>191</v>
+        <v>259</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>72</v>
@@ -4330,7 +4636,7 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/070_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/070_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/070_F04_domine-refugium_pem71010_square.mei -notation square</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>185</v>
@@ -4341,15 +4647,15 @@
       </c>
       <c r="L71" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M71" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N71" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4357,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>191</v>
+        <v>260</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>73</v>
@@ -4367,15 +4673,15 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/071_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/071_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/071_F05_in-matutinis_pem92154_aquit.mei </v>
       </c>
       <c r="H72" s="10" t="s">
         <v>184</v>
@@ -4386,15 +4692,15 @@
       </c>
       <c r="L72" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M72" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N72" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4402,7 +4708,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>191</v>
+        <v>261</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>74</v>
@@ -4420,7 +4726,7 @@
       </c>
       <c r="G73" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/072_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/072_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/072_F06_in-matutinis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H73" s="10" t="s">
         <v>185</v>
@@ -4431,15 +4737,15 @@
       </c>
       <c r="L73" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M73" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N73" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4447,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>191</v>
+        <v>262</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>75</v>
@@ -4457,15 +4763,15 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/073_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/073_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/073_F07_cantemus-domino_pem92154_aquit.mei </v>
       </c>
       <c r="H74" s="10" t="s">
         <v>184</v>
@@ -4476,15 +4782,15 @@
       </c>
       <c r="L74" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M74" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N74" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4492,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>191</v>
+        <v>263</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>76</v>
@@ -4510,7 +4816,7 @@
       </c>
       <c r="G75" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/074_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/074_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/074_F08_cantemus-domino_pem71010_square.mei -notation square</v>
       </c>
       <c r="H75" s="10" t="s">
         <v>185</v>
@@ -4524,15 +4830,15 @@
       </c>
       <c r="L75" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M75" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N75" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4540,7 +4846,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>191</v>
+        <v>264</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>77</v>
@@ -4550,15 +4856,15 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/075_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/075_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/075_F09_in-sanctis-ejus_pem92154_aquit.mei </v>
       </c>
       <c r="H76" s="10" t="s">
         <v>184</v>
@@ -4569,15 +4875,15 @@
       </c>
       <c r="L76" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M76" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N76" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4585,7 +4891,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>191</v>
+        <v>265</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>78</v>
@@ -4603,7 +4909,7 @@
       </c>
       <c r="G77" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/076_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/076_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/076_F10_in-sanctis-ejus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H77" s="10" t="s">
         <v>185</v>
@@ -4614,15 +4920,15 @@
       </c>
       <c r="L77" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M77" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N77" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4630,7 +4936,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>79</v>
@@ -4640,15 +4946,15 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/077_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/077_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/077_F11_in-sanctitate-serviamus_pem92154_aquit.mei </v>
       </c>
       <c r="H78" s="10" t="s">
         <v>184</v>
@@ -4659,15 +4965,15 @@
       </c>
       <c r="L78" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M78" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N78" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4675,7 +4981,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>191</v>
+        <v>267</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>80</v>
@@ -4693,7 +4999,7 @@
       </c>
       <c r="G79" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/078_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/078_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/078_F12_in-sanctitate-serviamus_pem71010_square.mei -notation square</v>
       </c>
       <c r="H79" s="10" t="s">
         <v>185</v>
@@ -4704,15 +5010,15 @@
       </c>
       <c r="L79" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M79" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N79" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4720,7 +5026,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>191</v>
+        <v>268</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>81</v>
@@ -4730,15 +5036,15 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/079_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/079_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/079_F13_et-omnis_pem92154_aquit.mei </v>
       </c>
       <c r="H80" s="10" t="s">
         <v>184</v>
@@ -4749,15 +5055,15 @@
       </c>
       <c r="L80" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M80" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N80" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4765,7 +5071,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>82</v>
@@ -4783,7 +5089,7 @@
       </c>
       <c r="G81" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/080_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/080_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/080_F14_et-omnis_pem71010_square.mei -notation square</v>
       </c>
       <c r="H81" s="10" t="s">
         <v>185</v>
@@ -4794,15 +5100,15 @@
       </c>
       <c r="L81" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M81" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N81" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4810,7 +5116,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>83</v>
@@ -4820,15 +5126,15 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/081_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/081_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/081_F15_ecce-quam-bonum_pem92154_aquit.mei </v>
       </c>
       <c r="H82" s="10" t="s">
         <v>184</v>
@@ -4839,15 +5145,15 @@
       </c>
       <c r="L82" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M82" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N82" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4855,7 +5161,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>191</v>
+        <v>271</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>84</v>
@@ -4873,7 +5179,7 @@
       </c>
       <c r="G83" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/082_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/082_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/082_F16_ecce-quam-bonum_pem71010_square.mei -notation square</v>
       </c>
       <c r="H83" s="10" t="s">
         <v>185</v>
@@ -4884,15 +5190,15 @@
       </c>
       <c r="L83" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M83" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N83" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4900,7 +5206,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>191</v>
+        <v>272</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>85</v>
@@ -4910,15 +5216,15 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/083_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/083_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.gabc MEI_outfiles/antiphonae_feriale/083_F17_laudate-nomen_pem92154_aquit.mei </v>
       </c>
       <c r="H84" s="10" t="s">
         <v>184</v>
@@ -4929,15 +5235,15 @@
       </c>
       <c r="L84" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>92154_aquit</v>
       </c>
       <c r="M84" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>92154</v>
       </c>
       <c r="N84" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4945,7 +5251,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>191</v>
+        <v>273</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>86</v>
@@ -4963,7 +5269,7 @@
       </c>
       <c r="G85" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/084_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/084_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.gabc MEI_outfiles/antiphonae_feriale/084_F18_laudate-nomen_pem71010_square.mei -notation square</v>
       </c>
       <c r="H85" s="10" t="s">
         <v>185</v>
@@ -4974,15 +5280,15 @@
       </c>
       <c r="L85" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71010_square</v>
       </c>
       <c r="M85" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71010</v>
       </c>
       <c r="N85" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4990,7 +5296,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>191</v>
+        <v>274</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>87</v>
@@ -5000,15 +5306,15 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/085_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/085_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/085_F19_metuant-dominum_pem80159_aquit.mei </v>
       </c>
       <c r="H86" s="10" t="s">
         <v>186</v>
@@ -5019,15 +5325,15 @@
       </c>
       <c r="L86" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M86" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N86" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5035,7 +5341,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>191</v>
+        <v>275</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>88</v>
@@ -5053,7 +5359,7 @@
       </c>
       <c r="G87" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/086_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/086_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/086_F20_metuant-dominum_pem71012_square.mei -notation square</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>187</v>
@@ -5064,15 +5370,15 @@
       </c>
       <c r="L87" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71012_square</v>
       </c>
       <c r="M87" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71012</v>
       </c>
       <c r="N87" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5080,7 +5386,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>191</v>
+        <v>276</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>89</v>
@@ -5090,15 +5396,15 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/087_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/087_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/087_F21_et-in-servis_pem80159_aquit.mei </v>
       </c>
       <c r="H88" s="10" t="s">
         <v>186</v>
@@ -5109,15 +5415,15 @@
       </c>
       <c r="L88" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M88" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N88" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5125,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>191</v>
+        <v>277</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>90</v>
@@ -5143,7 +5449,7 @@
       </c>
       <c r="G89" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/088_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/088_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/088_F22_et-in-servis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H89" s="10" t="s">
         <v>187</v>
@@ -5154,15 +5460,15 @@
       </c>
       <c r="L89" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71012_square</v>
       </c>
       <c r="M89" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71012</v>
       </c>
       <c r="N89" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5170,7 +5476,7 @@
         <v>2</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>91</v>
@@ -5180,15 +5486,15 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/089_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/089_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/089_F23_in-cimbalis_pem80159_aquit.mei </v>
       </c>
       <c r="H90" s="10" t="s">
         <v>186</v>
@@ -5199,15 +5505,15 @@
       </c>
       <c r="L90" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M90" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N90" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5215,7 +5521,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>191</v>
+        <v>279</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>92</v>
@@ -5233,7 +5539,7 @@
       </c>
       <c r="G91" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/090_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/090_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/090_F24_in-cimbalis_pem71012_square.mei -notation square</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>187</v>
@@ -5244,15 +5550,15 @@
       </c>
       <c r="L91" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71012_square</v>
       </c>
       <c r="M91" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71012</v>
       </c>
       <c r="N91" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5260,7 +5566,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>191</v>
+        <v>280</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>93</v>
@@ -5270,15 +5576,15 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/091_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/091_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/091_F25_in-viam_pem80159_aquit.mei </v>
       </c>
       <c r="H92" s="10" t="s">
         <v>186</v>
@@ -5289,15 +5595,15 @@
       </c>
       <c r="L92" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M92" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N92" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5305,7 +5611,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>191</v>
+        <v>281</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>94</v>
@@ -5323,7 +5629,7 @@
       </c>
       <c r="G93" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/092_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/092_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.gabc MEI_outfiles/antiphonae_feriale/092_F26_in-viam_pem71012_square.mei -notation square</v>
       </c>
       <c r="H93" s="10" t="s">
         <v>187</v>
@@ -5334,15 +5640,15 @@
       </c>
       <c r="L93" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71012_square</v>
       </c>
       <c r="M93" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71012</v>
       </c>
       <c r="N93" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5350,7 +5656,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>191</v>
+        <v>282</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>95</v>
@@ -5360,15 +5666,15 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/093_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/093_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/093_F27_benedictus_pem80159_aquit.mei </v>
       </c>
       <c r="H94" s="10" t="s">
         <v>186</v>
@@ -5379,15 +5685,15 @@
       </c>
       <c r="L94" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M94" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N94" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5395,7 +5701,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>191</v>
+        <v>283</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>96</v>
@@ -5413,7 +5719,7 @@
       </c>
       <c r="G95" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/094_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/094_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/094_F28_benedictus_pem71013_square.mei -notation square</v>
       </c>
       <c r="H95" s="10" t="s">
         <v>188</v>
@@ -5424,15 +5730,15 @@
       </c>
       <c r="L95" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71013_square</v>
       </c>
       <c r="M95" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71013</v>
       </c>
       <c r="N95" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -5440,7 +5746,7 @@
         <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>191</v>
+        <v>284</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>97</v>
@@ -5450,15 +5756,15 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/095_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/095_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/095_F29_per-singulos_pem80159_aquit.mei </v>
       </c>
       <c r="H96" s="8" t="s">
         <v>186</v>
@@ -5469,15 +5775,15 @@
       </c>
       <c r="L96" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M96" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N96" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5485,7 +5791,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>98</v>
@@ -5503,7 +5809,7 @@
       </c>
       <c r="G97" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/096_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/096_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/096_F30_per-singulos_pem71013_square.mei -notation square</v>
       </c>
       <c r="H97" s="10" t="s">
         <v>188</v>
@@ -5514,15 +5820,15 @@
       </c>
       <c r="L97" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71013_square</v>
       </c>
       <c r="M97" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71013</v>
       </c>
       <c r="N97" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -5530,7 +5836,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>191</v>
+        <v>286</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>99</v>
@@ -5540,15 +5846,15 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/097_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/097_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/097_F31_laudabo_pem80159_aquit.mei </v>
       </c>
       <c r="H98" s="8" t="s">
         <v>186</v>
@@ -5559,15 +5865,15 @@
       </c>
       <c r="L98" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M98" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N98" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5575,7 +5881,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>191</v>
+        <v>287</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>100</v>
@@ -5593,7 +5899,7 @@
       </c>
       <c r="G99" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/098_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/098_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/098_F32_laudabo_pem71013_square.mei -notation square</v>
       </c>
       <c r="H99" s="10" t="s">
         <v>188</v>
@@ -5604,15 +5910,15 @@
       </c>
       <c r="L99" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71013_square</v>
       </c>
       <c r="M99" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71013</v>
       </c>
       <c r="N99" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5620,7 +5926,7 @@
         <v>2</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>191</v>
+        <v>288</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>101</v>
@@ -5630,15 +5936,15 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/099_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/099_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/099_F33_deo-nostro_pem80159_aquit.mei </v>
       </c>
       <c r="H100" s="8" t="s">
         <v>186</v>
@@ -5649,15 +5955,15 @@
       </c>
       <c r="L100" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M100" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N100" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5665,7 +5971,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>102</v>
@@ -5683,7 +5989,7 @@
       </c>
       <c r="G101" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/100_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/100_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/100_F34_deo-nostro_pem71013_square.mei -notation square</v>
       </c>
       <c r="H101" s="10" t="s">
         <v>188</v>
@@ -5694,15 +6000,15 @@
       </c>
       <c r="L101" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71013_square</v>
       </c>
       <c r="M101" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71013</v>
       </c>
       <c r="N101" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -5710,7 +6016,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>191</v>
+        <v>290</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>103</v>
@@ -5720,15 +6026,15 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="8"/>
-        <v>square</v>
+        <v>_aquit</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="9"/>
-        <v>-notation square</v>
+        <v/>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/101_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/101_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.gabc MEI_outfiles/antiphonae_feriale/101_F35_benedixit_pem80159_aquit.mei </v>
       </c>
       <c r="H102" s="8" t="s">
         <v>186</v>
@@ -5739,15 +6045,15 @@
       </c>
       <c r="L102" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>80159_aquit</v>
       </c>
       <c r="M102" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>80159</v>
       </c>
       <c r="N102" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -5755,7 +6061,7 @@
         <v>2</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>104</v>
@@ -5773,7 +6079,7 @@
       </c>
       <c r="G103" t="str">
         <f t="shared" si="14"/>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/102_F02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_feriale/102_F02_benedicite-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.gabc MEI_outfiles/antiphonae_feriale/102_F36_benedixit_pem71013_square.mei -notation square</v>
       </c>
       <c r="H103" s="10" t="s">
         <v>188</v>
@@ -5784,15 +6090,15 @@
       </c>
       <c r="L103" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>85041_square</v>
+        <v>71013_square</v>
       </c>
       <c r="M103" s="14" t="str">
         <f t="shared" si="12"/>
-        <v>85041</v>
+        <v>71013</v>
       </c>
       <c r="N103" s="15" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix filenames once more
</commit_message>
<xml_diff>
--- a/commands_for_processing_pieces.xlsx
+++ b/commands_for_processing_pieces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/GABCtoMEI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1268545D-0F86-A740-BB6E-1855A2DF3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7FD4EC-801B-054C-8D9F-1D6DAF869E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="4280" windowWidth="48280" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
+    <workbookView xWindow="2920" yWindow="4280" windowWidth="48280" windowHeight="16780" xr2:uid="{E4997A24-5992-8040-BD65-A8C26412DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,12 +636,6 @@
     <t>Evaluation of links vs. filenames</t>
   </si>
   <si>
-    <t>01_benedicte-omnes_pem82441_aquit</t>
-  </si>
-  <si>
-    <t>02_benedicte-omnes_pem85041_square</t>
-  </si>
-  <si>
     <t>03_de-fructu-operum_pem56766_aquit</t>
   </si>
   <si>
@@ -940,6 +934,12 @@
   </si>
   <si>
     <t>36_benedixit_pem71013_square</t>
+  </si>
+  <si>
+    <t>01_benedicite-omnes_pem82441_aquit</t>
+  </si>
+  <si>
+    <t>02_benedicite-omnes_pem85041_square</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1100,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1436,7 +1436,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,19 +1477,19 @@
       <c r="G1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>290</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A2,"/",C2,"_",D2,B2,".gabc MEI_outfiles/", A2, "/", C2, "_", D2, B2, ".mei ",F2)</f>
-        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicte-omnes_pem82441_aquit.mei </v>
+        <v xml:space="preserve">python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/001_C01_benedicite-omnes_pem82441_aquit.gabc MEI_outfiles/antiphonae_ad_communionem/001_C01_benedicite-omnes_pem82441_aquit.mei </v>
       </c>
       <c r="H2" s="12" t="s">
         <v>118</v>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="G3" t="str">
         <f>_xlfn.CONCAT("python3 gabc-tokens_to_mei-elements.py GABC_infiles/",A3,"/",C3,"_",D3,B3,".gabc MEI_outfiles/", A3, "/", C3, "_", D3, B3, ".mei ",F3)</f>
-        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicte-omnes_pem85041_square.mei -notation square</v>
+        <v>python3 gabc-tokens_to_mei-elements.py GABC_infiles/antiphonae_ad_communionem/002_C02_benedicite-omnes_pem85041_square.gabc MEI_outfiles/antiphonae_ad_communionem/002_C02_benedicite-omnes_pem85041_square.mei -notation square</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>119</v>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -1942,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
@@ -2035,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -2080,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
@@ -2305,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -2350,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -2440,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -2620,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>28</v>
@@ -2668,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>29</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>30</v>
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>31</v>
@@ -2803,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>32</v>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>33</v>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>34</v>
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>35</v>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>36</v>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>37</v>
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>38</v>
@@ -3117,8 +3117,8 @@
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>226</v>
+      <c r="B38" s="17" t="s">
+        <v>224</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>39</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>40</v>
@@ -3211,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>41</v>
@@ -3256,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>42</v>
@@ -3301,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>43</v>
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>44</v>
@@ -3391,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>45</v>
@@ -3436,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>46</v>
@@ -3481,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>47</v>
@@ -3526,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -3571,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>49</v>
@@ -3619,7 +3619,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>50</v>
@@ -3664,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>51</v>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>52</v>
@@ -3754,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>53</v>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>54</v>
@@ -3844,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>55</v>
@@ -3889,7 +3889,7 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>56</v>
@@ -3937,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>57</v>
@@ -3982,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>58</v>
@@ -4027,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>59</v>
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>60</v>
@@ -4117,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>61</v>
@@ -4162,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>62</v>
@@ -4210,7 +4210,7 @@
         <v>1</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>63</v>
@@ -4255,7 +4255,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>64</v>
@@ -4300,7 +4300,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>65</v>
@@ -4345,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>66</v>
@@ -4390,7 +4390,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>67</v>
@@ -4438,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>68</v>
@@ -4483,7 +4483,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>69</v>
@@ -4528,7 +4528,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>70</v>
@@ -4573,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>71</v>
@@ -4618,7 +4618,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>72</v>
@@ -4663,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>73</v>
@@ -4708,7 +4708,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>74</v>
@@ -4753,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>75</v>
@@ -4798,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>76</v>
@@ -4846,7 +4846,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>77</v>
@@ -4891,7 +4891,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>78</v>
@@ -4936,7 +4936,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>79</v>
@@ -4981,7 +4981,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>80</v>
@@ -5026,7 +5026,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>81</v>
@@ -5071,7 +5071,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>82</v>
@@ -5116,7 +5116,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>83</v>
@@ -5161,7 +5161,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>84</v>
@@ -5206,7 +5206,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>85</v>
@@ -5251,7 +5251,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>86</v>
@@ -5296,7 +5296,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>87</v>
@@ -5341,7 +5341,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>88</v>
@@ -5386,7 +5386,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>89</v>
@@ -5431,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>90</v>
@@ -5476,7 +5476,7 @@
         <v>2</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>91</v>
@@ -5521,7 +5521,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>92</v>
@@ -5566,7 +5566,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>93</v>
@@ -5611,7 +5611,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>94</v>
@@ -5656,7 +5656,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>95</v>
@@ -5701,7 +5701,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>96</v>
@@ -5746,7 +5746,7 @@
         <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>97</v>
@@ -5791,7 +5791,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>98</v>
@@ -5836,7 +5836,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>99</v>
@@ -5881,7 +5881,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>100</v>
@@ -5926,7 +5926,7 @@
         <v>2</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>101</v>
@@ -5971,7 +5971,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>102</v>
@@ -6016,7 +6016,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>103</v>
@@ -6061,7 +6061,7 @@
         <v>2</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>104</v>

</xml_diff>